<commit_message>
#31 remove some anti skill
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Weapon.xlsx
+++ b/ConfigData/Xlsx/Weapon.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -4002,7 +4002,7 @@
             <v>55100001</v>
           </cell>
           <cell r="V4">
-            <v>0</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="5">
@@ -4517,8 +4517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF130"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="C121" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="U4" sqref="U4"/>
@@ -17677,7 +17677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>

</xml_diff>

<commit_message>
remove some skill and add a add weapon method for monster
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Weapon.xlsx
+++ b/ConfigData/Xlsx/Weapon.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -5306,31 +5306,31 @@
   <dimension ref="A1:AG124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B95" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AA12" sqref="AA12"/>
+      <selection pane="bottomRight" activeCell="L106" sqref="L106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.25" customWidth="1"/>
-    <col min="5" max="9" width="4.125" customWidth="1"/>
-    <col min="10" max="11" width="3.75" customWidth="1"/>
-    <col min="12" max="20" width="3.875" customWidth="1"/>
-    <col min="21" max="21" width="6.375" customWidth="1"/>
-    <col min="22" max="23" width="3.875" customWidth="1"/>
-    <col min="24" max="25" width="4.75" customWidth="1"/>
-    <col min="26" max="26" width="9.5" customWidth="1"/>
-    <col min="27" max="27" width="7.125" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" customWidth="1"/>
+    <col min="5" max="9" width="4.109375" customWidth="1"/>
+    <col min="10" max="11" width="3.77734375" customWidth="1"/>
+    <col min="12" max="20" width="3.88671875" customWidth="1"/>
+    <col min="21" max="21" width="6.33203125" customWidth="1"/>
+    <col min="22" max="23" width="3.88671875" customWidth="1"/>
+    <col min="24" max="25" width="4.77734375" customWidth="1"/>
+    <col min="26" max="26" width="9.44140625" customWidth="1"/>
+    <col min="27" max="27" width="7.109375" customWidth="1"/>
     <col min="28" max="29" width="9" customWidth="1"/>
-    <col min="30" max="31" width="7.375" customWidth="1"/>
-    <col min="32" max="33" width="4.375" customWidth="1"/>
-    <col min="36" max="36" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="7.33203125" customWidth="1"/>
+    <col min="32" max="33" width="4.33203125" customWidth="1"/>
+    <col min="36" max="36" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="69">
+    <row r="1" spans="1:33" ht="73.2">
       <c r="A1" s="19" t="s">
         <v>242</v>
       </c>
@@ -15813,7 +15813,7 @@
       </c>
       <c r="D106" s="25"/>
       <c r="E106" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F106">
         <v>103</v>
@@ -15823,10 +15823,10 @@
       </c>
       <c r="H106" s="4">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I106" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J106" s="7">
         <v>0</v>
@@ -15835,7 +15835,7 @@
         <v>50</v>
       </c>
       <c r="L106" s="14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M106" s="8">
         <v>4</v>
@@ -15863,7 +15863,7 @@
       </c>
       <c r="U106" s="10">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="V106" s="8">
         <v>0</v>
@@ -15884,7 +15884,7 @@
         <v>5</v>
       </c>
       <c r="AC106" s="4">
-        <v>11000006</v>
+        <v>11000008</v>
       </c>
       <c r="AD106" s="4">
         <v>5</v>
@@ -17953,23 +17953,23 @@
       <selection pane="bottomRight" activeCell="AC1" sqref="AC1:AC3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="11.25" customWidth="1"/>
-    <col min="5" max="9" width="4.125" customWidth="1"/>
-    <col min="10" max="11" width="3.75" customWidth="1"/>
-    <col min="12" max="12" width="4.375" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" customWidth="1"/>
+    <col min="5" max="9" width="4.109375" customWidth="1"/>
+    <col min="10" max="11" width="3.77734375" customWidth="1"/>
+    <col min="12" max="12" width="4.33203125" customWidth="1"/>
     <col min="13" max="20" width="4" customWidth="1"/>
-    <col min="21" max="21" width="3.75" customWidth="1"/>
+    <col min="21" max="21" width="3.77734375" customWidth="1"/>
     <col min="22" max="24" width="4" customWidth="1"/>
-    <col min="25" max="25" width="3.75" customWidth="1"/>
-    <col min="26" max="27" width="7.125" customWidth="1"/>
+    <col min="25" max="25" width="3.77734375" customWidth="1"/>
+    <col min="26" max="27" width="7.109375" customWidth="1"/>
     <col min="28" max="29" width="9" customWidth="1"/>
-    <col min="30" max="31" width="7.375" customWidth="1"/>
-    <col min="32" max="33" width="4.375" customWidth="1"/>
+    <col min="30" max="31" width="7.33203125" customWidth="1"/>
+    <col min="32" max="33" width="4.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="69">
+    <row r="1" spans="1:33" ht="73.2">
       <c r="A1" s="19" t="s">
         <v>242</v>
       </c>
@@ -18612,7 +18612,7 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="B1" t="s">

</xml_diff>

<commit_message>
new card sap and backhit #58
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Weapon.xlsx
+++ b/ConfigData/Xlsx/Weapon.xlsx
@@ -3623,79 +3623,79 @@
         </row>
         <row r="12">
           <cell r="A12">
-            <v>55100009</v>
+            <v>55100010</v>
           </cell>
           <cell r="X12">
-            <v>15</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="13">
           <cell r="A13">
-            <v>55100010</v>
+            <v>55100011</v>
           </cell>
           <cell r="X13">
-            <v>12</v>
+            <v>6</v>
           </cell>
         </row>
         <row r="14">
           <cell r="A14">
-            <v>55100011</v>
+            <v>55100012</v>
           </cell>
           <cell r="X14">
-            <v>6</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="15">
           <cell r="A15">
-            <v>55100012</v>
+            <v>55100013</v>
           </cell>
           <cell r="X15">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="16">
           <cell r="A16">
-            <v>55100013</v>
+            <v>55100014</v>
           </cell>
           <cell r="X16">
-            <v>10</v>
+            <v>24</v>
           </cell>
         </row>
         <row r="17">
           <cell r="A17">
-            <v>55100014</v>
+            <v>55100015</v>
           </cell>
           <cell r="X17">
-            <v>24</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="18">
           <cell r="A18">
-            <v>55100015</v>
+            <v>55110001</v>
           </cell>
           <cell r="X18">
-            <v>16</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="19">
           <cell r="A19">
-            <v>55110001</v>
+            <v>55110002</v>
           </cell>
           <cell r="X19">
-            <v>5</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="20">
           <cell r="A20">
-            <v>55110002</v>
+            <v>55110003</v>
           </cell>
           <cell r="X20">
-            <v>8</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="21">
           <cell r="A21">
-            <v>55110003</v>
+            <v>55110004</v>
           </cell>
           <cell r="X21">
             <v>25</v>
@@ -3703,135 +3703,135 @@
         </row>
         <row r="22">
           <cell r="A22">
-            <v>55110004</v>
+            <v>55110005</v>
           </cell>
           <cell r="X22">
-            <v>25</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="23">
           <cell r="A23">
-            <v>55110005</v>
+            <v>55110006</v>
           </cell>
           <cell r="X23">
-            <v>20</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="24">
           <cell r="A24">
-            <v>55110006</v>
+            <v>55110007</v>
           </cell>
           <cell r="X24">
-            <v>15</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="25">
           <cell r="A25">
-            <v>55110007</v>
+            <v>55110008</v>
           </cell>
           <cell r="X25">
-            <v>10</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="26">
           <cell r="A26">
-            <v>55110008</v>
+            <v>55110009</v>
           </cell>
           <cell r="X26">
-            <v>50</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="27">
           <cell r="A27">
-            <v>55110009</v>
+            <v>55110010</v>
           </cell>
           <cell r="X27">
-            <v>12</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="28">
           <cell r="A28">
-            <v>55110010</v>
+            <v>55110011</v>
           </cell>
           <cell r="X28">
-            <v>30</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="29">
           <cell r="A29">
-            <v>55110011</v>
+            <v>55110012</v>
           </cell>
           <cell r="X29">
-            <v>10</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="30">
           <cell r="A30">
-            <v>55110012</v>
+            <v>55110013</v>
           </cell>
           <cell r="X30">
-            <v>30</v>
+            <v>200</v>
           </cell>
         </row>
         <row r="31">
           <cell r="A31">
-            <v>55110013</v>
+            <v>55110014</v>
           </cell>
           <cell r="X31">
-            <v>200</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="32">
           <cell r="A32">
-            <v>55110014</v>
+            <v>55110015</v>
           </cell>
           <cell r="X32">
-            <v>50</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="33">
           <cell r="A33">
-            <v>55110015</v>
+            <v>55110016</v>
           </cell>
           <cell r="X33">
-            <v>20</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="34">
           <cell r="A34">
-            <v>55110016</v>
+            <v>55110017</v>
           </cell>
           <cell r="X34">
-            <v>15</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="35">
           <cell r="A35">
-            <v>55110017</v>
+            <v>55110018</v>
           </cell>
           <cell r="X35">
-            <v>8</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="36">
           <cell r="A36">
-            <v>55110018</v>
+            <v>55110019</v>
           </cell>
           <cell r="X36">
-            <v>20</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="37">
           <cell r="A37">
-            <v>55110019</v>
+            <v>55110020</v>
           </cell>
           <cell r="X37">
-            <v>30</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="38">
           <cell r="A38">
-            <v>55110020</v>
+            <v>55200001</v>
           </cell>
           <cell r="X38">
             <v>40</v>
@@ -3839,39 +3839,39 @@
         </row>
         <row r="39">
           <cell r="A39">
-            <v>55200001</v>
+            <v>55200002</v>
           </cell>
           <cell r="X39">
-            <v>40</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="40">
           <cell r="A40">
-            <v>55200002</v>
+            <v>55200003</v>
           </cell>
           <cell r="X40">
-            <v>15</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="41">
           <cell r="A41">
-            <v>55200003</v>
+            <v>55200004</v>
           </cell>
           <cell r="X41">
-            <v>25</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="42">
           <cell r="A42">
-            <v>55200004</v>
+            <v>55200005</v>
           </cell>
           <cell r="X42">
-            <v>40</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="43">
           <cell r="A43">
-            <v>55200005</v>
+            <v>55200006</v>
           </cell>
           <cell r="X43">
             <v>20</v>
@@ -3879,7 +3879,7 @@
         </row>
         <row r="44">
           <cell r="A44">
-            <v>55200006</v>
+            <v>55200007</v>
           </cell>
           <cell r="X44">
             <v>20</v>
@@ -3887,15 +3887,15 @@
         </row>
         <row r="45">
           <cell r="A45">
-            <v>55200007</v>
+            <v>55200008</v>
           </cell>
           <cell r="X45">
-            <v>20</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="46">
           <cell r="A46">
-            <v>55200008</v>
+            <v>55200009</v>
           </cell>
           <cell r="X46">
             <v>25</v>
@@ -3903,7 +3903,7 @@
         </row>
         <row r="47">
           <cell r="A47">
-            <v>55200009</v>
+            <v>55200010</v>
           </cell>
           <cell r="X47">
             <v>25</v>
@@ -3911,55 +3911,55 @@
         </row>
         <row r="48">
           <cell r="A48">
-            <v>55200010</v>
+            <v>55200011</v>
           </cell>
           <cell r="X48">
-            <v>25</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="49">
           <cell r="A49">
-            <v>55200011</v>
+            <v>55200012</v>
           </cell>
           <cell r="X49">
-            <v>20</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="50">
           <cell r="A50">
-            <v>55200012</v>
+            <v>55200013</v>
           </cell>
           <cell r="X50">
-            <v>30</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="51">
           <cell r="A51">
-            <v>55200013</v>
+            <v>55200014</v>
           </cell>
           <cell r="X51">
-            <v>10</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="52">
           <cell r="A52">
-            <v>55200014</v>
+            <v>55300001</v>
           </cell>
           <cell r="X52">
-            <v>25</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="53">
           <cell r="A53">
-            <v>55300001</v>
+            <v>55300002</v>
           </cell>
           <cell r="X53">
-            <v>40</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="54">
           <cell r="A54">
-            <v>55300002</v>
+            <v>55300003</v>
           </cell>
           <cell r="X54">
             <v>30</v>
@@ -3967,7 +3967,7 @@
         </row>
         <row r="55">
           <cell r="A55">
-            <v>55300003</v>
+            <v>55300004</v>
           </cell>
           <cell r="X55">
             <v>30</v>
@@ -3975,7 +3975,7 @@
         </row>
         <row r="56">
           <cell r="A56">
-            <v>55300004</v>
+            <v>55300005</v>
           </cell>
           <cell r="X56">
             <v>30</v>
@@ -3983,15 +3983,15 @@
         </row>
         <row r="57">
           <cell r="A57">
-            <v>55300005</v>
+            <v>55300006</v>
           </cell>
           <cell r="X57">
-            <v>30</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="58">
           <cell r="A58">
-            <v>55300006</v>
+            <v>55300007</v>
           </cell>
           <cell r="X58">
             <v>25</v>
@@ -3999,15 +3999,15 @@
         </row>
         <row r="59">
           <cell r="A59">
-            <v>55300007</v>
+            <v>55300008</v>
           </cell>
           <cell r="X59">
-            <v>25</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="60">
           <cell r="A60">
-            <v>55300008</v>
+            <v>55300009</v>
           </cell>
           <cell r="X60">
             <v>30</v>
@@ -4015,71 +4015,71 @@
         </row>
         <row r="61">
           <cell r="A61">
-            <v>55300009</v>
+            <v>55300010</v>
           </cell>
           <cell r="X61">
-            <v>30</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="62">
           <cell r="A62">
-            <v>55300010</v>
+            <v>55300011</v>
           </cell>
           <cell r="X62">
-            <v>35</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="63">
           <cell r="A63">
-            <v>55300011</v>
+            <v>55300012</v>
           </cell>
           <cell r="X63">
-            <v>25</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="64">
           <cell r="A64">
-            <v>55300012</v>
+            <v>55300013</v>
           </cell>
           <cell r="X64">
-            <v>5</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="65">
           <cell r="A65">
-            <v>55300013</v>
+            <v>55310001</v>
           </cell>
           <cell r="X65">
-            <v>15</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="66">
           <cell r="A66">
-            <v>55310001</v>
+            <v>55310002</v>
           </cell>
           <cell r="X66">
-            <v>100</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="67">
           <cell r="A67">
-            <v>55310002</v>
+            <v>55310003</v>
           </cell>
           <cell r="X67">
-            <v>15</v>
+            <v>13</v>
           </cell>
         </row>
         <row r="68">
           <cell r="A68">
-            <v>55310003</v>
+            <v>55400001</v>
           </cell>
           <cell r="X68">
-            <v>13</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="69">
           <cell r="A69">
-            <v>55400001</v>
+            <v>55400002</v>
           </cell>
           <cell r="X69">
             <v>80</v>
@@ -4087,7 +4087,7 @@
         </row>
         <row r="70">
           <cell r="A70">
-            <v>55400002</v>
+            <v>55400003</v>
           </cell>
           <cell r="X70">
             <v>80</v>
@@ -4095,47 +4095,47 @@
         </row>
         <row r="71">
           <cell r="A71">
-            <v>55400003</v>
+            <v>55400005</v>
           </cell>
           <cell r="X71">
-            <v>80</v>
+            <v>55</v>
           </cell>
         </row>
         <row r="72">
           <cell r="A72">
-            <v>55400005</v>
+            <v>55400006</v>
           </cell>
           <cell r="X72">
-            <v>55</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="73">
           <cell r="A73">
-            <v>55400006</v>
+            <v>55400007</v>
           </cell>
           <cell r="X73">
-            <v>30</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="74">
           <cell r="A74">
-            <v>55400007</v>
+            <v>55410001</v>
           </cell>
           <cell r="X74">
-            <v>25</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="75">
           <cell r="A75">
-            <v>55410001</v>
+            <v>55500001</v>
           </cell>
           <cell r="X75">
-            <v>50</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="76">
           <cell r="A76">
-            <v>55500001</v>
+            <v>55500002</v>
           </cell>
           <cell r="X76">
             <v>5</v>
@@ -4143,7 +4143,7 @@
         </row>
         <row r="77">
           <cell r="A77">
-            <v>55500002</v>
+            <v>55500003</v>
           </cell>
           <cell r="X77">
             <v>5</v>
@@ -4151,7 +4151,7 @@
         </row>
         <row r="78">
           <cell r="A78">
-            <v>55500003</v>
+            <v>55500004</v>
           </cell>
           <cell r="X78">
             <v>5</v>
@@ -4159,7 +4159,7 @@
         </row>
         <row r="79">
           <cell r="A79">
-            <v>55500004</v>
+            <v>55500005</v>
           </cell>
           <cell r="X79">
             <v>5</v>
@@ -4167,7 +4167,7 @@
         </row>
         <row r="80">
           <cell r="A80">
-            <v>55500005</v>
+            <v>55500006</v>
           </cell>
           <cell r="X80">
             <v>5</v>
@@ -4175,7 +4175,7 @@
         </row>
         <row r="81">
           <cell r="A81">
-            <v>55500006</v>
+            <v>55500007</v>
           </cell>
           <cell r="X81">
             <v>5</v>
@@ -4183,7 +4183,7 @@
         </row>
         <row r="82">
           <cell r="A82">
-            <v>55500007</v>
+            <v>55500008</v>
           </cell>
           <cell r="X82">
             <v>5</v>
@@ -4191,7 +4191,7 @@
         </row>
         <row r="83">
           <cell r="A83">
-            <v>55500008</v>
+            <v>55500009</v>
           </cell>
           <cell r="X83">
             <v>5</v>
@@ -4199,7 +4199,7 @@
         </row>
         <row r="84">
           <cell r="A84">
-            <v>55500009</v>
+            <v>55500010</v>
           </cell>
           <cell r="X84">
             <v>5</v>
@@ -4207,7 +4207,7 @@
         </row>
         <row r="85">
           <cell r="A85">
-            <v>55500010</v>
+            <v>55500011</v>
           </cell>
           <cell r="X85">
             <v>5</v>
@@ -4215,7 +4215,7 @@
         </row>
         <row r="86">
           <cell r="A86">
-            <v>55500011</v>
+            <v>55500012</v>
           </cell>
           <cell r="X86">
             <v>5</v>
@@ -4223,7 +4223,7 @@
         </row>
         <row r="87">
           <cell r="A87">
-            <v>55500012</v>
+            <v>55500013</v>
           </cell>
           <cell r="X87">
             <v>5</v>
@@ -4231,7 +4231,7 @@
         </row>
         <row r="88">
           <cell r="A88">
-            <v>55500013</v>
+            <v>55500014</v>
           </cell>
           <cell r="X88">
             <v>5</v>
@@ -4239,7 +4239,7 @@
         </row>
         <row r="89">
           <cell r="A89">
-            <v>55500014</v>
+            <v>55500015</v>
           </cell>
           <cell r="X89">
             <v>5</v>
@@ -4247,7 +4247,7 @@
         </row>
         <row r="90">
           <cell r="A90">
-            <v>55500015</v>
+            <v>55500016</v>
           </cell>
           <cell r="X90">
             <v>5</v>
@@ -4255,23 +4255,23 @@
         </row>
         <row r="91">
           <cell r="A91">
-            <v>55500016</v>
+            <v>55510001</v>
           </cell>
           <cell r="X91">
-            <v>5</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="92">
           <cell r="A92">
-            <v>55510001</v>
+            <v>55510002</v>
           </cell>
           <cell r="X92">
-            <v>12</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="93">
           <cell r="A93">
-            <v>55510002</v>
+            <v>55510003</v>
           </cell>
           <cell r="X93">
             <v>15</v>
@@ -4279,87 +4279,87 @@
         </row>
         <row r="94">
           <cell r="A94">
-            <v>55510003</v>
+            <v>55510004</v>
           </cell>
           <cell r="X94">
-            <v>15</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="95">
           <cell r="A95">
-            <v>55510004</v>
+            <v>55510006</v>
           </cell>
           <cell r="X95">
-            <v>12</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="96">
           <cell r="A96">
-            <v>55510006</v>
+            <v>55510007</v>
           </cell>
           <cell r="X96">
-            <v>25</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="97">
           <cell r="A97">
-            <v>55510007</v>
+            <v>55510009</v>
           </cell>
           <cell r="X97">
-            <v>10</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="98">
           <cell r="A98">
-            <v>55510009</v>
+            <v>55510010</v>
           </cell>
           <cell r="X98">
-            <v>50</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="99">
           <cell r="A99">
-            <v>55510010</v>
+            <v>55510011</v>
           </cell>
           <cell r="X99">
-            <v>5</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="100">
           <cell r="A100">
-            <v>55510011</v>
+            <v>55510012</v>
           </cell>
           <cell r="X100">
-            <v>15</v>
+            <v>62</v>
           </cell>
         </row>
         <row r="101">
           <cell r="A101">
-            <v>55510012</v>
+            <v>55510013</v>
           </cell>
           <cell r="X101">
-            <v>62</v>
+            <v>12</v>
           </cell>
         </row>
         <row r="102">
           <cell r="A102">
-            <v>55510013</v>
+            <v>55510014</v>
           </cell>
           <cell r="X102">
-            <v>12</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="103">
           <cell r="A103">
-            <v>55510014</v>
+            <v>55510018</v>
           </cell>
           <cell r="X103">
-            <v>25</v>
+            <v>37</v>
           </cell>
         </row>
         <row r="104">
           <cell r="A104">
-            <v>55510018</v>
+            <v>55510019</v>
           </cell>
           <cell r="X104">
             <v>37</v>
@@ -4367,63 +4367,63 @@
         </row>
         <row r="105">
           <cell r="A105">
-            <v>55510019</v>
+            <v>55520001</v>
           </cell>
           <cell r="X105">
-            <v>37</v>
+            <v>-25</v>
           </cell>
         </row>
         <row r="106">
           <cell r="A106">
-            <v>55520001</v>
+            <v>55520002</v>
           </cell>
           <cell r="X106">
-            <v>-25</v>
+            <v>62</v>
           </cell>
         </row>
         <row r="107">
           <cell r="A107">
-            <v>55520002</v>
+            <v>55520003</v>
           </cell>
           <cell r="X107">
-            <v>62</v>
+            <v>27</v>
           </cell>
         </row>
         <row r="108">
           <cell r="A108">
-            <v>55520003</v>
+            <v>55600001</v>
           </cell>
           <cell r="X108">
-            <v>27</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="109">
           <cell r="A109">
-            <v>55600001</v>
+            <v>55600002</v>
           </cell>
           <cell r="X109">
-            <v>8</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="110">
           <cell r="A110">
-            <v>55600002</v>
+            <v>55600004</v>
           </cell>
           <cell r="X110">
-            <v>10</v>
+            <v>8</v>
           </cell>
         </row>
         <row r="111">
           <cell r="A111">
-            <v>55600004</v>
+            <v>55600005</v>
           </cell>
           <cell r="X111">
-            <v>8</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="112">
           <cell r="A112">
-            <v>55600005</v>
+            <v>55600006</v>
           </cell>
           <cell r="X112">
             <v>15</v>
@@ -4431,103 +4431,103 @@
         </row>
         <row r="113">
           <cell r="A113">
-            <v>55600006</v>
+            <v>55600007</v>
           </cell>
           <cell r="X113">
-            <v>15</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="114">
           <cell r="A114">
-            <v>55600007</v>
+            <v>55600008</v>
           </cell>
           <cell r="X114">
-            <v>20</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="115">
           <cell r="A115">
-            <v>55600008</v>
+            <v>55600009</v>
           </cell>
           <cell r="X115">
-            <v>30</v>
+            <v>13</v>
           </cell>
         </row>
         <row r="116">
           <cell r="A116">
-            <v>55600009</v>
+            <v>55600010</v>
           </cell>
           <cell r="X116">
-            <v>13</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="117">
           <cell r="A117">
-            <v>55600010</v>
+            <v>55600011</v>
           </cell>
           <cell r="X117">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="118">
           <cell r="A118">
-            <v>55600011</v>
+            <v>55600012</v>
           </cell>
           <cell r="X118">
-            <v>20</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="119">
           <cell r="A119">
-            <v>55600012</v>
+            <v>55600013</v>
           </cell>
           <cell r="X119">
-            <v>30</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="120">
           <cell r="A120">
-            <v>55600013</v>
+            <v>55600014</v>
           </cell>
           <cell r="X120">
-            <v>15</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="121">
           <cell r="A121">
-            <v>55600014</v>
+            <v>55600015</v>
           </cell>
           <cell r="X121">
-            <v>30</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="122">
           <cell r="A122">
-            <v>55600015</v>
+            <v>55600016</v>
           </cell>
           <cell r="X122">
-            <v>10</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="123">
           <cell r="A123">
-            <v>55600016</v>
+            <v>55610001</v>
           </cell>
           <cell r="X123">
-            <v>15</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="124">
           <cell r="A124">
-            <v>55610001</v>
+            <v>55610002</v>
           </cell>
           <cell r="X124">
-            <v>30</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="125">
           <cell r="A125">
-            <v>55610002</v>
+            <v>55610003</v>
           </cell>
           <cell r="X125">
             <v>5</v>
@@ -4535,23 +4535,23 @@
         </row>
         <row r="126">
           <cell r="A126">
-            <v>55610003</v>
+            <v>55610004</v>
           </cell>
           <cell r="X126">
-            <v>5</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="127">
           <cell r="A127">
-            <v>55610004</v>
+            <v>55700001</v>
           </cell>
           <cell r="X127">
-            <v>10</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="128">
           <cell r="A128">
-            <v>55700001</v>
+            <v>55700002</v>
           </cell>
           <cell r="X128">
             <v>20</v>
@@ -4559,7 +4559,7 @@
         </row>
         <row r="129">
           <cell r="A129">
-            <v>55700002</v>
+            <v>55700003</v>
           </cell>
           <cell r="X129">
             <v>20</v>
@@ -4567,7 +4567,7 @@
         </row>
         <row r="130">
           <cell r="A130">
-            <v>55700003</v>
+            <v>55700004</v>
           </cell>
           <cell r="X130">
             <v>20</v>
@@ -4575,207 +4575,207 @@
         </row>
         <row r="131">
           <cell r="A131">
-            <v>55700004</v>
+            <v>55700005</v>
           </cell>
           <cell r="X131">
-            <v>20</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="132">
           <cell r="A132">
-            <v>55700005</v>
+            <v>55900001</v>
           </cell>
           <cell r="X132">
-            <v>40</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="133">
           <cell r="A133">
-            <v>55900001</v>
+            <v>55900002</v>
           </cell>
           <cell r="X133">
-            <v>35</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="134">
           <cell r="A134">
-            <v>55900002</v>
+            <v>55900003</v>
           </cell>
           <cell r="X134">
-            <v>30</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="135">
           <cell r="A135">
-            <v>55900003</v>
+            <v>55900004</v>
           </cell>
           <cell r="X135">
-            <v>80</v>
+            <v>-30</v>
           </cell>
         </row>
         <row r="136">
           <cell r="A136">
-            <v>55900004</v>
+            <v>55900005</v>
           </cell>
           <cell r="X136">
-            <v>-30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="137">
           <cell r="A137">
-            <v>55900005</v>
+            <v>55900006</v>
           </cell>
           <cell r="X137">
-            <v>20</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="138">
           <cell r="A138">
-            <v>55900006</v>
+            <v>55900007</v>
           </cell>
           <cell r="X138">
-            <v>35</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="139">
           <cell r="A139">
-            <v>55900007</v>
+            <v>55900008</v>
           </cell>
           <cell r="X139">
-            <v>25</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="140">
           <cell r="A140">
-            <v>55900008</v>
+            <v>55900009</v>
           </cell>
           <cell r="X140">
-            <v>40</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="141">
           <cell r="A141">
-            <v>55900009</v>
+            <v>55900010</v>
           </cell>
           <cell r="X141">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="142">
           <cell r="A142">
-            <v>55900010</v>
+            <v>55900011</v>
           </cell>
           <cell r="X142">
-            <v>20</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="143">
           <cell r="A143">
-            <v>55900011</v>
+            <v>55900012</v>
           </cell>
           <cell r="X143">
-            <v>15</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="144">
           <cell r="A144">
-            <v>55900012</v>
+            <v>55900013</v>
           </cell>
           <cell r="X144">
-            <v>25</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="145">
           <cell r="A145">
-            <v>55900013</v>
+            <v>55900014</v>
           </cell>
           <cell r="X145">
-            <v>10</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="146">
           <cell r="A146">
-            <v>55900014</v>
+            <v>55900015</v>
           </cell>
           <cell r="X146">
-            <v>20</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="147">
           <cell r="A147">
-            <v>55900015</v>
+            <v>55900016</v>
           </cell>
           <cell r="X147">
-            <v>30</v>
+            <v>45</v>
           </cell>
         </row>
         <row r="148">
           <cell r="A148">
-            <v>55900016</v>
+            <v>55900017</v>
           </cell>
           <cell r="X148">
-            <v>45</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="149">
           <cell r="A149">
-            <v>55900017</v>
+            <v>55900018</v>
           </cell>
           <cell r="X149">
-            <v>10</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="150">
           <cell r="A150">
-            <v>55900018</v>
+            <v>55900019</v>
           </cell>
           <cell r="X150">
-            <v>30</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="151">
           <cell r="A151">
-            <v>55900019</v>
+            <v>55900020</v>
           </cell>
           <cell r="X151">
-            <v>80</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="152">
           <cell r="A152">
-            <v>55900020</v>
+            <v>55900021</v>
           </cell>
           <cell r="X152">
-            <v>20</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="153">
           <cell r="A153">
-            <v>55900021</v>
+            <v>55900022</v>
           </cell>
           <cell r="X153">
-            <v>10</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="154">
           <cell r="A154">
-            <v>55900022</v>
+            <v>55900023</v>
           </cell>
           <cell r="X154">
-            <v>20</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="155">
           <cell r="A155">
-            <v>55900023</v>
+            <v>55900024</v>
           </cell>
           <cell r="X155">
-            <v>25</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="156">
           <cell r="A156">
-            <v>55900024</v>
+            <v>55900025</v>
           </cell>
           <cell r="X156">
             <v>10</v>
@@ -4783,61 +4783,60 @@
         </row>
         <row r="157">
           <cell r="A157">
-            <v>55900025</v>
+            <v>55900026</v>
           </cell>
           <cell r="X157">
-            <v>10</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="158">
           <cell r="A158">
-            <v>55900026</v>
+            <v>55900027</v>
           </cell>
           <cell r="X158">
-            <v>20</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="159">
           <cell r="A159">
-            <v>55900027</v>
-          </cell>
-          <cell r="X159">
-            <v>35</v>
+            <v>55900028</v>
           </cell>
         </row>
         <row r="160">
           <cell r="A160">
-            <v>55900028</v>
-          </cell>
-          <cell r="X160"/>
+            <v>55900029</v>
+          </cell>
+          <cell r="X160">
+            <v>15</v>
+          </cell>
         </row>
         <row r="161">
           <cell r="A161">
-            <v>55900029</v>
+            <v>55900030</v>
           </cell>
           <cell r="X161">
-            <v>15</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="162">
           <cell r="A162">
-            <v>55900030</v>
+            <v>55900031</v>
           </cell>
           <cell r="X162">
-            <v>25</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="163">
           <cell r="A163">
-            <v>55900031</v>
+            <v>55900032</v>
           </cell>
           <cell r="X163">
-            <v>5</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="164">
           <cell r="A164">
-            <v>55900032</v>
+            <v>55900033</v>
           </cell>
           <cell r="X164">
             <v>20</v>
@@ -4845,15 +4844,15 @@
         </row>
         <row r="165">
           <cell r="A165">
-            <v>55900033</v>
+            <v>55900034</v>
           </cell>
           <cell r="X165">
-            <v>20</v>
+            <v>14</v>
           </cell>
         </row>
         <row r="166">
           <cell r="A166">
-            <v>55900034</v>
+            <v>55900035</v>
           </cell>
           <cell r="X166">
             <v>14</v>
@@ -4861,31 +4860,31 @@
         </row>
         <row r="167">
           <cell r="A167">
-            <v>55900035</v>
+            <v>55900036</v>
           </cell>
           <cell r="X167">
-            <v>14</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="168">
           <cell r="A168">
-            <v>55900036</v>
+            <v>55900037</v>
           </cell>
           <cell r="X168">
-            <v>50</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="169">
           <cell r="A169">
-            <v>55900037</v>
+            <v>55900038</v>
           </cell>
           <cell r="X169">
-            <v>35</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="170">
           <cell r="A170">
-            <v>55900038</v>
+            <v>55900039</v>
           </cell>
           <cell r="X170">
             <v>40</v>
@@ -4893,55 +4892,55 @@
         </row>
         <row r="171">
           <cell r="A171">
-            <v>55900039</v>
+            <v>55900040</v>
           </cell>
           <cell r="X171">
-            <v>40</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="172">
           <cell r="A172">
-            <v>55900040</v>
+            <v>55900041</v>
           </cell>
           <cell r="X172">
-            <v>30</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="173">
           <cell r="A173">
-            <v>55900041</v>
+            <v>55900042</v>
           </cell>
           <cell r="X173">
-            <v>0</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="174">
           <cell r="A174">
-            <v>55900042</v>
+            <v>55900043</v>
           </cell>
           <cell r="X174">
-            <v>25</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="175">
           <cell r="A175">
-            <v>55900043</v>
+            <v>55900044</v>
           </cell>
           <cell r="X175">
-            <v>30</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="176">
           <cell r="A176">
-            <v>55900044</v>
+            <v>55900045</v>
           </cell>
           <cell r="X176">
-            <v>40</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="177">
           <cell r="A177">
-            <v>55900045</v>
+            <v>55900046</v>
           </cell>
           <cell r="X177">
             <v>25</v>
@@ -4949,26 +4948,26 @@
         </row>
         <row r="178">
           <cell r="A178">
-            <v>55900046</v>
+            <v>55900047</v>
           </cell>
           <cell r="X178">
-            <v>25</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="179">
           <cell r="A179">
-            <v>55900047</v>
+            <v>55900048</v>
           </cell>
           <cell r="X179">
-            <v>30</v>
+            <v>70</v>
           </cell>
         </row>
         <row r="180">
           <cell r="A180">
-            <v>55900048</v>
+            <v>55900049</v>
           </cell>
           <cell r="X180">
-            <v>70</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="181">
@@ -5504,10 +5503,10 @@
   <dimension ref="A1:AF124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B88" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L105" sqref="L105"/>
+      <selection pane="bottomRight" activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6631,7 +6630,7 @@
         <v>0</v>
       </c>
       <c r="Q12" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R12" s="8">
         <v>10</v>
@@ -6657,14 +6656,10 @@
       </c>
       <c r="Y12" s="8">
         <f>IF(ISBLANK(Z12),0, LOOKUP(Z12,[1]Skill!$A:$A,[1]Skill!$X:$X)*AA12/100)</f>
-        <v>15</v>
-      </c>
-      <c r="Z12" s="13">
-        <v>55100009</v>
-      </c>
-      <c r="AA12" s="4">
-        <v>100</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Z12" s="13"/>
+      <c r="AA12" s="4"/>
       <c r="AB12" s="4" t="s">
         <v>5</v>
       </c>
@@ -7369,7 +7364,7 @@
         <v>0</v>
       </c>
       <c r="AF19" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:32">
@@ -7565,7 +7560,7 @@
         <v>0</v>
       </c>
       <c r="AF21" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:32">
@@ -8238,7 +8233,7 @@
         <v>0</v>
       </c>
       <c r="AF28" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:32">
@@ -8933,7 +8928,7 @@
         <v>0</v>
       </c>
       <c r="AF35" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:32">
@@ -15161,7 +15156,7 @@
         <v>0</v>
       </c>
       <c r="U100" s="10">
-        <f t="shared" ref="U100:U131" si="7">J100+K100-100+L100+ SUM(N100:T100)*5+IF(ISNUMBER(Y100),Y100,0)+X100</f>
+        <f t="shared" ref="U100:U124" si="7">J100+K100-100+L100+ SUM(N100:T100)*5+IF(ISNUMBER(Y100),Y100,0)+X100</f>
         <v>0</v>
       </c>
       <c r="V100" s="8">
@@ -16752,7 +16747,7 @@
         <v>0</v>
       </c>
       <c r="AF116" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:32">

</xml_diff>

<commit_message>
finish card for hunters
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Weapon.xlsx
+++ b/ConfigData/Xlsx/Weapon.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="36" windowWidth="18132" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="376">
   <si>
     <t>铁杖</t>
   </si>
@@ -1262,6 +1262,26 @@
   </si>
   <si>
     <t>PArmor</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>arrow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>幽篁</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Silent Bamboo</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gladiator Longbow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>角斗士长弓</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2201,138 +2221,6 @@
   <dxfs count="87">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2934,6 +2822,44 @@
         <name val="宋体"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3566,6 +3492,100 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4646,199 +4666,199 @@
         </row>
         <row r="133">
           <cell r="A133">
-            <v>55900001</v>
+            <v>55700006</v>
           </cell>
           <cell r="X133">
-            <v>35</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="134">
           <cell r="A134">
-            <v>55900002</v>
+            <v>55900001</v>
           </cell>
           <cell r="X134">
-            <v>30</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="135">
           <cell r="A135">
-            <v>55900003</v>
+            <v>55900002</v>
           </cell>
           <cell r="X135">
-            <v>80</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="136">
           <cell r="A136">
-            <v>55900004</v>
+            <v>55900003</v>
           </cell>
           <cell r="X136">
-            <v>-30</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="137">
           <cell r="A137">
-            <v>55900005</v>
+            <v>55900004</v>
           </cell>
           <cell r="X137">
-            <v>20</v>
+            <v>-30</v>
           </cell>
         </row>
         <row r="138">
           <cell r="A138">
-            <v>55900006</v>
+            <v>55900005</v>
           </cell>
           <cell r="X138">
-            <v>35</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="139">
           <cell r="A139">
-            <v>55900007</v>
+            <v>55900006</v>
           </cell>
           <cell r="X139">
-            <v>25</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="140">
           <cell r="A140">
-            <v>55900008</v>
+            <v>55900007</v>
           </cell>
           <cell r="X140">
-            <v>40</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="141">
           <cell r="A141">
-            <v>55900009</v>
+            <v>55900008</v>
           </cell>
           <cell r="X141">
-            <v>30</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="142">
           <cell r="A142">
-            <v>55900010</v>
+            <v>55900009</v>
           </cell>
           <cell r="X142">
-            <v>20</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="143">
           <cell r="A143">
-            <v>55900011</v>
+            <v>55900010</v>
           </cell>
           <cell r="X143">
-            <v>15</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="144">
           <cell r="A144">
-            <v>55900012</v>
+            <v>55900011</v>
           </cell>
           <cell r="X144">
-            <v>25</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="145">
           <cell r="A145">
-            <v>55900013</v>
+            <v>55900012</v>
           </cell>
           <cell r="X145">
-            <v>10</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="146">
           <cell r="A146">
-            <v>55900014</v>
+            <v>55900013</v>
           </cell>
           <cell r="X146">
-            <v>20</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="147">
           <cell r="A147">
-            <v>55900015</v>
+            <v>55900014</v>
           </cell>
           <cell r="X147">
-            <v>30</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="148">
           <cell r="A148">
-            <v>55900016</v>
+            <v>55900015</v>
           </cell>
           <cell r="X148">
-            <v>45</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="149">
           <cell r="A149">
-            <v>55900017</v>
+            <v>55900016</v>
           </cell>
           <cell r="X149">
-            <v>10</v>
+            <v>45</v>
           </cell>
         </row>
         <row r="150">
           <cell r="A150">
-            <v>55900018</v>
+            <v>55900017</v>
           </cell>
           <cell r="X150">
-            <v>30</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="151">
           <cell r="A151">
-            <v>55900019</v>
+            <v>55900018</v>
           </cell>
           <cell r="X151">
-            <v>80</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="152">
           <cell r="A152">
-            <v>55900020</v>
+            <v>55900019</v>
           </cell>
           <cell r="X152">
-            <v>20</v>
+            <v>80</v>
           </cell>
         </row>
         <row r="153">
           <cell r="A153">
-            <v>55900021</v>
+            <v>55900020</v>
           </cell>
           <cell r="X153">
-            <v>10</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="154">
           <cell r="A154">
-            <v>55900022</v>
+            <v>55900021</v>
           </cell>
           <cell r="X154">
-            <v>20</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="155">
           <cell r="A155">
-            <v>55900023</v>
+            <v>55900022</v>
           </cell>
           <cell r="X155">
-            <v>25</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="156">
           <cell r="A156">
-            <v>55900024</v>
+            <v>55900023</v>
           </cell>
           <cell r="X156">
-            <v>10</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="157">
           <cell r="A157">
-            <v>55900025</v>
+            <v>55900024</v>
           </cell>
           <cell r="X157">
             <v>10</v>
@@ -4846,61 +4866,61 @@
         </row>
         <row r="158">
           <cell r="A158">
-            <v>55900026</v>
+            <v>55900025</v>
           </cell>
           <cell r="X158">
-            <v>20</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="159">
           <cell r="A159">
-            <v>55900027</v>
+            <v>55900026</v>
           </cell>
           <cell r="X159">
-            <v>35</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="160">
           <cell r="A160">
-            <v>55900028</v>
-          </cell>
-          <cell r="X160"/>
+            <v>55900027</v>
+          </cell>
+          <cell r="X160">
+            <v>35</v>
+          </cell>
         </row>
         <row r="161">
           <cell r="A161">
-            <v>55900029</v>
-          </cell>
-          <cell r="X161">
-            <v>15</v>
-          </cell>
+            <v>55900028</v>
+          </cell>
+          <cell r="X161"/>
         </row>
         <row r="162">
           <cell r="A162">
-            <v>55900030</v>
+            <v>55900029</v>
           </cell>
           <cell r="X162">
-            <v>25</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="163">
           <cell r="A163">
-            <v>55900031</v>
+            <v>55900030</v>
           </cell>
           <cell r="X163">
-            <v>5</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="164">
           <cell r="A164">
-            <v>55900032</v>
+            <v>55900031</v>
           </cell>
           <cell r="X164">
-            <v>20</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="165">
           <cell r="A165">
-            <v>55900033</v>
+            <v>55900032</v>
           </cell>
           <cell r="X165">
             <v>20</v>
@@ -4908,15 +4928,15 @@
         </row>
         <row r="166">
           <cell r="A166">
-            <v>55900034</v>
+            <v>55900033</v>
           </cell>
           <cell r="X166">
-            <v>14</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="167">
           <cell r="A167">
-            <v>55900035</v>
+            <v>55900034</v>
           </cell>
           <cell r="X167">
             <v>14</v>
@@ -4924,31 +4944,31 @@
         </row>
         <row r="168">
           <cell r="A168">
-            <v>55900036</v>
+            <v>55900035</v>
           </cell>
           <cell r="X168">
-            <v>50</v>
+            <v>14</v>
           </cell>
         </row>
         <row r="169">
           <cell r="A169">
-            <v>55900037</v>
+            <v>55900036</v>
           </cell>
           <cell r="X169">
-            <v>35</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="170">
           <cell r="A170">
-            <v>55900038</v>
+            <v>55900037</v>
           </cell>
           <cell r="X170">
-            <v>40</v>
+            <v>35</v>
           </cell>
         </row>
         <row r="171">
           <cell r="A171">
-            <v>55900039</v>
+            <v>55900038</v>
           </cell>
           <cell r="X171">
             <v>40</v>
@@ -4956,55 +4976,55 @@
         </row>
         <row r="172">
           <cell r="A172">
-            <v>55900040</v>
+            <v>55900039</v>
           </cell>
           <cell r="X172">
-            <v>30</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="173">
           <cell r="A173">
-            <v>55900041</v>
+            <v>55900040</v>
           </cell>
           <cell r="X173">
-            <v>0</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="174">
           <cell r="A174">
-            <v>55900042</v>
+            <v>55900041</v>
           </cell>
           <cell r="X174">
-            <v>25</v>
+            <v>0</v>
           </cell>
         </row>
         <row r="175">
           <cell r="A175">
-            <v>55900043</v>
+            <v>55900042</v>
           </cell>
           <cell r="X175">
-            <v>30</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="176">
           <cell r="A176">
-            <v>55900044</v>
+            <v>55900043</v>
           </cell>
           <cell r="X176">
-            <v>40</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="177">
           <cell r="A177">
-            <v>55900045</v>
+            <v>55900044</v>
           </cell>
           <cell r="X177">
-            <v>25</v>
+            <v>40</v>
           </cell>
         </row>
         <row r="178">
           <cell r="A178">
-            <v>55900046</v>
+            <v>55900045</v>
           </cell>
           <cell r="X178">
             <v>25</v>
@@ -5012,71 +5032,71 @@
         </row>
         <row r="179">
           <cell r="A179">
-            <v>55900047</v>
+            <v>55900046</v>
           </cell>
           <cell r="X179">
-            <v>30</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="180">
           <cell r="A180">
-            <v>55900048</v>
+            <v>55900047</v>
           </cell>
           <cell r="X180">
-            <v>70</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="181">
           <cell r="A181">
-            <v>55900049</v>
+            <v>55900048</v>
           </cell>
           <cell r="X181">
-            <v>25</v>
+            <v>70</v>
           </cell>
         </row>
         <row r="182">
           <cell r="A182">
-            <v>55900050</v>
+            <v>55900049</v>
           </cell>
           <cell r="X182">
-            <v>20</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="183">
           <cell r="A183">
-            <v>55900051</v>
+            <v>55900050</v>
           </cell>
           <cell r="X183">
-            <v>25</v>
+            <v>20</v>
           </cell>
         </row>
         <row r="184">
           <cell r="A184">
-            <v>55990001</v>
+            <v>55900051</v>
           </cell>
           <cell r="X184">
-            <v>15</v>
+            <v>25</v>
           </cell>
         </row>
         <row r="185">
           <cell r="A185">
-            <v>55990002</v>
+            <v>55900052</v>
           </cell>
           <cell r="X185">
-            <v>15</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="186">
           <cell r="A186">
-            <v>55990003</v>
+            <v>55900053</v>
           </cell>
           <cell r="X186">
-            <v>15</v>
+            <v>30</v>
           </cell>
         </row>
         <row r="187">
           <cell r="A187">
-            <v>55990004</v>
+            <v>55900054</v>
           </cell>
           <cell r="X187">
             <v>15</v>
@@ -5084,7 +5104,7 @@
         </row>
         <row r="188">
           <cell r="A188">
-            <v>55990005</v>
+            <v>55990001</v>
           </cell>
           <cell r="X188">
             <v>15</v>
@@ -5092,7 +5112,7 @@
         </row>
         <row r="189">
           <cell r="A189">
-            <v>55990006</v>
+            <v>55990002</v>
           </cell>
           <cell r="X189">
             <v>15</v>
@@ -5100,7 +5120,7 @@
         </row>
         <row r="190">
           <cell r="A190">
-            <v>55990011</v>
+            <v>55990003</v>
           </cell>
           <cell r="X190">
             <v>15</v>
@@ -5108,7 +5128,7 @@
         </row>
         <row r="191">
           <cell r="A191">
-            <v>55990012</v>
+            <v>55990004</v>
           </cell>
           <cell r="X191">
             <v>15</v>
@@ -5116,7 +5136,7 @@
         </row>
         <row r="192">
           <cell r="A192">
-            <v>55990013</v>
+            <v>55990005</v>
           </cell>
           <cell r="X192">
             <v>15</v>
@@ -5124,7 +5144,7 @@
         </row>
         <row r="193">
           <cell r="A193">
-            <v>55990014</v>
+            <v>55990006</v>
           </cell>
           <cell r="X193">
             <v>15</v>
@@ -5132,7 +5152,7 @@
         </row>
         <row r="194">
           <cell r="A194">
-            <v>55990015</v>
+            <v>55990011</v>
           </cell>
           <cell r="X194">
             <v>15</v>
@@ -5140,7 +5160,7 @@
         </row>
         <row r="195">
           <cell r="A195">
-            <v>55990016</v>
+            <v>55990012</v>
           </cell>
           <cell r="X195">
             <v>15</v>
@@ -5148,41 +5168,73 @@
         </row>
         <row r="196">
           <cell r="A196">
-            <v>55990101</v>
+            <v>55990013</v>
           </cell>
           <cell r="X196">
-            <v>8</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="197">
           <cell r="A197">
-            <v>55990102</v>
+            <v>55990014</v>
           </cell>
           <cell r="X197">
-            <v>25</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="198">
           <cell r="A198">
-            <v>55990103</v>
+            <v>55990015</v>
           </cell>
           <cell r="X198">
-            <v>35</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="199">
           <cell r="A199">
-            <v>55990104</v>
+            <v>55990016</v>
           </cell>
           <cell r="X199">
-            <v>50</v>
+            <v>15</v>
           </cell>
         </row>
         <row r="200">
           <cell r="A200">
+            <v>55990101</v>
+          </cell>
+          <cell r="X200">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="201">
+          <cell r="A201">
+            <v>55990102</v>
+          </cell>
+          <cell r="X201">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="202">
+          <cell r="A202">
+            <v>55990103</v>
+          </cell>
+          <cell r="X202">
+            <v>35</v>
+          </cell>
+        </row>
+        <row r="203">
+          <cell r="A203">
+            <v>55990104</v>
+          </cell>
+          <cell r="X203">
+            <v>50</v>
+          </cell>
+        </row>
+        <row r="204">
+          <cell r="A204">
             <v>55990105</v>
           </cell>
-          <cell r="X200">
+          <cell r="X204">
             <v>150</v>
           </cell>
         </row>
@@ -5194,102 +5246,102 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AG125" totalsRowShown="0" dataDxfId="86" tableBorderDxfId="85">
-  <autoFilter ref="A3:AG125"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AG127" totalsRowShown="0" dataDxfId="73" tableBorderDxfId="72">
+  <autoFilter ref="A3:AG127"/>
   <sortState ref="A4:AF124">
     <sortCondition ref="A3:A124"/>
   </sortState>
   <tableColumns count="33">
-    <tableColumn id="1" name="Id" dataDxfId="84"/>
-    <tableColumn id="2" name="Name" dataDxfId="83"/>
-    <tableColumn id="3" name="Ename" dataDxfId="82"/>
-    <tableColumn id="4" name="Remark" dataDxfId="81"/>
-    <tableColumn id="5" name="Star" dataDxfId="80"/>
-    <tableColumn id="6" name="Type" dataDxfId="79"/>
-    <tableColumn id="7" name="Attr" dataDxfId="78"/>
-    <tableColumn id="34" name="Quality" dataDxfId="77">
+    <tableColumn id="1" name="Id" dataDxfId="71"/>
+    <tableColumn id="2" name="Name" dataDxfId="70"/>
+    <tableColumn id="3" name="Ename" dataDxfId="69"/>
+    <tableColumn id="4" name="Remark" dataDxfId="68"/>
+    <tableColumn id="5" name="Star" dataDxfId="67"/>
+    <tableColumn id="6" name="Type" dataDxfId="66"/>
+    <tableColumn id="7" name="Attr" dataDxfId="65"/>
+    <tableColumn id="34" name="Quality" dataDxfId="64">
       <calculatedColumnFormula>IF(AND(V4&gt;=13,V4&lt;=16),5,IF(AND(V4&gt;=9,V4&lt;=12),4,IF(AND(V4&gt;=5,V4&lt;=8),3,IF(AND(V4&gt;=1,V4&lt;=4),2,IF(AND(V4&gt;=-3,V4&lt;=0),1,IF(AND(V4&gt;=-5,V4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Cost" dataDxfId="76"/>
-    <tableColumn id="8" name="AtkP" dataDxfId="75"/>
-    <tableColumn id="9" name="PArmor" dataDxfId="74"/>
-    <tableColumn id="17" name="MArmor" dataDxfId="73"/>
-    <tableColumn id="25" name="Modify" dataDxfId="72"/>
-    <tableColumn id="27" name="Dura" dataDxfId="71"/>
-    <tableColumn id="20" name="Def" dataDxfId="70"/>
-    <tableColumn id="21" name="Mag" dataDxfId="69"/>
-    <tableColumn id="29" name="Spd" dataDxfId="68"/>
-    <tableColumn id="30" name="Hit" dataDxfId="67"/>
-    <tableColumn id="19" name="Dhit" dataDxfId="66"/>
-    <tableColumn id="12" name="Crt" dataDxfId="65"/>
-    <tableColumn id="11" name="Luk" dataDxfId="64"/>
-    <tableColumn id="32" name="Sum" dataDxfId="63">
+    <tableColumn id="15" name="Cost" dataDxfId="63"/>
+    <tableColumn id="8" name="AtkP" dataDxfId="62"/>
+    <tableColumn id="9" name="PArmor" dataDxfId="61"/>
+    <tableColumn id="17" name="MArmor" dataDxfId="60"/>
+    <tableColumn id="25" name="Modify" dataDxfId="59"/>
+    <tableColumn id="27" name="Dura" dataDxfId="58"/>
+    <tableColumn id="20" name="Def" dataDxfId="57"/>
+    <tableColumn id="21" name="Mag" dataDxfId="56"/>
+    <tableColumn id="29" name="Spd" dataDxfId="55"/>
+    <tableColumn id="30" name="Hit" dataDxfId="54"/>
+    <tableColumn id="19" name="Dhit" dataDxfId="53"/>
+    <tableColumn id="12" name="Crt" dataDxfId="52"/>
+    <tableColumn id="11" name="Luk" dataDxfId="51"/>
+    <tableColumn id="32" name="Sum" dataDxfId="50">
       <calculatedColumnFormula>J4+K4+L4-100+M4+ SUM(O4:U4)*5+IF(ISNUMBER(Z4),Z4,0)+Y4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Range" dataDxfId="62"/>
-    <tableColumn id="31" name="Mov" dataDxfId="61"/>
-    <tableColumn id="24" name="~SkillMark" dataDxfId="60"/>
-    <tableColumn id="33" name="~SkillMark2" dataDxfId="59">
+    <tableColumn id="10" name="Range" dataDxfId="49"/>
+    <tableColumn id="31" name="Mov" dataDxfId="48"/>
+    <tableColumn id="24" name="~SkillMark" dataDxfId="47"/>
+    <tableColumn id="33" name="~SkillMark2" dataDxfId="46">
       <calculatedColumnFormula>IF(ISBLANK(AA4),0, LOOKUP(AA4,[1]Skill!$A:$A,[1]Skill!$X:$X)*AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="SkillId" dataDxfId="58"/>
-    <tableColumn id="14" name="Percent" dataDxfId="57"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="56"/>
-    <tableColumn id="26" name="JobId" dataDxfId="55"/>
-    <tableColumn id="18" name="Icon" dataDxfId="54"/>
-    <tableColumn id="22" name="IsSpecial" dataDxfId="53"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="52"/>
+    <tableColumn id="13" name="SkillId" dataDxfId="45"/>
+    <tableColumn id="14" name="Percent" dataDxfId="44"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="43"/>
+    <tableColumn id="26" name="JobId" dataDxfId="42"/>
+    <tableColumn id="18" name="Icon" dataDxfId="41"/>
+    <tableColumn id="22" name="IsSpecial" dataDxfId="40"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AG4" totalsRowShown="0" dataDxfId="51" tableBorderDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AG4" totalsRowShown="0" dataDxfId="33" tableBorderDxfId="32">
   <autoFilter ref="A3:AG4"/>
   <sortState ref="A4:W130">
     <sortCondition ref="A3:A130"/>
   </sortState>
   <tableColumns count="33">
-    <tableColumn id="1" name="Id" dataDxfId="49"/>
-    <tableColumn id="2" name="Name" dataDxfId="48"/>
-    <tableColumn id="3" name="Ename" dataDxfId="47"/>
-    <tableColumn id="4" name="Remark" dataDxfId="46"/>
-    <tableColumn id="5" name="Star" dataDxfId="45"/>
-    <tableColumn id="6" name="Type" dataDxfId="44"/>
-    <tableColumn id="7" name="Attr" dataDxfId="43"/>
-    <tableColumn id="34" name="Quality" dataDxfId="42">
+    <tableColumn id="1" name="Id" dataDxfId="31"/>
+    <tableColumn id="2" name="Name" dataDxfId="30"/>
+    <tableColumn id="3" name="Ename" dataDxfId="29"/>
+    <tableColumn id="4" name="Remark" dataDxfId="28"/>
+    <tableColumn id="5" name="Star" dataDxfId="27"/>
+    <tableColumn id="6" name="Type" dataDxfId="26"/>
+    <tableColumn id="7" name="Attr" dataDxfId="25"/>
+    <tableColumn id="34" name="Quality" dataDxfId="24">
       <calculatedColumnFormula>IF(AND(V4&gt;=13,V4&lt;=16),5,IF(AND(V4&gt;=9,V4&lt;=12),4,IF(AND(V4&gt;=5,V4&lt;=8),3,IF(AND(V4&gt;=1,V4&lt;=4),2,IF(AND(V4&gt;=-3,V4&lt;=0),1,IF(AND(V4&gt;=-5,V4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Cost" dataDxfId="41"/>
-    <tableColumn id="8" name="AtkP" dataDxfId="40"/>
-    <tableColumn id="9" name="PArmor" dataDxfId="39"/>
-    <tableColumn id="17" name="MArmor" dataDxfId="38"/>
-    <tableColumn id="25" name="Modify" dataDxfId="37"/>
-    <tableColumn id="31" name="Dura" dataDxfId="36"/>
-    <tableColumn id="11" name="Def" dataDxfId="35"/>
-    <tableColumn id="21" name="Mag" dataDxfId="34"/>
-    <tableColumn id="29" name="Spd" dataDxfId="33"/>
-    <tableColumn id="30" name="Hit" dataDxfId="32"/>
-    <tableColumn id="20" name="Dhit" dataDxfId="31"/>
-    <tableColumn id="19" name="Crt" dataDxfId="30"/>
-    <tableColumn id="12" name="Luk" dataDxfId="29"/>
-    <tableColumn id="32" name="Sum" dataDxfId="28">
+    <tableColumn id="15" name="Cost" dataDxfId="23"/>
+    <tableColumn id="8" name="AtkP" dataDxfId="22"/>
+    <tableColumn id="9" name="PArmor" dataDxfId="21"/>
+    <tableColumn id="17" name="MArmor" dataDxfId="20"/>
+    <tableColumn id="25" name="Modify" dataDxfId="19"/>
+    <tableColumn id="31" name="Dura" dataDxfId="18"/>
+    <tableColumn id="11" name="Def" dataDxfId="17"/>
+    <tableColumn id="21" name="Mag" dataDxfId="16"/>
+    <tableColumn id="29" name="Spd" dataDxfId="15"/>
+    <tableColumn id="30" name="Hit" dataDxfId="14"/>
+    <tableColumn id="20" name="Dhit" dataDxfId="13"/>
+    <tableColumn id="19" name="Crt" dataDxfId="12"/>
+    <tableColumn id="12" name="Luk" dataDxfId="11"/>
+    <tableColumn id="32" name="Sum" dataDxfId="10">
       <calculatedColumnFormula>J4+K4+L4-100+M4+ SUM(O4:U4)*5+IF(ISNUMBER(Z4),Z4,0)+Y4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Range" dataDxfId="27"/>
-    <tableColumn id="27" name="Mov" dataDxfId="26"/>
-    <tableColumn id="24" name="~SkillMark" dataDxfId="25"/>
-    <tableColumn id="33" name="~SkillMark2" dataDxfId="24">
+    <tableColumn id="10" name="Range" dataDxfId="9"/>
+    <tableColumn id="27" name="Mov" dataDxfId="8"/>
+    <tableColumn id="24" name="~SkillMark" dataDxfId="7"/>
+    <tableColumn id="33" name="~SkillMark2" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(AA4),0, LOOKUP(AA4,[1]Skill!$A:$A,[1]Skill!$X:$X)*AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="SkillId" dataDxfId="23"/>
-    <tableColumn id="14" name="Percent" dataDxfId="22"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="21"/>
+    <tableColumn id="13" name="SkillId" dataDxfId="5"/>
+    <tableColumn id="14" name="Percent" dataDxfId="4"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="3"/>
     <tableColumn id="26" name="JobId"/>
-    <tableColumn id="18" name="Icon" dataDxfId="20"/>
-    <tableColumn id="22" name="IsSpecial" dataDxfId="19"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="18"/>
+    <tableColumn id="18" name="Icon" dataDxfId="2"/>
+    <tableColumn id="22" name="IsSpecial" dataDxfId="1"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5582,13 +5634,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG125"/>
+  <dimension ref="A1:AG127"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomRight" activeCell="AC7" sqref="AC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8124,13 +8176,13 @@
       </c>
       <c r="H26" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I26" s="15">
         <v>4</v>
       </c>
       <c r="J26" s="16">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="K26" s="16">
         <v>0</v>
@@ -8139,7 +8191,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="8">
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="N26" s="8">
         <v>6</v>
@@ -8154,7 +8206,7 @@
         <v>0</v>
       </c>
       <c r="R26" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="S26" s="8">
         <v>0</v>
@@ -8167,7 +8219,7 @@
       </c>
       <c r="V26" s="10">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="W26" s="8">
         <v>30</v>
@@ -17098,7 +17150,7 @@
         <v>355</v>
       </c>
       <c r="E116" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F116">
         <v>100</v>
@@ -17108,10 +17160,10 @@
       </c>
       <c r="H116" s="4">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I116" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J116" s="6">
         <v>45</v>
@@ -17123,7 +17175,7 @@
         <v>0</v>
       </c>
       <c r="M116" s="14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N116" s="8">
         <v>4</v>
@@ -17151,7 +17203,7 @@
       </c>
       <c r="V116" s="36">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="W116" s="8">
         <v>20</v>
@@ -18077,6 +18129,202 @@
         <v>0</v>
       </c>
       <c r="AG125" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:33">
+      <c r="A126">
+        <v>52000123</v>
+      </c>
+      <c r="B126" s="15" t="s">
+        <v>372</v>
+      </c>
+      <c r="C126" s="15" t="s">
+        <v>373</v>
+      </c>
+      <c r="D126" s="42"/>
+      <c r="E126" s="15">
+        <v>3</v>
+      </c>
+      <c r="F126" s="15">
+        <v>100</v>
+      </c>
+      <c r="G126" s="15">
+        <v>0</v>
+      </c>
+      <c r="H126" s="41">
+        <f t="shared" ref="H126:H127" si="9">IF(AND(V126&gt;=13,V126&lt;=16),5,IF(AND(V126&gt;=9,V126&lt;=12),4,IF(AND(V126&gt;=5,V126&lt;=8),3,IF(AND(V126&gt;=1,V126&lt;=4),2,IF(AND(V126&gt;=-3,V126&lt;=0),1,IF(AND(V126&gt;=-5,V126&lt;=-4),0,6))))))</f>
+        <v>2</v>
+      </c>
+      <c r="I126" s="15">
+        <v>3</v>
+      </c>
+      <c r="J126" s="16">
+        <v>100</v>
+      </c>
+      <c r="K126" s="16">
+        <v>0</v>
+      </c>
+      <c r="L126" s="7">
+        <v>0</v>
+      </c>
+      <c r="M126" s="14">
+        <v>-44</v>
+      </c>
+      <c r="N126" s="8">
+        <v>4</v>
+      </c>
+      <c r="O126" s="8">
+        <v>0</v>
+      </c>
+      <c r="P126" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q126" s="8">
+        <v>2</v>
+      </c>
+      <c r="R126" s="8">
+        <v>0</v>
+      </c>
+      <c r="S126" s="8">
+        <v>0</v>
+      </c>
+      <c r="T126" s="8">
+        <v>0</v>
+      </c>
+      <c r="U126" s="8">
+        <v>0</v>
+      </c>
+      <c r="V126" s="10">
+        <f t="shared" ref="V126:V127" si="10">J126+K126+L126-100+M126+ SUM(O126:U126)*5+IF(ISNUMBER(Z126),Z126,0)+Y126</f>
+        <v>1</v>
+      </c>
+      <c r="W126" s="8">
+        <v>20</v>
+      </c>
+      <c r="X126" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y126" s="8">
+        <v>25</v>
+      </c>
+      <c r="Z126" s="10">
+        <f>IF(ISBLANK(AA126),0, LOOKUP(AA126,[1]Skill!$A:$A,[1]Skill!$X:$X)*AB126/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AA126" s="15"/>
+      <c r="AB126" s="15"/>
+      <c r="AC126" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="AD126" s="15">
+        <v>11000004</v>
+      </c>
+      <c r="AE126" s="17">
+        <v>123</v>
+      </c>
+      <c r="AF126" s="26">
+        <v>0</v>
+      </c>
+      <c r="AG126" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:33">
+      <c r="A127">
+        <v>52000124</v>
+      </c>
+      <c r="B127" s="15" t="s">
+        <v>375</v>
+      </c>
+      <c r="C127" s="15" t="s">
+        <v>374</v>
+      </c>
+      <c r="D127" s="42"/>
+      <c r="E127" s="15">
+        <v>6</v>
+      </c>
+      <c r="F127" s="15">
+        <v>100</v>
+      </c>
+      <c r="G127" s="15">
+        <v>0</v>
+      </c>
+      <c r="H127" s="41">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="I127" s="15">
+        <v>6</v>
+      </c>
+      <c r="J127" s="16">
+        <v>100</v>
+      </c>
+      <c r="K127" s="16">
+        <v>0</v>
+      </c>
+      <c r="L127" s="7">
+        <v>0</v>
+      </c>
+      <c r="M127" s="14">
+        <v>-40</v>
+      </c>
+      <c r="N127" s="8">
+        <v>2</v>
+      </c>
+      <c r="O127" s="8">
+        <v>0</v>
+      </c>
+      <c r="P127" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q127" s="8">
+        <v>0</v>
+      </c>
+      <c r="R127" s="8">
+        <v>1</v>
+      </c>
+      <c r="S127" s="8">
+        <v>0</v>
+      </c>
+      <c r="T127" s="8">
+        <v>3</v>
+      </c>
+      <c r="U127" s="8">
+        <v>0</v>
+      </c>
+      <c r="V127" s="10">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="W127" s="8">
+        <v>20</v>
+      </c>
+      <c r="X127" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y127" s="8">
+        <v>25</v>
+      </c>
+      <c r="Z127" s="10">
+        <f>IF(ISBLANK(AA127),0, LOOKUP(AA127,[1]Skill!$A:$A,[1]Skill!$X:$X)*AB127/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AA127" s="15"/>
+      <c r="AB127" s="15"/>
+      <c r="AC127" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="AD127" s="15">
+        <v>11000004</v>
+      </c>
+      <c r="AE127" s="17">
+        <v>124</v>
+      </c>
+      <c r="AF127" s="26">
+        <v>0</v>
+      </c>
+      <c r="AG127" s="15">
         <v>1</v>
       </c>
     </row>
@@ -18275,37 +18523,37 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H124">
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="12" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="13" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="83" priority="14" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="6" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="8" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="9" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="10" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V4:V125">
+  <conditionalFormatting sqref="V4:V127">
     <cfRule type="colorScale" priority="95">
       <colorScale>
         <cfvo type="min"/>
@@ -18317,21 +18565,21 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H125">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+  <conditionalFormatting sqref="H125:H127">
+    <cfRule type="cellIs" dxfId="77" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="74" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V125">
+  <conditionalFormatting sqref="V125:V127">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -18355,7 +18603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -18780,19 +19028,19 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="2" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add 2 new weapons
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Weapon.xlsx
+++ b/ConfigData/Xlsx/Weapon.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="380">
   <si>
     <t>铁杖</t>
   </si>
@@ -1282,6 +1282,22 @@
   </si>
   <si>
     <t>角斗士长弓</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Glaive</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>阔剑</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>夜叉</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yaksha</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2218,7 +2234,35 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="87">
+  <dxfs count="91">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -5246,102 +5290,108 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AG127" totalsRowShown="0" dataDxfId="73" tableBorderDxfId="72">
-  <autoFilter ref="A3:AG127"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AG129" totalsRowShown="0" dataDxfId="77" tableBorderDxfId="76">
+  <autoFilter ref="A3:AG129">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="2"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A4:AF124">
     <sortCondition ref="A3:A124"/>
   </sortState>
   <tableColumns count="33">
-    <tableColumn id="1" name="Id" dataDxfId="71"/>
-    <tableColumn id="2" name="Name" dataDxfId="70"/>
-    <tableColumn id="3" name="Ename" dataDxfId="69"/>
-    <tableColumn id="4" name="Remark" dataDxfId="68"/>
-    <tableColumn id="5" name="Star" dataDxfId="67"/>
-    <tableColumn id="6" name="Type" dataDxfId="66"/>
-    <tableColumn id="7" name="Attr" dataDxfId="65"/>
-    <tableColumn id="34" name="Quality" dataDxfId="64">
+    <tableColumn id="1" name="Id" dataDxfId="75"/>
+    <tableColumn id="2" name="Name" dataDxfId="74"/>
+    <tableColumn id="3" name="Ename" dataDxfId="73"/>
+    <tableColumn id="4" name="Remark" dataDxfId="72"/>
+    <tableColumn id="5" name="Star" dataDxfId="71"/>
+    <tableColumn id="6" name="Type" dataDxfId="70"/>
+    <tableColumn id="7" name="Attr" dataDxfId="69"/>
+    <tableColumn id="34" name="Quality" dataDxfId="68">
       <calculatedColumnFormula>IF(AND(V4&gt;=13,V4&lt;=16),5,IF(AND(V4&gt;=9,V4&lt;=12),4,IF(AND(V4&gt;=5,V4&lt;=8),3,IF(AND(V4&gt;=1,V4&lt;=4),2,IF(AND(V4&gt;=-3,V4&lt;=0),1,IF(AND(V4&gt;=-5,V4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Cost" dataDxfId="63"/>
-    <tableColumn id="8" name="AtkP" dataDxfId="62"/>
-    <tableColumn id="9" name="PArmor" dataDxfId="61"/>
-    <tableColumn id="17" name="MArmor" dataDxfId="60"/>
-    <tableColumn id="25" name="Modify" dataDxfId="59"/>
-    <tableColumn id="27" name="Dura" dataDxfId="58"/>
-    <tableColumn id="20" name="Def" dataDxfId="57"/>
-    <tableColumn id="21" name="Mag" dataDxfId="56"/>
-    <tableColumn id="29" name="Spd" dataDxfId="55"/>
-    <tableColumn id="30" name="Hit" dataDxfId="54"/>
-    <tableColumn id="19" name="Dhit" dataDxfId="53"/>
-    <tableColumn id="12" name="Crt" dataDxfId="52"/>
-    <tableColumn id="11" name="Luk" dataDxfId="51"/>
-    <tableColumn id="32" name="Sum" dataDxfId="50">
+    <tableColumn id="15" name="Cost" dataDxfId="67"/>
+    <tableColumn id="8" name="AtkP" dataDxfId="66"/>
+    <tableColumn id="9" name="PArmor" dataDxfId="65"/>
+    <tableColumn id="17" name="MArmor" dataDxfId="64"/>
+    <tableColumn id="25" name="Modify" dataDxfId="63"/>
+    <tableColumn id="27" name="Dura" dataDxfId="62"/>
+    <tableColumn id="20" name="Def" dataDxfId="61"/>
+    <tableColumn id="21" name="Mag" dataDxfId="60"/>
+    <tableColumn id="29" name="Spd" dataDxfId="59"/>
+    <tableColumn id="30" name="Hit" dataDxfId="58"/>
+    <tableColumn id="19" name="Dhit" dataDxfId="57"/>
+    <tableColumn id="12" name="Crt" dataDxfId="56"/>
+    <tableColumn id="11" name="Luk" dataDxfId="55"/>
+    <tableColumn id="32" name="Sum" dataDxfId="54">
       <calculatedColumnFormula>J4+K4+L4-100+M4+ SUM(O4:U4)*5+IF(ISNUMBER(Z4),Z4,0)+Y4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Range" dataDxfId="49"/>
-    <tableColumn id="31" name="Mov" dataDxfId="48"/>
-    <tableColumn id="24" name="~SkillMark" dataDxfId="47"/>
-    <tableColumn id="33" name="~SkillMark2" dataDxfId="46">
+    <tableColumn id="10" name="Range" dataDxfId="53"/>
+    <tableColumn id="31" name="Mov" dataDxfId="52"/>
+    <tableColumn id="24" name="~SkillMark" dataDxfId="51"/>
+    <tableColumn id="33" name="~SkillMark2" dataDxfId="50">
       <calculatedColumnFormula>IF(ISBLANK(AA4),0, LOOKUP(AA4,[1]Skill!$A:$A,[1]Skill!$X:$X)*AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="SkillId" dataDxfId="45"/>
-    <tableColumn id="14" name="Percent" dataDxfId="44"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="43"/>
-    <tableColumn id="26" name="JobId" dataDxfId="42"/>
-    <tableColumn id="18" name="Icon" dataDxfId="41"/>
-    <tableColumn id="22" name="IsSpecial" dataDxfId="40"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="39"/>
+    <tableColumn id="13" name="SkillId" dataDxfId="49"/>
+    <tableColumn id="14" name="Percent" dataDxfId="48"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="47"/>
+    <tableColumn id="26" name="JobId" dataDxfId="46"/>
+    <tableColumn id="18" name="Icon" dataDxfId="45"/>
+    <tableColumn id="22" name="IsSpecial" dataDxfId="44"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AG4" totalsRowShown="0" dataDxfId="33" tableBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AG4" totalsRowShown="0" dataDxfId="37" tableBorderDxfId="36">
   <autoFilter ref="A3:AG4"/>
   <sortState ref="A4:W130">
     <sortCondition ref="A3:A130"/>
   </sortState>
   <tableColumns count="33">
-    <tableColumn id="1" name="Id" dataDxfId="31"/>
-    <tableColumn id="2" name="Name" dataDxfId="30"/>
-    <tableColumn id="3" name="Ename" dataDxfId="29"/>
-    <tableColumn id="4" name="Remark" dataDxfId="28"/>
-    <tableColumn id="5" name="Star" dataDxfId="27"/>
-    <tableColumn id="6" name="Type" dataDxfId="26"/>
-    <tableColumn id="7" name="Attr" dataDxfId="25"/>
-    <tableColumn id="34" name="Quality" dataDxfId="24">
+    <tableColumn id="1" name="Id" dataDxfId="35"/>
+    <tableColumn id="2" name="Name" dataDxfId="34"/>
+    <tableColumn id="3" name="Ename" dataDxfId="33"/>
+    <tableColumn id="4" name="Remark" dataDxfId="32"/>
+    <tableColumn id="5" name="Star" dataDxfId="31"/>
+    <tableColumn id="6" name="Type" dataDxfId="30"/>
+    <tableColumn id="7" name="Attr" dataDxfId="29"/>
+    <tableColumn id="34" name="Quality" dataDxfId="28">
       <calculatedColumnFormula>IF(AND(V4&gt;=13,V4&lt;=16),5,IF(AND(V4&gt;=9,V4&lt;=12),4,IF(AND(V4&gt;=5,V4&lt;=8),3,IF(AND(V4&gt;=1,V4&lt;=4),2,IF(AND(V4&gt;=-3,V4&lt;=0),1,IF(AND(V4&gt;=-5,V4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Cost" dataDxfId="23"/>
-    <tableColumn id="8" name="AtkP" dataDxfId="22"/>
-    <tableColumn id="9" name="PArmor" dataDxfId="21"/>
-    <tableColumn id="17" name="MArmor" dataDxfId="20"/>
-    <tableColumn id="25" name="Modify" dataDxfId="19"/>
-    <tableColumn id="31" name="Dura" dataDxfId="18"/>
-    <tableColumn id="11" name="Def" dataDxfId="17"/>
-    <tableColumn id="21" name="Mag" dataDxfId="16"/>
-    <tableColumn id="29" name="Spd" dataDxfId="15"/>
-    <tableColumn id="30" name="Hit" dataDxfId="14"/>
-    <tableColumn id="20" name="Dhit" dataDxfId="13"/>
-    <tableColumn id="19" name="Crt" dataDxfId="12"/>
-    <tableColumn id="12" name="Luk" dataDxfId="11"/>
-    <tableColumn id="32" name="Sum" dataDxfId="10">
+    <tableColumn id="15" name="Cost" dataDxfId="27"/>
+    <tableColumn id="8" name="AtkP" dataDxfId="26"/>
+    <tableColumn id="9" name="PArmor" dataDxfId="25"/>
+    <tableColumn id="17" name="MArmor" dataDxfId="24"/>
+    <tableColumn id="25" name="Modify" dataDxfId="23"/>
+    <tableColumn id="31" name="Dura" dataDxfId="22"/>
+    <tableColumn id="11" name="Def" dataDxfId="21"/>
+    <tableColumn id="21" name="Mag" dataDxfId="20"/>
+    <tableColumn id="29" name="Spd" dataDxfId="19"/>
+    <tableColumn id="30" name="Hit" dataDxfId="18"/>
+    <tableColumn id="20" name="Dhit" dataDxfId="17"/>
+    <tableColumn id="19" name="Crt" dataDxfId="16"/>
+    <tableColumn id="12" name="Luk" dataDxfId="15"/>
+    <tableColumn id="32" name="Sum" dataDxfId="14">
       <calculatedColumnFormula>J4+K4+L4-100+M4+ SUM(O4:U4)*5+IF(ISNUMBER(Z4),Z4,0)+Y4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Range" dataDxfId="9"/>
-    <tableColumn id="27" name="Mov" dataDxfId="8"/>
-    <tableColumn id="24" name="~SkillMark" dataDxfId="7"/>
-    <tableColumn id="33" name="~SkillMark2" dataDxfId="6">
+    <tableColumn id="10" name="Range" dataDxfId="13"/>
+    <tableColumn id="27" name="Mov" dataDxfId="12"/>
+    <tableColumn id="24" name="~SkillMark" dataDxfId="11"/>
+    <tableColumn id="33" name="~SkillMark2" dataDxfId="10">
       <calculatedColumnFormula>IF(ISBLANK(AA4),0, LOOKUP(AA4,[1]Skill!$A:$A,[1]Skill!$X:$X)*AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="SkillId" dataDxfId="5"/>
-    <tableColumn id="14" name="Percent" dataDxfId="4"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="3"/>
+    <tableColumn id="13" name="SkillId" dataDxfId="9"/>
+    <tableColumn id="14" name="Percent" dataDxfId="8"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="7"/>
     <tableColumn id="26" name="JobId"/>
-    <tableColumn id="18" name="Icon" dataDxfId="2"/>
-    <tableColumn id="22" name="IsSpecial" dataDxfId="1"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="0"/>
+    <tableColumn id="18" name="Icon" dataDxfId="6"/>
+    <tableColumn id="22" name="IsSpecial" dataDxfId="5"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5634,13 +5684,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG127"/>
+  <dimension ref="A1:AG129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AC7" sqref="AC7"/>
+      <selection pane="bottomRight" activeCell="Q129" sqref="Q129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5964,7 +6014,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:33" hidden="1">
       <c r="A4">
         <v>52000001</v>
       </c>
@@ -6160,7 +6210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:33" hidden="1">
       <c r="A6">
         <v>52000003</v>
       </c>
@@ -6356,7 +6406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:33" hidden="1">
       <c r="A8">
         <v>52000005</v>
       </c>
@@ -6454,7 +6504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:33" hidden="1">
       <c r="A9">
         <v>52000006</v>
       </c>
@@ -6552,7 +6602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:33" hidden="1">
       <c r="A10">
         <v>52000007</v>
       </c>
@@ -6650,7 +6700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:33">
+    <row r="11" spans="1:33" hidden="1">
       <c r="A11">
         <v>52000008</v>
       </c>
@@ -7456,7 +7506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:33">
+    <row r="19" spans="1:33" hidden="1">
       <c r="A19">
         <v>52000016</v>
       </c>
@@ -7662,7 +7712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:33">
+    <row r="21" spans="1:33" hidden="1">
       <c r="A21">
         <v>52000018</v>
       </c>
@@ -7760,7 +7810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:33">
+    <row r="22" spans="1:33" hidden="1">
       <c r="A22">
         <v>52000019</v>
       </c>
@@ -7956,7 +8006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:33">
+    <row r="24" spans="1:33" hidden="1">
       <c r="A24">
         <v>52000021</v>
       </c>
@@ -8054,7 +8104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:33">
+    <row r="25" spans="1:33" hidden="1">
       <c r="A25">
         <v>52000022</v>
       </c>
@@ -8152,7 +8202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:33">
+    <row r="26" spans="1:33" hidden="1">
       <c r="A26">
         <v>52000023</v>
       </c>
@@ -8252,7 +8302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:33">
+    <row r="27" spans="1:33" hidden="1">
       <c r="A27">
         <v>52000024</v>
       </c>
@@ -8356,7 +8406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:33">
+    <row r="28" spans="1:33" hidden="1">
       <c r="A28">
         <v>52000025</v>
       </c>
@@ -8458,7 +8508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:33">
+    <row r="29" spans="1:33" hidden="1">
       <c r="A29">
         <v>52000026</v>
       </c>
@@ -8560,7 +8610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:33">
+    <row r="30" spans="1:33" hidden="1">
       <c r="A30">
         <v>52000027</v>
       </c>
@@ -8662,7 +8712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:33">
+    <row r="31" spans="1:33" hidden="1">
       <c r="A31">
         <v>52000028</v>
       </c>
@@ -8764,7 +8814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:33">
+    <row r="32" spans="1:33" hidden="1">
       <c r="A32">
         <v>52000029</v>
       </c>
@@ -8866,7 +8916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:33">
+    <row r="33" spans="1:33" hidden="1">
       <c r="A33">
         <v>52000030</v>
       </c>
@@ -8968,7 +9018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:33">
+    <row r="34" spans="1:33" hidden="1">
       <c r="A34">
         <v>52000031</v>
       </c>
@@ -9070,7 +9120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:33">
+    <row r="35" spans="1:33" hidden="1">
       <c r="A35">
         <v>52000032</v>
       </c>
@@ -10062,7 +10112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:33">
+    <row r="45" spans="1:33" hidden="1">
       <c r="A45">
         <v>52000042</v>
       </c>
@@ -10162,7 +10212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:33">
+    <row r="46" spans="1:33" hidden="1">
       <c r="A46">
         <v>52000043</v>
       </c>
@@ -10264,7 +10314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:33">
+    <row r="47" spans="1:33" hidden="1">
       <c r="A47">
         <v>52000044</v>
       </c>
@@ -10462,7 +10512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:33">
+    <row r="49" spans="1:33" hidden="1">
       <c r="A49">
         <v>52000046</v>
       </c>
@@ -10756,7 +10806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:33">
+    <row r="52" spans="1:33" hidden="1">
       <c r="A52">
         <v>52000049</v>
       </c>
@@ -10852,7 +10902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:33">
+    <row r="53" spans="1:33" hidden="1">
       <c r="A53">
         <v>52000050</v>
       </c>
@@ -10948,7 +10998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:33">
+    <row r="54" spans="1:33" hidden="1">
       <c r="A54">
         <v>52000051</v>
       </c>
@@ -11046,7 +11096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:33">
+    <row r="55" spans="1:33" hidden="1">
       <c r="A55">
         <v>52000052</v>
       </c>
@@ -11338,7 +11388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:33">
+    <row r="58" spans="1:33" hidden="1">
       <c r="A58">
         <v>52000055</v>
       </c>
@@ -11436,7 +11486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:33">
+    <row r="59" spans="1:33" hidden="1">
       <c r="A59">
         <v>52000056</v>
       </c>
@@ -11534,7 +11584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:33">
+    <row r="60" spans="1:33" hidden="1">
       <c r="A60">
         <v>52000057</v>
       </c>
@@ -11630,7 +11680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:33">
+    <row r="61" spans="1:33" hidden="1">
       <c r="A61">
         <v>52000058</v>
       </c>
@@ -11732,7 +11782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:33">
+    <row r="62" spans="1:33" hidden="1">
       <c r="A62">
         <v>52000059</v>
       </c>
@@ -11836,7 +11886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:33">
+    <row r="63" spans="1:33" hidden="1">
       <c r="A63">
         <v>52000060</v>
       </c>
@@ -11936,7 +11986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:33">
+    <row r="64" spans="1:33" hidden="1">
       <c r="A64">
         <v>52000061</v>
       </c>
@@ -12036,7 +12086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:33">
+    <row r="65" spans="1:33" hidden="1">
       <c r="A65">
         <v>52000062</v>
       </c>
@@ -12138,7 +12188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:33">
+    <row r="66" spans="1:33" hidden="1">
       <c r="A66">
         <v>52000063</v>
       </c>
@@ -12236,7 +12286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:33">
+    <row r="67" spans="1:33" hidden="1">
       <c r="A67">
         <v>52000064</v>
       </c>
@@ -12331,7 +12381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:33">
+    <row r="68" spans="1:33" hidden="1">
       <c r="A68">
         <v>52000065</v>
       </c>
@@ -12525,7 +12575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:33">
+    <row r="70" spans="1:33" hidden="1">
       <c r="A70">
         <v>52000067</v>
       </c>
@@ -12717,7 +12767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:33">
+    <row r="72" spans="1:33" hidden="1">
       <c r="A72">
         <v>52000069</v>
       </c>
@@ -12912,7 +12962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:33">
+    <row r="74" spans="1:33" hidden="1">
       <c r="A74">
         <v>52000071</v>
       </c>
@@ -13116,7 +13166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:33">
+    <row r="76" spans="1:33" hidden="1">
       <c r="A76">
         <v>52000073</v>
       </c>
@@ -13318,7 +13368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:33">
+    <row r="78" spans="1:33" hidden="1">
       <c r="A78">
         <v>52000075</v>
       </c>
@@ -13420,7 +13470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:33">
+    <row r="79" spans="1:33" hidden="1">
       <c r="A79">
         <v>52000076</v>
       </c>
@@ -13522,7 +13572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:33">
+    <row r="80" spans="1:33" hidden="1">
       <c r="A80">
         <v>52000077</v>
       </c>
@@ -13624,7 +13674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:33">
+    <row r="81" spans="1:33" hidden="1">
       <c r="A81">
         <v>52000078</v>
       </c>
@@ -13828,7 +13878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:33">
+    <row r="83" spans="1:33" hidden="1">
       <c r="A83">
         <v>52000080</v>
       </c>
@@ -14032,7 +14082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:33">
+    <row r="85" spans="1:33" hidden="1">
       <c r="A85">
         <v>52000082</v>
       </c>
@@ -14128,7 +14178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:33">
+    <row r="86" spans="1:33" hidden="1">
       <c r="A86">
         <v>52000083</v>
       </c>
@@ -14226,7 +14276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:33">
+    <row r="87" spans="1:33" hidden="1">
       <c r="A87">
         <v>52000084</v>
       </c>
@@ -14324,7 +14374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:33">
+    <row r="88" spans="1:33" hidden="1">
       <c r="A88">
         <v>52000085</v>
       </c>
@@ -14420,7 +14470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:33">
+    <row r="89" spans="1:33" hidden="1">
       <c r="A89">
         <v>52000086</v>
       </c>
@@ -14524,7 +14574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:33">
+    <row r="90" spans="1:33" hidden="1">
       <c r="A90">
         <v>52000087</v>
       </c>
@@ -14628,7 +14678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:33">
+    <row r="91" spans="1:33" hidden="1">
       <c r="A91">
         <v>52000088</v>
       </c>
@@ -14726,7 +14776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:33">
+    <row r="92" spans="1:33" hidden="1">
       <c r="A92">
         <v>52000089</v>
       </c>
@@ -14824,7 +14874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:33">
+    <row r="93" spans="1:33" hidden="1">
       <c r="A93">
         <v>52000090</v>
       </c>
@@ -14922,7 +14972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:33">
+    <row r="94" spans="1:33" hidden="1">
       <c r="A94">
         <v>52000091</v>
       </c>
@@ -15128,7 +15178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:33">
+    <row r="96" spans="1:33" hidden="1">
       <c r="A96">
         <v>52000093</v>
       </c>
@@ -15226,7 +15276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:33">
+    <row r="97" spans="1:33" hidden="1">
       <c r="A97">
         <v>52000094</v>
       </c>
@@ -15324,7 +15374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:33">
+    <row r="98" spans="1:33" hidden="1">
       <c r="A98">
         <v>52000095</v>
       </c>
@@ -15426,7 +15476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:33">
+    <row r="99" spans="1:33" hidden="1">
       <c r="A99">
         <v>52000096</v>
       </c>
@@ -15632,7 +15682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:33">
+    <row r="101" spans="1:33" hidden="1">
       <c r="A101">
         <v>52000098</v>
       </c>
@@ -15830,7 +15880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:33">
+    <row r="103" spans="1:33" hidden="1">
       <c r="A103">
         <v>52000100</v>
       </c>
@@ -16036,7 +16086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:33">
+    <row r="105" spans="1:33" hidden="1">
       <c r="A105">
         <v>52000102</v>
       </c>
@@ -16236,7 +16286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:33">
+    <row r="107" spans="1:33" hidden="1">
       <c r="A107">
         <v>52000104</v>
       </c>
@@ -16640,7 +16690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:33">
+    <row r="111" spans="1:33" hidden="1">
       <c r="A111">
         <v>52000108</v>
       </c>
@@ -16838,7 +16888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:33">
+    <row r="113" spans="1:33" hidden="1">
       <c r="A113">
         <v>52000110</v>
       </c>
@@ -16940,7 +16990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:33">
+    <row r="114" spans="1:33" hidden="1">
       <c r="A114">
         <v>52000111</v>
       </c>
@@ -17038,7 +17088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:33">
+    <row r="115" spans="1:33" hidden="1">
       <c r="A115">
         <v>52000112</v>
       </c>
@@ -17440,7 +17490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:33">
+    <row r="119" spans="1:33" hidden="1">
       <c r="A119">
         <v>52000116</v>
       </c>
@@ -17540,7 +17590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:33">
+    <row r="120" spans="1:33" hidden="1">
       <c r="A120">
         <v>52000117</v>
       </c>
@@ -17642,7 +17692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:33">
+    <row r="121" spans="1:33" hidden="1">
       <c r="A121">
         <v>52000118</v>
       </c>
@@ -17740,7 +17790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:33">
+    <row r="122" spans="1:33" hidden="1">
       <c r="A122">
         <v>52000119</v>
       </c>
@@ -17838,7 +17888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:33">
+    <row r="123" spans="1:33" hidden="1">
       <c r="A123">
         <v>52000120</v>
       </c>
@@ -17936,7 +17986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:33">
+    <row r="124" spans="1:33" hidden="1">
       <c r="A124">
         <v>52000121</v>
       </c>
@@ -18034,7 +18084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:33">
+    <row r="125" spans="1:33" hidden="1">
       <c r="A125">
         <v>52000122</v>
       </c>
@@ -18132,7 +18182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:33">
+    <row r="126" spans="1:33" hidden="1">
       <c r="A126">
         <v>52000123</v>
       </c>
@@ -18230,7 +18280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:33">
+    <row r="127" spans="1:33" hidden="1">
       <c r="A127">
         <v>52000124</v>
       </c>
@@ -18325,6 +18375,202 @@
         <v>0</v>
       </c>
       <c r="AG127" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:33">
+      <c r="A128">
+        <v>52000125</v>
+      </c>
+      <c r="B128" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="C128" s="15" t="s">
+        <v>376</v>
+      </c>
+      <c r="D128" s="42"/>
+      <c r="E128" s="15">
+        <v>2</v>
+      </c>
+      <c r="F128" s="15">
+        <v>100</v>
+      </c>
+      <c r="G128" s="15">
+        <v>0</v>
+      </c>
+      <c r="H128" s="41">
+        <f t="shared" ref="H128" si="11">IF(AND(V128&gt;=13,V128&lt;=16),5,IF(AND(V128&gt;=9,V128&lt;=12),4,IF(AND(V128&gt;=5,V128&lt;=8),3,IF(AND(V128&gt;=1,V128&lt;=4),2,IF(AND(V128&gt;=-3,V128&lt;=0),1,IF(AND(V128&gt;=-5,V128&lt;=-4),0,6))))))</f>
+        <v>1</v>
+      </c>
+      <c r="I128" s="15">
+        <v>2</v>
+      </c>
+      <c r="J128" s="16">
+        <v>90</v>
+      </c>
+      <c r="K128" s="16">
+        <v>0</v>
+      </c>
+      <c r="L128" s="7">
+        <v>0</v>
+      </c>
+      <c r="M128" s="14">
+        <v>5</v>
+      </c>
+      <c r="N128" s="8">
+        <v>3</v>
+      </c>
+      <c r="O128" s="8">
+        <v>0</v>
+      </c>
+      <c r="P128" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q128" s="8">
+        <v>0</v>
+      </c>
+      <c r="R128" s="8">
+        <v>0</v>
+      </c>
+      <c r="S128" s="8">
+        <v>0</v>
+      </c>
+      <c r="T128" s="8">
+        <v>1</v>
+      </c>
+      <c r="U128" s="8">
+        <v>0</v>
+      </c>
+      <c r="V128" s="10">
+        <f t="shared" ref="V128" si="12">J128+K128+L128-100+M128+ SUM(O128:U128)*5+IF(ISNUMBER(Z128),Z128,0)+Y128</f>
+        <v>0</v>
+      </c>
+      <c r="W128" s="8">
+        <v>10</v>
+      </c>
+      <c r="X128" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y128" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z128" s="10">
+        <f>IF(ISBLANK(AA128),0, LOOKUP(AA128,[1]Skill!$A:$A,[1]Skill!$X:$X)*AB128/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AA128" s="15"/>
+      <c r="AB128" s="15"/>
+      <c r="AC128" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD128" s="15">
+        <v>11000005</v>
+      </c>
+      <c r="AE128" s="17">
+        <v>125</v>
+      </c>
+      <c r="AF128" s="26">
+        <v>0</v>
+      </c>
+      <c r="AG128" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:33">
+      <c r="A129">
+        <v>52000126</v>
+      </c>
+      <c r="B129" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="C129" s="15" t="s">
+        <v>379</v>
+      </c>
+      <c r="D129" s="42"/>
+      <c r="E129" s="15">
+        <v>3</v>
+      </c>
+      <c r="F129" s="15">
+        <v>100</v>
+      </c>
+      <c r="G129" s="15">
+        <v>0</v>
+      </c>
+      <c r="H129" s="41">
+        <f t="shared" ref="H129" si="13">IF(AND(V129&gt;=13,V129&lt;=16),5,IF(AND(V129&gt;=9,V129&lt;=12),4,IF(AND(V129&gt;=5,V129&lt;=8),3,IF(AND(V129&gt;=1,V129&lt;=4),2,IF(AND(V129&gt;=-3,V129&lt;=0),1,IF(AND(V129&gt;=-5,V129&lt;=-4),0,6))))))</f>
+        <v>2</v>
+      </c>
+      <c r="I129" s="15">
+        <v>3</v>
+      </c>
+      <c r="J129" s="16">
+        <v>90</v>
+      </c>
+      <c r="K129" s="16">
+        <v>0</v>
+      </c>
+      <c r="L129" s="43">
+        <v>0</v>
+      </c>
+      <c r="M129" s="14">
+        <v>2</v>
+      </c>
+      <c r="N129" s="8">
+        <v>4</v>
+      </c>
+      <c r="O129" s="8">
+        <v>0</v>
+      </c>
+      <c r="P129" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q129" s="8">
+        <v>1</v>
+      </c>
+      <c r="R129" s="8">
+        <v>1</v>
+      </c>
+      <c r="S129" s="8">
+        <v>0</v>
+      </c>
+      <c r="T129" s="8">
+        <v>0</v>
+      </c>
+      <c r="U129" s="8">
+        <v>0</v>
+      </c>
+      <c r="V129" s="10">
+        <f t="shared" ref="V129" si="14">J129+K129+L129-100+M129+ SUM(O129:U129)*5+IF(ISNUMBER(Z129),Z129,0)+Y129</f>
+        <v>2</v>
+      </c>
+      <c r="W129" s="8">
+        <v>10</v>
+      </c>
+      <c r="X129" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y129" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z129" s="10">
+        <f>IF(ISBLANK(AA129),0, LOOKUP(AA129,[1]Skill!$A:$A,[1]Skill!$X:$X)*AB129/100)</f>
+        <v>0</v>
+      </c>
+      <c r="AA129" s="15"/>
+      <c r="AB129" s="15"/>
+      <c r="AC129" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD129" s="15">
+        <v>11000005</v>
+      </c>
+      <c r="AE129" s="17">
+        <v>126</v>
+      </c>
+      <c r="AF129" s="26">
+        <v>0</v>
+      </c>
+      <c r="AG129" s="15">
         <v>1</v>
       </c>
     </row>
@@ -18523,37 +18769,37 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H124">
-    <cfRule type="cellIs" dxfId="86" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="12" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="13" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="14" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="87" priority="14" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="82" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="6" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="8" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="9" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="10" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V4:V127">
+  <conditionalFormatting sqref="V4:V129">
     <cfRule type="colorScale" priority="95">
       <colorScale>
         <cfvo type="min"/>
@@ -18565,21 +18811,21 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H125:H127">
-    <cfRule type="cellIs" dxfId="77" priority="1" operator="equal">
+  <conditionalFormatting sqref="H125:H129">
+    <cfRule type="cellIs" dxfId="81" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="78" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V125:V127">
+  <conditionalFormatting sqref="V125:V129">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -19028,19 +19274,19 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="38" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="6" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
skill can do with the player use card event now
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Weapon.xlsx
+++ b/ConfigData/Xlsx/Weapon.xlsx
@@ -2270,138 +2270,6 @@
   <dxfs count="87">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9148C8"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -3003,6 +2871,44 @@
         <name val="宋体"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3635,6 +3541,100 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF9148C8"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B0F0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -5299,7 +5299,7 @@
             <v>55990106</v>
           </cell>
           <cell r="X206">
-            <v>40</v>
+            <v>80</v>
           </cell>
         </row>
       </sheetData>
@@ -5310,102 +5310,102 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AG130" totalsRowShown="0" dataDxfId="86" tableBorderDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AG130" totalsRowShown="0" dataDxfId="73" tableBorderDxfId="72">
   <autoFilter ref="A3:AG130"/>
   <sortState ref="A4:AF124">
     <sortCondition ref="A3:A124"/>
   </sortState>
   <tableColumns count="33">
-    <tableColumn id="1" name="Id" dataDxfId="84"/>
-    <tableColumn id="2" name="Name" dataDxfId="83"/>
-    <tableColumn id="3" name="Ename" dataDxfId="82"/>
-    <tableColumn id="4" name="Remark" dataDxfId="81"/>
-    <tableColumn id="5" name="Star" dataDxfId="80"/>
-    <tableColumn id="6" name="Type" dataDxfId="79"/>
-    <tableColumn id="7" name="Attr" dataDxfId="78"/>
-    <tableColumn id="34" name="Quality" dataDxfId="77">
+    <tableColumn id="1" name="Id" dataDxfId="71"/>
+    <tableColumn id="2" name="Name" dataDxfId="70"/>
+    <tableColumn id="3" name="Ename" dataDxfId="69"/>
+    <tableColumn id="4" name="Remark" dataDxfId="68"/>
+    <tableColumn id="5" name="Star" dataDxfId="67"/>
+    <tableColumn id="6" name="Type" dataDxfId="66"/>
+    <tableColumn id="7" name="Attr" dataDxfId="65"/>
+    <tableColumn id="34" name="Quality" dataDxfId="64">
       <calculatedColumnFormula>IF(AND(V4&gt;=13,V4&lt;=16),5,IF(AND(V4&gt;=9,V4&lt;=12),4,IF(AND(V4&gt;=5,V4&lt;=8),3,IF(AND(V4&gt;=1,V4&lt;=4),2,IF(AND(V4&gt;=-3,V4&lt;=0),1,IF(AND(V4&gt;=-5,V4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Cost" dataDxfId="76"/>
-    <tableColumn id="8" name="AtkP" dataDxfId="75"/>
-    <tableColumn id="9" name="PArmor" dataDxfId="74"/>
-    <tableColumn id="17" name="MArmor" dataDxfId="73"/>
-    <tableColumn id="25" name="Modify" dataDxfId="72"/>
-    <tableColumn id="27" name="Dura" dataDxfId="71"/>
-    <tableColumn id="20" name="Def" dataDxfId="70"/>
-    <tableColumn id="21" name="Mag" dataDxfId="69"/>
-    <tableColumn id="29" name="Spd" dataDxfId="68"/>
-    <tableColumn id="30" name="Hit" dataDxfId="67"/>
-    <tableColumn id="19" name="Dhit" dataDxfId="66"/>
-    <tableColumn id="12" name="Crt" dataDxfId="65"/>
-    <tableColumn id="11" name="Luk" dataDxfId="64"/>
-    <tableColumn id="32" name="Sum" dataDxfId="63">
+    <tableColumn id="15" name="Cost" dataDxfId="63"/>
+    <tableColumn id="8" name="AtkP" dataDxfId="62"/>
+    <tableColumn id="9" name="PArmor" dataDxfId="61"/>
+    <tableColumn id="17" name="MArmor" dataDxfId="60"/>
+    <tableColumn id="25" name="Modify" dataDxfId="59"/>
+    <tableColumn id="27" name="Dura" dataDxfId="58"/>
+    <tableColumn id="20" name="Def" dataDxfId="57"/>
+    <tableColumn id="21" name="Mag" dataDxfId="56"/>
+    <tableColumn id="29" name="Spd" dataDxfId="55"/>
+    <tableColumn id="30" name="Hit" dataDxfId="54"/>
+    <tableColumn id="19" name="Dhit" dataDxfId="53"/>
+    <tableColumn id="12" name="Crt" dataDxfId="52"/>
+    <tableColumn id="11" name="Luk" dataDxfId="51"/>
+    <tableColumn id="32" name="Sum" dataDxfId="50">
       <calculatedColumnFormula>J4+K4+L4-100+M4+ SUM(O4:U4)*5+IF(ISNUMBER(Z4),Z4,0)+Y4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Range" dataDxfId="62"/>
-    <tableColumn id="31" name="Mov" dataDxfId="61"/>
-    <tableColumn id="24" name="~SkillMark" dataDxfId="60"/>
-    <tableColumn id="33" name="~SkillMark2" dataDxfId="59">
+    <tableColumn id="10" name="Range" dataDxfId="49"/>
+    <tableColumn id="31" name="Mov" dataDxfId="48"/>
+    <tableColumn id="24" name="~SkillMark" dataDxfId="47"/>
+    <tableColumn id="33" name="~SkillMark2" dataDxfId="46">
       <calculatedColumnFormula>IF(ISBLANK(AA4),0, LOOKUP(AA4,[1]Skill!$A:$A,[1]Skill!$X:$X)*AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="SkillId" dataDxfId="58"/>
-    <tableColumn id="14" name="Percent" dataDxfId="57"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="56"/>
-    <tableColumn id="26" name="JobId" dataDxfId="55"/>
-    <tableColumn id="18" name="Icon" dataDxfId="54"/>
-    <tableColumn id="22" name="IsSpecial" dataDxfId="53"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="52"/>
+    <tableColumn id="13" name="SkillId" dataDxfId="45"/>
+    <tableColumn id="14" name="Percent" dataDxfId="44"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="43"/>
+    <tableColumn id="26" name="JobId" dataDxfId="42"/>
+    <tableColumn id="18" name="Icon" dataDxfId="41"/>
+    <tableColumn id="22" name="IsSpecial" dataDxfId="40"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AG4" totalsRowShown="0" dataDxfId="51" tableBorderDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AG4" totalsRowShown="0" dataDxfId="33" tableBorderDxfId="32">
   <autoFilter ref="A3:AG4"/>
   <sortState ref="A4:W130">
     <sortCondition ref="A3:A130"/>
   </sortState>
   <tableColumns count="33">
-    <tableColumn id="1" name="Id" dataDxfId="49"/>
-    <tableColumn id="2" name="Name" dataDxfId="48"/>
-    <tableColumn id="3" name="Ename" dataDxfId="47"/>
-    <tableColumn id="4" name="Remark" dataDxfId="46"/>
-    <tableColumn id="5" name="Star" dataDxfId="45"/>
-    <tableColumn id="6" name="Type" dataDxfId="44"/>
-    <tableColumn id="7" name="Attr" dataDxfId="43"/>
-    <tableColumn id="34" name="Quality" dataDxfId="42">
+    <tableColumn id="1" name="Id" dataDxfId="31"/>
+    <tableColumn id="2" name="Name" dataDxfId="30"/>
+    <tableColumn id="3" name="Ename" dataDxfId="29"/>
+    <tableColumn id="4" name="Remark" dataDxfId="28"/>
+    <tableColumn id="5" name="Star" dataDxfId="27"/>
+    <tableColumn id="6" name="Type" dataDxfId="26"/>
+    <tableColumn id="7" name="Attr" dataDxfId="25"/>
+    <tableColumn id="34" name="Quality" dataDxfId="24">
       <calculatedColumnFormula>IF(AND(V4&gt;=13,V4&lt;=16),5,IF(AND(V4&gt;=9,V4&lt;=12),4,IF(AND(V4&gt;=5,V4&lt;=8),3,IF(AND(V4&gt;=1,V4&lt;=4),2,IF(AND(V4&gt;=-3,V4&lt;=0),1,IF(AND(V4&gt;=-5,V4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Cost" dataDxfId="41"/>
-    <tableColumn id="8" name="AtkP" dataDxfId="40"/>
-    <tableColumn id="9" name="PArmor" dataDxfId="39"/>
-    <tableColumn id="17" name="MArmor" dataDxfId="38"/>
-    <tableColumn id="25" name="Modify" dataDxfId="37"/>
-    <tableColumn id="31" name="Dura" dataDxfId="36"/>
-    <tableColumn id="11" name="Def" dataDxfId="35"/>
-    <tableColumn id="21" name="Mag" dataDxfId="34"/>
-    <tableColumn id="29" name="Spd" dataDxfId="33"/>
-    <tableColumn id="30" name="Hit" dataDxfId="32"/>
-    <tableColumn id="20" name="Dhit" dataDxfId="31"/>
-    <tableColumn id="19" name="Crt" dataDxfId="30"/>
-    <tableColumn id="12" name="Luk" dataDxfId="29"/>
-    <tableColumn id="32" name="Sum" dataDxfId="28">
+    <tableColumn id="15" name="Cost" dataDxfId="23"/>
+    <tableColumn id="8" name="AtkP" dataDxfId="22"/>
+    <tableColumn id="9" name="PArmor" dataDxfId="21"/>
+    <tableColumn id="17" name="MArmor" dataDxfId="20"/>
+    <tableColumn id="25" name="Modify" dataDxfId="19"/>
+    <tableColumn id="31" name="Dura" dataDxfId="18"/>
+    <tableColumn id="11" name="Def" dataDxfId="17"/>
+    <tableColumn id="21" name="Mag" dataDxfId="16"/>
+    <tableColumn id="29" name="Spd" dataDxfId="15"/>
+    <tableColumn id="30" name="Hit" dataDxfId="14"/>
+    <tableColumn id="20" name="Dhit" dataDxfId="13"/>
+    <tableColumn id="19" name="Crt" dataDxfId="12"/>
+    <tableColumn id="12" name="Luk" dataDxfId="11"/>
+    <tableColumn id="32" name="Sum" dataDxfId="10">
       <calculatedColumnFormula>J4+K4+L4-100+M4+ SUM(O4:U4)*5+IF(ISNUMBER(Z4),Z4,0)+Y4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Range" dataDxfId="27"/>
-    <tableColumn id="27" name="Mov" dataDxfId="26"/>
-    <tableColumn id="24" name="~SkillMark" dataDxfId="25"/>
-    <tableColumn id="33" name="~SkillMark2" dataDxfId="24">
+    <tableColumn id="10" name="Range" dataDxfId="9"/>
+    <tableColumn id="27" name="Mov" dataDxfId="8"/>
+    <tableColumn id="24" name="~SkillMark" dataDxfId="7"/>
+    <tableColumn id="33" name="~SkillMark2" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(AA4),0, LOOKUP(AA4,[1]Skill!$A:$A,[1]Skill!$X:$X)*AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="SkillId" dataDxfId="23"/>
-    <tableColumn id="14" name="Percent" dataDxfId="22"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="21"/>
+    <tableColumn id="13" name="SkillId" dataDxfId="5"/>
+    <tableColumn id="14" name="Percent" dataDxfId="4"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="3"/>
     <tableColumn id="26" name="JobId"/>
-    <tableColumn id="18" name="Icon" dataDxfId="20"/>
-    <tableColumn id="22" name="IsSpecial" dataDxfId="19"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="18"/>
+    <tableColumn id="18" name="Icon" dataDxfId="2"/>
+    <tableColumn id="22" name="IsSpecial" dataDxfId="1"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5735,10 +5735,10 @@
   <dimension ref="A1:AG130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B103" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="M130" sqref="M130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6128,7 +6128,7 @@
         <v>0</v>
       </c>
       <c r="V4" s="10">
-        <f>J4+K4+L4-100+M4+ SUM(O4:U4)*5+IF(ISNUMBER(Z4),Z4,0)+Y4</f>
+        <f t="shared" ref="V4:V35" si="1">J4+K4+L4-100+M4+ SUM(O4:U4)*5+IF(ISNUMBER(Z4),Z4,0)+Y4</f>
         <v>-5</v>
       </c>
       <c r="W4" s="8">
@@ -6226,7 +6226,7 @@
         <v>0</v>
       </c>
       <c r="V5" s="10">
-        <f>J5+K5+L5-100+M5+ SUM(O5:U5)*5+IF(ISNUMBER(Z5),Z5,0)+Y5</f>
+        <f t="shared" si="1"/>
         <v>-5</v>
       </c>
       <c r="W5" s="8">
@@ -6324,7 +6324,7 @@
         <v>0</v>
       </c>
       <c r="V6" s="10">
-        <f>J6+K6+L6-100+M6+ SUM(O6:U6)*5+IF(ISNUMBER(Z6),Z6,0)+Y6</f>
+        <f t="shared" si="1"/>
         <v>-5</v>
       </c>
       <c r="W6" s="8">
@@ -6422,7 +6422,7 @@
         <v>0</v>
       </c>
       <c r="V7" s="10">
-        <f>J7+K7+L7-100+M7+ SUM(O7:U7)*5+IF(ISNUMBER(Z7),Z7,0)+Y7</f>
+        <f t="shared" si="1"/>
         <v>-5</v>
       </c>
       <c r="W7" s="8">
@@ -6520,7 +6520,7 @@
         <v>0</v>
       </c>
       <c r="V8" s="18">
-        <f>J8+K8+L8-100+M8+ SUM(O8:U8)*5+IF(ISNUMBER(Z8),Z8,0)+Y8</f>
+        <f t="shared" si="1"/>
         <v>-5</v>
       </c>
       <c r="W8" s="8">
@@ -6618,7 +6618,7 @@
         <v>0</v>
       </c>
       <c r="V9" s="10">
-        <f>J9+K9+L9-100+M9+ SUM(O9:U9)*5+IF(ISNUMBER(Z9),Z9,0)+Y9</f>
+        <f t="shared" si="1"/>
         <v>-4</v>
       </c>
       <c r="W9" s="8">
@@ -6716,7 +6716,7 @@
         <v>0</v>
       </c>
       <c r="V10" s="10">
-        <f>J10+K10+L10-100+M10+ SUM(O10:U10)*5+IF(ISNUMBER(Z10),Z10,0)+Y10</f>
+        <f t="shared" si="1"/>
         <v>-5</v>
       </c>
       <c r="W10" s="8">
@@ -6814,7 +6814,7 @@
         <v>0</v>
       </c>
       <c r="V11" s="18">
-        <f>J11+K11+L11-100+M11+ SUM(O11:U11)*5+IF(ISNUMBER(Z11),Z11,0)+Y11</f>
+        <f t="shared" si="1"/>
         <v>-5</v>
       </c>
       <c r="W11" s="8">
@@ -6910,7 +6910,7 @@
         <v>0</v>
       </c>
       <c r="V12" s="18">
-        <f>J12+K12+L12-100+M12+ SUM(O12:U12)*5+IF(ISNUMBER(Z12),Z12,0)+Y12</f>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="W12" s="8">
@@ -7008,7 +7008,7 @@
         <v>0</v>
       </c>
       <c r="V13" s="10">
-        <f>J13+K13+L13-100+M13+ SUM(O13:U13)*5+IF(ISNUMBER(Z13),Z13,0)+Y13</f>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="W13" s="8">
@@ -7110,7 +7110,7 @@
         <v>0</v>
       </c>
       <c r="V14" s="18">
-        <f>J14+K14+L14-100+M14+ SUM(O14:U14)*5+IF(ISNUMBER(Z14),Z14,0)+Y14</f>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="W14" s="8">
@@ -7212,7 +7212,7 @@
         <v>0</v>
       </c>
       <c r="V15" s="10">
-        <f>J15+K15+L15-100+M15+ SUM(O15:U15)*5+IF(ISNUMBER(Z15),Z15,0)+Y15</f>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="W15" s="8">
@@ -7314,7 +7314,7 @@
         <v>0</v>
       </c>
       <c r="V16" s="10">
-        <f>J16+K16+L16-100+M16+ SUM(O16:U16)*5+IF(ISNUMBER(Z16),Z16,0)+Y16</f>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="W16" s="8">
@@ -7416,7 +7416,7 @@
         <v>0</v>
       </c>
       <c r="V17" s="18">
-        <f>J17+K17+L17-100+M17+ SUM(O17:U17)*5+IF(ISNUMBER(Z17),Z17,0)+Y17</f>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="W17" s="8">
@@ -7518,7 +7518,7 @@
         <v>0</v>
       </c>
       <c r="V18" s="10">
-        <f>J18+K18+L18-100+M18+ SUM(O18:U18)*5+IF(ISNUMBER(Z18),Z18,0)+Y18</f>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="W18" s="8">
@@ -7596,7 +7596,7 @@
         <v>0</v>
       </c>
       <c r="N19" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O19" s="8">
         <v>0</v>
@@ -7620,7 +7620,7 @@
         <v>0</v>
       </c>
       <c r="V19" s="18">
-        <f>J19+K19+L19-100+M19+ SUM(O19:U19)*5+IF(ISNUMBER(Z19),Z19,0)+Y19</f>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="W19" s="8">
@@ -7722,7 +7722,7 @@
         <v>0</v>
       </c>
       <c r="V20" s="10">
-        <f>J20+K20+L20-100+M20+ SUM(O20:U20)*5+IF(ISNUMBER(Z20),Z20,0)+Y20</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="W20" s="8">
@@ -7826,7 +7826,7 @@
         <v>0</v>
       </c>
       <c r="V21" s="18">
-        <f>J21+K21+L21-100+M21+ SUM(O21:U21)*5+IF(ISNUMBER(Z21),Z21,0)+Y21</f>
+        <f t="shared" si="1"/>
         <v>-4</v>
       </c>
       <c r="W21" s="8">
@@ -7922,7 +7922,7 @@
         <v>0</v>
       </c>
       <c r="V22" s="10">
-        <f>J22+K22+L22-100+M22+ SUM(O22:U22)*5+IF(ISNUMBER(Z22),Z22,0)+Y22</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="W22" s="8">
@@ -8022,7 +8022,7 @@
         <v>0</v>
       </c>
       <c r="V23" s="10">
-        <f>J23+K23+L23-100+M23+ SUM(O23:U23)*5+IF(ISNUMBER(Z23),Z23,0)+Y23</f>
+        <f t="shared" si="1"/>
         <v>-5</v>
       </c>
       <c r="W23" s="8">
@@ -8120,7 +8120,7 @@
         <v>0</v>
       </c>
       <c r="V24" s="10">
-        <f>J24+K24+L24-100+M24+ SUM(O24:U24)*5+IF(ISNUMBER(Z24),Z24,0)+Y24</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="W24" s="8">
@@ -8218,7 +8218,7 @@
         <v>0</v>
       </c>
       <c r="V25" s="10">
-        <f>J25+K25+L25-100+M25+ SUM(O25:U25)*5+IF(ISNUMBER(Z25),Z25,0)+Y25</f>
+        <f t="shared" si="1"/>
         <v>-4</v>
       </c>
       <c r="W25" s="8">
@@ -8316,7 +8316,7 @@
         <v>0</v>
       </c>
       <c r="V26" s="10">
-        <f>J26+K26+L26-100+M26+ SUM(O26:U26)*5+IF(ISNUMBER(Z26),Z26,0)+Y26</f>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="W26" s="8">
@@ -8416,7 +8416,7 @@
         <v>0</v>
       </c>
       <c r="V27" s="10">
-        <f>J27+K27+L27-100+M27+ SUM(O27:U27)*5+IF(ISNUMBER(Z27),Z27,0)+Y27</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="W27" s="8">
@@ -8518,7 +8518,7 @@
         <v>0</v>
       </c>
       <c r="V28" s="18">
-        <f>J28+K28+L28-100+M28+ SUM(O28:U28)*5+IF(ISNUMBER(Z28),Z28,0)+Y28</f>
+        <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
       <c r="W28" s="8">
@@ -8622,7 +8622,7 @@
         <v>0</v>
       </c>
       <c r="V29" s="10">
-        <f>J29+K29+L29-100+M29+ SUM(O29:U29)*5+IF(ISNUMBER(Z29),Z29,0)+Y29</f>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="W29" s="8">
@@ -8724,7 +8724,7 @@
         <v>0</v>
       </c>
       <c r="V30" s="18">
-        <f>J30+K30+L30-100+M30+ SUM(O30:U30)*5+IF(ISNUMBER(Z30),Z30,0)+Y30</f>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="W30" s="8">
@@ -8826,7 +8826,7 @@
         <v>0</v>
       </c>
       <c r="V31" s="10">
-        <f>J31+K31+L31-100+M31+ SUM(O31:U31)*5+IF(ISNUMBER(Z31),Z31,0)+Y31</f>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="W31" s="8">
@@ -8928,7 +8928,7 @@
         <v>0</v>
       </c>
       <c r="V32" s="10">
-        <f>J32+K32+L32-100+M32+ SUM(O32:U32)*5+IF(ISNUMBER(Z32),Z32,0)+Y32</f>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="W32" s="8">
@@ -9030,7 +9030,7 @@
         <v>0</v>
       </c>
       <c r="V33" s="10">
-        <f>J33+K33+L33-100+M33+ SUM(O33:U33)*5+IF(ISNUMBER(Z33),Z33,0)+Y33</f>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="W33" s="8">
@@ -9132,7 +9132,7 @@
         <v>0</v>
       </c>
       <c r="V34" s="10">
-        <f>J34+K34+L34-100+M34+ SUM(O34:U34)*5+IF(ISNUMBER(Z34),Z34,0)+Y34</f>
+        <f t="shared" si="1"/>
         <v>-2</v>
       </c>
       <c r="W34" s="8">
@@ -9234,7 +9234,7 @@
         <v>0</v>
       </c>
       <c r="V35" s="18">
-        <f>J35+K35+L35-100+M35+ SUM(O35:U35)*5+IF(ISNUMBER(Z35),Z35,0)+Y35</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="W35" s="8">
@@ -9293,7 +9293,7 @@
         <v>1</v>
       </c>
       <c r="H36" s="4">
-        <f t="shared" ref="H36:H67" si="1">IF(AND(V36&gt;=13,V36&lt;=16),5,IF(AND(V36&gt;=9,V36&lt;=12),4,IF(AND(V36&gt;=5,V36&lt;=8),3,IF(AND(V36&gt;=1,V36&lt;=4),2,IF(AND(V36&gt;=-3,V36&lt;=0),1,IF(AND(V36&gt;=-5,V36&lt;=-4),0,6))))))</f>
+        <f t="shared" ref="H36:H67" si="2">IF(AND(V36&gt;=13,V36&lt;=16),5,IF(AND(V36&gt;=9,V36&lt;=12),4,IF(AND(V36&gt;=5,V36&lt;=8),3,IF(AND(V36&gt;=1,V36&lt;=4),2,IF(AND(V36&gt;=-3,V36&lt;=0),1,IF(AND(V36&gt;=-5,V36&lt;=-4),0,6))))))</f>
         <v>1</v>
       </c>
       <c r="I36" s="4">
@@ -9336,7 +9336,7 @@
         <v>0</v>
       </c>
       <c r="V36" s="10">
-        <f>J36+K36+L36-100+M36+ SUM(O36:U36)*5+IF(ISNUMBER(Z36),Z36,0)+Y36</f>
+        <f t="shared" ref="V36:V67" si="3">J36+K36+L36-100+M36+ SUM(O36:U36)*5+IF(ISNUMBER(Z36),Z36,0)+Y36</f>
         <v>0</v>
       </c>
       <c r="W36" s="8">
@@ -9389,7 +9389,7 @@
         <v>2</v>
       </c>
       <c r="H37" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I37" s="4">
@@ -9432,7 +9432,7 @@
         <v>0</v>
       </c>
       <c r="V37" s="10">
-        <f>J37+K37+L37-100+M37+ SUM(O37:U37)*5+IF(ISNUMBER(Z37),Z37,0)+Y37</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W37" s="8">
@@ -9487,7 +9487,7 @@
         <v>3</v>
       </c>
       <c r="H38" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I38" s="4">
@@ -9530,7 +9530,7 @@
         <v>0</v>
       </c>
       <c r="V38" s="10">
-        <f>J38+K38+L38-100+M38+ SUM(O38:U38)*5+IF(ISNUMBER(Z38),Z38,0)+Y38</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W38" s="8">
@@ -9585,7 +9585,7 @@
         <v>4</v>
       </c>
       <c r="H39" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I39" s="4">
@@ -9628,7 +9628,7 @@
         <v>0</v>
       </c>
       <c r="V39" s="10">
-        <f>J39+K39+L39-100+M39+ SUM(O39:U39)*5+IF(ISNUMBER(Z39),Z39,0)+Y39</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W39" s="8">
@@ -9683,7 +9683,7 @@
         <v>1</v>
       </c>
       <c r="H40" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I40" s="4">
@@ -9726,7 +9726,7 @@
         <v>0</v>
       </c>
       <c r="V40" s="10">
-        <f>J40+K40+L40-100+M40+ SUM(O40:U40)*5+IF(ISNUMBER(Z40),Z40,0)+Y40</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="W40" s="8">
@@ -9787,7 +9787,7 @@
         <v>5</v>
       </c>
       <c r="H41" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I41" s="4">
@@ -9830,7 +9830,7 @@
         <v>0</v>
       </c>
       <c r="V41" s="10">
-        <f>J41+K41+L41-100+M41+ SUM(O41:U41)*5+IF(ISNUMBER(Z41),Z41,0)+Y41</f>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
       <c r="W41" s="8">
@@ -9889,7 +9889,7 @@
         <v>5</v>
       </c>
       <c r="H42" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I42" s="4">
@@ -9932,7 +9932,7 @@
         <v>0</v>
       </c>
       <c r="V42" s="10">
-        <f>J42+K42+L42-100+M42+ SUM(O42:U42)*5+IF(ISNUMBER(Z42),Z42,0)+Y42</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W42" s="8">
@@ -9987,7 +9987,7 @@
         <v>6</v>
       </c>
       <c r="H43" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I43" s="4">
@@ -10030,7 +10030,7 @@
         <v>0</v>
       </c>
       <c r="V43" s="10">
-        <f>J43+K43+L43-100+M43+ SUM(O43:U43)*5+IF(ISNUMBER(Z43),Z43,0)+Y43</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W43" s="8">
@@ -10085,7 +10085,7 @@
         <v>0</v>
       </c>
       <c r="H44" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I44" s="4">
@@ -10128,7 +10128,7 @@
         <v>0</v>
       </c>
       <c r="V44" s="10">
-        <f>J44+K44+L44-100+M44+ SUM(O44:U44)*5+IF(ISNUMBER(Z44),Z44,0)+Y44</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W44" s="8">
@@ -10181,7 +10181,7 @@
         <v>0</v>
       </c>
       <c r="H45" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I45" s="4">
@@ -10224,7 +10224,7 @@
         <v>0</v>
       </c>
       <c r="V45" s="10">
-        <f>J45+K45+L45-100+M45+ SUM(O45:U45)*5+IF(ISNUMBER(Z45),Z45,0)+Y45</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W45" s="8">
@@ -10281,7 +10281,7 @@
         <v>0</v>
       </c>
       <c r="H46" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I46" s="4">
@@ -10324,7 +10324,7 @@
         <v>0</v>
       </c>
       <c r="V46" s="10">
-        <f>J46+K46+L46-100+M46+ SUM(O46:U46)*5+IF(ISNUMBER(Z46),Z46,0)+Y46</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="W46" s="8">
@@ -10383,7 +10383,7 @@
         <v>0</v>
       </c>
       <c r="H47" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I47" s="4">
@@ -10426,7 +10426,7 @@
         <v>0</v>
       </c>
       <c r="V47" s="10">
-        <f>J47+K47+L47-100+M47+ SUM(O47:U47)*5+IF(ISNUMBER(Z47),Z47,0)+Y47</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="W47" s="8">
@@ -10481,7 +10481,7 @@
         <v>0</v>
       </c>
       <c r="H48" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I48" s="4">
@@ -10524,7 +10524,7 @@
         <v>0</v>
       </c>
       <c r="V48" s="10">
-        <f>J48+K48+L48-100+M48+ SUM(O48:U48)*5+IF(ISNUMBER(Z48),Z48,0)+Y48</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="W48" s="8">
@@ -10581,7 +10581,7 @@
         <v>0</v>
       </c>
       <c r="H49" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I49" s="4">
@@ -10624,7 +10624,7 @@
         <v>0</v>
       </c>
       <c r="V49" s="10">
-        <f>J49+K49+L49-100+M49+ SUM(O49:U49)*5+IF(ISNUMBER(Z49),Z49,0)+Y49</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W49" s="8">
@@ -10677,7 +10677,7 @@
         <v>0</v>
       </c>
       <c r="H50" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I50" s="4">
@@ -10720,7 +10720,7 @@
         <v>0</v>
       </c>
       <c r="V50" s="10">
-        <f>J50+K50+L50-100+M50+ SUM(O50:U50)*5+IF(ISNUMBER(Z50),Z50,0)+Y50</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W50" s="8">
@@ -10773,7 +10773,7 @@
         <v>0</v>
       </c>
       <c r="H51" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I51" s="4">
@@ -10816,7 +10816,7 @@
         <v>0</v>
       </c>
       <c r="V51" s="10">
-        <f>J51+K51+L51-100+M51+ SUM(O51:U51)*5+IF(ISNUMBER(Z51),Z51,0)+Y51</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="W51" s="8">
@@ -10875,7 +10875,7 @@
         <v>0</v>
       </c>
       <c r="H52" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I52" s="4">
@@ -10918,7 +10918,7 @@
         <v>2</v>
       </c>
       <c r="V52" s="10">
-        <f>J52+K52+L52-100+M52+ SUM(O52:U52)*5+IF(ISNUMBER(Z52),Z52,0)+Y52</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W52" s="8">
@@ -10971,7 +10971,7 @@
         <v>0</v>
       </c>
       <c r="H53" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I53" s="4">
@@ -11014,7 +11014,7 @@
         <v>0</v>
       </c>
       <c r="V53" s="10">
-        <f>J53+K53+L53-100+M53+ SUM(O53:U53)*5+IF(ISNUMBER(Z53),Z53,0)+Y53</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W53" s="8">
@@ -11067,7 +11067,7 @@
         <v>0</v>
       </c>
       <c r="H54" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I54" s="4">
@@ -11110,7 +11110,7 @@
         <v>0</v>
       </c>
       <c r="V54" s="10">
-        <f>J54+K54+L54-100+M54+ SUM(O54:U54)*5+IF(ISNUMBER(Z54),Z54,0)+Y54</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="W54" s="8">
@@ -11167,7 +11167,7 @@
         <v>0</v>
       </c>
       <c r="H55" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I55" s="4">
@@ -11210,7 +11210,7 @@
         <v>0</v>
       </c>
       <c r="V55" s="10">
-        <f>J55+K55+L55-100+M55+ SUM(O55:U55)*5+IF(ISNUMBER(Z55),Z55,0)+Y55</f>
+        <f t="shared" si="3"/>
         <v>-2</v>
       </c>
       <c r="W55" s="8">
@@ -11263,7 +11263,7 @@
         <v>0</v>
       </c>
       <c r="H56" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I56" s="4">
@@ -11306,7 +11306,7 @@
         <v>0</v>
       </c>
       <c r="V56" s="10">
-        <f>J56+K56+L56-100+M56+ SUM(O56:U56)*5+IF(ISNUMBER(Z56),Z56,0)+Y56</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="W56" s="8">
@@ -11361,7 +11361,7 @@
         <v>0</v>
       </c>
       <c r="H57" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I57" s="4">
@@ -11404,7 +11404,7 @@
         <v>0</v>
       </c>
       <c r="V57" s="10">
-        <f>J57+K57+L57-100+M57+ SUM(O57:U57)*5+IF(ISNUMBER(Z57),Z57,0)+Y57</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W57" s="8">
@@ -11457,7 +11457,7 @@
         <v>0</v>
       </c>
       <c r="H58" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I58" s="4">
@@ -11500,7 +11500,7 @@
         <v>0</v>
       </c>
       <c r="V58" s="10">
-        <f>J58+K58+L58-100+M58+ SUM(O58:U58)*5+IF(ISNUMBER(Z58),Z58,0)+Y58</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="W58" s="8">
@@ -11555,7 +11555,7 @@
         <v>0</v>
       </c>
       <c r="H59" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I59" s="4">
@@ -11598,7 +11598,7 @@
         <v>0</v>
       </c>
       <c r="V59" s="10">
-        <f>J59+K59+L59-100+M59+ SUM(O59:U59)*5+IF(ISNUMBER(Z59),Z59,0)+Y59</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="W59" s="8">
@@ -11653,7 +11653,7 @@
         <v>0</v>
       </c>
       <c r="H60" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I60" s="4">
@@ -11696,7 +11696,7 @@
         <v>0</v>
       </c>
       <c r="V60" s="10">
-        <f>J60+K60+L60-100+M60+ SUM(O60:U60)*5+IF(ISNUMBER(Z60),Z60,0)+Y60</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="W60" s="8">
@@ -11751,7 +11751,7 @@
         <v>0</v>
       </c>
       <c r="H61" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I61" s="4">
@@ -11794,7 +11794,7 @@
         <v>0</v>
       </c>
       <c r="V61" s="10">
-        <f>J61+K61+L61-100+M61+ SUM(O61:U61)*5+IF(ISNUMBER(Z61),Z61,0)+Y61</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="W61" s="8">
@@ -11853,7 +11853,7 @@
         <v>0</v>
       </c>
       <c r="H62" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I62" s="4">
@@ -11896,7 +11896,7 @@
         <v>0</v>
       </c>
       <c r="V62" s="10">
-        <f>J62+K62+L62-100+M62+ SUM(O62:U62)*5+IF(ISNUMBER(Z62),Z62,0)+Y62</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="W62" s="8">
@@ -11955,7 +11955,7 @@
         <v>0</v>
       </c>
       <c r="H63" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I63" s="4">
@@ -11998,7 +11998,7 @@
         <v>0</v>
       </c>
       <c r="V63" s="10">
-        <f>J63+K63+L63-100+M63+ SUM(O63:U63)*5+IF(ISNUMBER(Z63),Z63,0)+Y63</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W63" s="8">
@@ -12055,7 +12055,7 @@
         <v>0</v>
       </c>
       <c r="H64" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I64" s="4">
@@ -12098,7 +12098,7 @@
         <v>0</v>
       </c>
       <c r="V64" s="10">
-        <f>J64+K64+L64-100+M64+ SUM(O64:U64)*5+IF(ISNUMBER(Z64),Z64,0)+Y64</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="W64" s="8">
@@ -12155,7 +12155,7 @@
         <v>0</v>
       </c>
       <c r="H65" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I65" s="4">
@@ -12198,7 +12198,7 @@
         <v>3</v>
       </c>
       <c r="V65" s="10">
-        <f>J65+K65+L65-100+M65+ SUM(O65:U65)*5+IF(ISNUMBER(Z65),Z65,0)+Y65</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="W65" s="8">
@@ -12259,7 +12259,7 @@
         <v>0</v>
       </c>
       <c r="H66" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I66" s="4">
@@ -12302,7 +12302,7 @@
         <v>0</v>
       </c>
       <c r="V66" s="10">
-        <f>J66+K66+L66-100+M66+ SUM(O66:U66)*5+IF(ISNUMBER(Z66),Z66,0)+Y66</f>
+        <f t="shared" si="3"/>
         <v>-3</v>
       </c>
       <c r="W66" s="8">
@@ -12355,7 +12355,7 @@
         <v>0</v>
       </c>
       <c r="H67" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I67" s="4">
@@ -12398,7 +12398,7 @@
         <v>0</v>
       </c>
       <c r="V67" s="10">
-        <f>J67+K67+L67-100+M67+ SUM(O67:U67)*5+IF(ISNUMBER(Z67),Z67,0)+Y67</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="W67" s="8">
@@ -12450,7 +12450,7 @@
         <v>0</v>
       </c>
       <c r="H68" s="4">
-        <f t="shared" ref="H68:H99" si="2">IF(AND(V68&gt;=13,V68&lt;=16),5,IF(AND(V68&gt;=9,V68&lt;=12),4,IF(AND(V68&gt;=5,V68&lt;=8),3,IF(AND(V68&gt;=1,V68&lt;=4),2,IF(AND(V68&gt;=-3,V68&lt;=0),1,IF(AND(V68&gt;=-5,V68&lt;=-4),0,6))))))</f>
+        <f t="shared" ref="H68:H99" si="4">IF(AND(V68&gt;=13,V68&lt;=16),5,IF(AND(V68&gt;=9,V68&lt;=12),4,IF(AND(V68&gt;=5,V68&lt;=8),3,IF(AND(V68&gt;=1,V68&lt;=4),2,IF(AND(V68&gt;=-3,V68&lt;=0),1,IF(AND(V68&gt;=-5,V68&lt;=-4),0,6))))))</f>
         <v>1</v>
       </c>
       <c r="I68" s="4">
@@ -12493,7 +12493,7 @@
         <v>0</v>
       </c>
       <c r="V68" s="10">
-        <f>J68+K68+L68-100+M68+ SUM(O68:U68)*5+IF(ISNUMBER(Z68),Z68,0)+Y68</f>
+        <f t="shared" ref="V68:V99" si="5">J68+K68+L68-100+M68+ SUM(O68:U68)*5+IF(ISNUMBER(Z68),Z68,0)+Y68</f>
         <v>-1</v>
       </c>
       <c r="W68" s="8">
@@ -12548,7 +12548,7 @@
         <v>0</v>
       </c>
       <c r="H69" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I69" s="4">
@@ -12591,7 +12591,7 @@
         <v>0</v>
       </c>
       <c r="V69" s="10">
-        <f>J69+K69+L69-100+M69+ SUM(O69:U69)*5+IF(ISNUMBER(Z69),Z69,0)+Y69</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W69" s="8">
@@ -12644,7 +12644,7 @@
         <v>0</v>
       </c>
       <c r="H70" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I70" s="4">
@@ -12687,7 +12687,7 @@
         <v>0</v>
       </c>
       <c r="V70" s="10">
-        <f>J70+K70+L70-100+M70+ SUM(O70:U70)*5+IF(ISNUMBER(Z70),Z70,0)+Y70</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W70" s="8">
@@ -12740,7 +12740,7 @@
         <v>0</v>
       </c>
       <c r="H71" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I71" s="4">
@@ -12783,7 +12783,7 @@
         <v>0</v>
       </c>
       <c r="V71" s="10">
-        <f>J71+K71+L71-100+M71+ SUM(O71:U71)*5+IF(ISNUMBER(Z71),Z71,0)+Y71</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W71" s="8">
@@ -12836,7 +12836,7 @@
         <v>0</v>
       </c>
       <c r="H72" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="I72" s="4">
@@ -12879,7 +12879,7 @@
         <v>0</v>
       </c>
       <c r="V72" s="10">
-        <f>J72+K72+L72-100+M72+ SUM(O72:U72)*5+IF(ISNUMBER(Z72),Z72,0)+Y72</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="W72" s="8">
@@ -12931,7 +12931,7 @@
         <v>0</v>
       </c>
       <c r="H73" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I73" s="4">
@@ -12974,7 +12974,7 @@
         <v>0</v>
       </c>
       <c r="V73" s="10">
-        <f>J73+K73+L73-100+M73+ SUM(O73:U73)*5+IF(ISNUMBER(Z73),Z73,0)+Y73</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W73" s="8">
@@ -13033,7 +13033,7 @@
         <v>0</v>
       </c>
       <c r="H74" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="I74" s="4">
@@ -13076,7 +13076,7 @@
         <v>0</v>
       </c>
       <c r="V74" s="10">
-        <f>J74+K74+L74-100+M74+ SUM(O74:U74)*5+IF(ISNUMBER(Z74),Z74,0)+Y74</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="W74" s="8">
@@ -13135,7 +13135,7 @@
         <v>0</v>
       </c>
       <c r="H75" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I75" s="4">
@@ -13178,7 +13178,7 @@
         <v>0</v>
       </c>
       <c r="V75" s="10">
-        <f>J75+K75+L75-100+M75+ SUM(O75:U75)*5+IF(ISNUMBER(Z75),Z75,0)+Y75</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W75" s="8">
@@ -13235,7 +13235,7 @@
         <v>0</v>
       </c>
       <c r="H76" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="I76" s="4">
@@ -13278,7 +13278,7 @@
         <v>0</v>
       </c>
       <c r="V76" s="10">
-        <f>J76+K76+L76-100+M76+ SUM(O76:U76)*5+IF(ISNUMBER(Z76),Z76,0)+Y76</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="W76" s="8">
@@ -13337,7 +13337,7 @@
         <v>0</v>
       </c>
       <c r="H77" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I77" s="4">
@@ -13380,7 +13380,7 @@
         <v>0</v>
       </c>
       <c r="V77" s="10">
-        <f>J77+K77+L77-100+M77+ SUM(O77:U77)*5+IF(ISNUMBER(Z77),Z77,0)+Y77</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W77" s="8">
@@ -13439,7 +13439,7 @@
         <v>0</v>
       </c>
       <c r="H78" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="I78" s="4">
@@ -13482,7 +13482,7 @@
         <v>0</v>
       </c>
       <c r="V78" s="10">
-        <f>J78+K78+L78-100+M78+ SUM(O78:U78)*5+IF(ISNUMBER(Z78),Z78,0)+Y78</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="W78" s="8">
@@ -13541,7 +13541,7 @@
         <v>0</v>
       </c>
       <c r="H79" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="I79" s="4">
@@ -13584,7 +13584,7 @@
         <v>0</v>
       </c>
       <c r="V79" s="10">
-        <f>J79+K79+L79-100+M79+ SUM(O79:U79)*5+IF(ISNUMBER(Z79),Z79,0)+Y79</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="W79" s="8">
@@ -13643,7 +13643,7 @@
         <v>0</v>
       </c>
       <c r="H80" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="I80" s="4">
@@ -13686,7 +13686,7 @@
         <v>0</v>
       </c>
       <c r="V80" s="10">
-        <f>J80+K80+L80-100+M80+ SUM(O80:U80)*5+IF(ISNUMBER(Z80),Z80,0)+Y80</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="W80" s="8">
@@ -13745,7 +13745,7 @@
         <v>0</v>
       </c>
       <c r="H81" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="I81" s="4">
@@ -13788,7 +13788,7 @@
         <v>0</v>
       </c>
       <c r="V81" s="10">
-        <f>J81+K81+L81-100+M81+ SUM(O81:U81)*5+IF(ISNUMBER(Z81),Z81,0)+Y81</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="W81" s="8">
@@ -13847,7 +13847,7 @@
         <v>0</v>
       </c>
       <c r="H82" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I82" s="4">
@@ -13890,7 +13890,7 @@
         <v>0</v>
       </c>
       <c r="V82" s="10">
-        <f>J82+K82+L82-100+M82+ SUM(O82:U82)*5+IF(ISNUMBER(Z82),Z82,0)+Y82</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W82" s="8">
@@ -13949,7 +13949,7 @@
         <v>0</v>
       </c>
       <c r="H83" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="I83" s="4">
@@ -13992,7 +13992,7 @@
         <v>0</v>
       </c>
       <c r="V83" s="10">
-        <f>J83+K83+L83-100+M83+ SUM(O83:U83)*5+IF(ISNUMBER(Z83),Z83,0)+Y83</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="W83" s="8">
@@ -14051,7 +14051,7 @@
         <v>0</v>
       </c>
       <c r="H84" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I84" s="4">
@@ -14094,7 +14094,7 @@
         <v>0</v>
       </c>
       <c r="V84" s="10">
-        <f>J84+K84+L84-100+M84+ SUM(O84:U84)*5+IF(ISNUMBER(Z84),Z84,0)+Y84</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W84" s="8">
@@ -14151,7 +14151,7 @@
         <v>1</v>
       </c>
       <c r="H85" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="I85" s="4">
@@ -14194,7 +14194,7 @@
         <v>0</v>
       </c>
       <c r="V85" s="10">
-        <f>J85+K85+L85-100+M85+ SUM(O85:U85)*5+IF(ISNUMBER(Z85),Z85,0)+Y85</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="W85" s="8">
@@ -14247,7 +14247,7 @@
         <v>2</v>
       </c>
       <c r="H86" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="I86" s="4">
@@ -14290,7 +14290,7 @@
         <v>0</v>
       </c>
       <c r="V86" s="10">
-        <f>J86+K86+L86-100+M86+ SUM(O86:U86)*5+IF(ISNUMBER(Z86),Z86,0)+Y86</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="W86" s="8">
@@ -14345,7 +14345,7 @@
         <v>3</v>
       </c>
       <c r="H87" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="I87" s="4">
@@ -14388,7 +14388,7 @@
         <v>0</v>
       </c>
       <c r="V87" s="10">
-        <f>J87+K87+L87-100+M87+ SUM(O87:U87)*5+IF(ISNUMBER(Z87),Z87,0)+Y87</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="W87" s="8">
@@ -14443,7 +14443,7 @@
         <v>4</v>
       </c>
       <c r="H88" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="I88" s="4">
@@ -14486,7 +14486,7 @@
         <v>0</v>
       </c>
       <c r="V88" s="10">
-        <f>J88+K88+L88-100+M88+ SUM(O88:U88)*5+IF(ISNUMBER(Z88),Z88,0)+Y88</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="W88" s="8">
@@ -14541,7 +14541,7 @@
         <v>1</v>
       </c>
       <c r="H89" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="I89" s="4">
@@ -14584,7 +14584,7 @@
         <v>0</v>
       </c>
       <c r="V89" s="10">
-        <f>J89+K89+L89-100+M89+ SUM(O89:U89)*5+IF(ISNUMBER(Z89),Z89,0)+Y89</f>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="W89" s="8">
@@ -14645,7 +14645,7 @@
         <v>5</v>
       </c>
       <c r="H90" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="I90" s="4">
@@ -14688,7 +14688,7 @@
         <v>0</v>
       </c>
       <c r="V90" s="10">
-        <f>J90+K90+L90-100+M90+ SUM(O90:U90)*5+IF(ISNUMBER(Z90),Z90,0)+Y90</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="W90" s="8">
@@ -14747,7 +14747,7 @@
         <v>5</v>
       </c>
       <c r="H91" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="I91" s="4">
@@ -14790,7 +14790,7 @@
         <v>0</v>
       </c>
       <c r="V91" s="10">
-        <f>J91+K91+L91-100+M91+ SUM(O91:U91)*5+IF(ISNUMBER(Z91),Z91,0)+Y91</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="W91" s="8">
@@ -14845,7 +14845,7 @@
         <v>6</v>
       </c>
       <c r="H92" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="I92" s="4">
@@ -14888,7 +14888,7 @@
         <v>0</v>
       </c>
       <c r="V92" s="10">
-        <f>J92+K92+L92-100+M92+ SUM(O92:U92)*5+IF(ISNUMBER(Z92),Z92,0)+Y92</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="W92" s="8">
@@ -14943,7 +14943,7 @@
         <v>3</v>
       </c>
       <c r="H93" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="I93" s="4">
@@ -14986,7 +14986,7 @@
         <v>0</v>
       </c>
       <c r="V93" s="10">
-        <f>J93+K93+L93-100+M93+ SUM(O93:U93)*5+IF(ISNUMBER(Z93),Z93,0)+Y93</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="W93" s="8">
@@ -15041,7 +15041,7 @@
         <v>0</v>
       </c>
       <c r="H94" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="I94" s="4">
@@ -15084,7 +15084,7 @@
         <v>0</v>
       </c>
       <c r="V94" s="10">
-        <f>J94+K94+L94-100+M94+ SUM(O94:U94)*5+IF(ISNUMBER(Z94),Z94,0)+Y94</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="W94" s="8">
@@ -15145,7 +15145,7 @@
         <v>0</v>
       </c>
       <c r="H95" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I95" s="4">
@@ -15188,7 +15188,7 @@
         <v>0</v>
       </c>
       <c r="V95" s="10">
-        <f>J95+K95+L95-100+M95+ SUM(O95:U95)*5+IF(ISNUMBER(Z95),Z95,0)+Y95</f>
+        <f t="shared" si="5"/>
         <v>-0.59999999999999964</v>
       </c>
       <c r="W95" s="8">
@@ -15247,7 +15247,7 @@
         <v>0</v>
       </c>
       <c r="H96" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="I96" s="4">
@@ -15290,7 +15290,7 @@
         <v>0</v>
       </c>
       <c r="V96" s="10">
-        <f>J96+K96+L96-100+M96+ SUM(O96:U96)*5+IF(ISNUMBER(Z96),Z96,0)+Y96</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="W96" s="8">
@@ -15345,7 +15345,7 @@
         <v>0</v>
       </c>
       <c r="H97" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I97" s="4">
@@ -15388,7 +15388,7 @@
         <v>0</v>
       </c>
       <c r="V97" s="10">
-        <f>J97+K97+L97-100+M97+ SUM(O97:U97)*5+IF(ISNUMBER(Z97),Z97,0)+Y97</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W97" s="8">
@@ -15443,7 +15443,7 @@
         <v>0</v>
       </c>
       <c r="H98" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="I98" s="4">
@@ -15486,7 +15486,7 @@
         <v>0</v>
       </c>
       <c r="V98" s="18">
-        <f>J98+K98+L98-100+M98+ SUM(O98:U98)*5+IF(ISNUMBER(Z98),Z98,0)+Y98</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="W98" s="8">
@@ -15547,7 +15547,7 @@
         <v>0</v>
       </c>
       <c r="H99" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="I99" s="4">
@@ -15590,7 +15590,7 @@
         <v>0</v>
       </c>
       <c r="V99" s="10">
-        <f>J99+K99+L99-100+M99+ SUM(O99:U99)*5+IF(ISNUMBER(Z99),Z99,0)+Y99</f>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="W99" s="8">
@@ -15649,7 +15649,7 @@
         <v>0</v>
       </c>
       <c r="H100" s="4">
-        <f t="shared" ref="H100:H124" si="3">IF(AND(V100&gt;=13,V100&lt;=16),5,IF(AND(V100&gt;=9,V100&lt;=12),4,IF(AND(V100&gt;=5,V100&lt;=8),3,IF(AND(V100&gt;=1,V100&lt;=4),2,IF(AND(V100&gt;=-3,V100&lt;=0),1,IF(AND(V100&gt;=-5,V100&lt;=-4),0,6))))))</f>
+        <f t="shared" ref="H100:H124" si="6">IF(AND(V100&gt;=13,V100&lt;=16),5,IF(AND(V100&gt;=9,V100&lt;=12),4,IF(AND(V100&gt;=5,V100&lt;=8),3,IF(AND(V100&gt;=1,V100&lt;=4),2,IF(AND(V100&gt;=-3,V100&lt;=0),1,IF(AND(V100&gt;=-5,V100&lt;=-4),0,6))))))</f>
         <v>1</v>
       </c>
       <c r="I100" s="4">
@@ -15692,7 +15692,7 @@
         <v>0</v>
       </c>
       <c r="V100" s="10">
-        <f>J100+K100+L100-100+M100+ SUM(O100:U100)*5+IF(ISNUMBER(Z100),Z100,0)+Y100</f>
+        <f t="shared" ref="V100:V131" si="7">J100+K100+L100-100+M100+ SUM(O100:U100)*5+IF(ISNUMBER(Z100),Z100,0)+Y100</f>
         <v>0</v>
       </c>
       <c r="W100" s="8">
@@ -15753,7 +15753,7 @@
         <v>6</v>
       </c>
       <c r="H101" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="I101" s="4">
@@ -15796,7 +15796,7 @@
         <v>0</v>
       </c>
       <c r="V101" s="10">
-        <f>J101+K101+L101-100+M101+ SUM(O101:U101)*5+IF(ISNUMBER(Z101),Z101,0)+Y101</f>
+        <f t="shared" si="7"/>
         <v>6.8000000000000007</v>
       </c>
       <c r="W101" s="8">
@@ -15853,7 +15853,7 @@
         <v>0</v>
       </c>
       <c r="H102" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I102" s="4">
@@ -15896,7 +15896,7 @@
         <v>0</v>
       </c>
       <c r="V102" s="10">
-        <f>J102+K102+L102-100+M102+ SUM(O102:U102)*5+IF(ISNUMBER(Z102),Z102,0)+Y102</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W102" s="8">
@@ -15951,7 +15951,7 @@
         <v>0</v>
       </c>
       <c r="H103" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="I103" s="4">
@@ -15994,7 +15994,7 @@
         <v>0</v>
       </c>
       <c r="V103" s="10">
-        <f>J103+K103+L103-100+M103+ SUM(O103:U103)*5+IF(ISNUMBER(Z103),Z103,0)+Y103</f>
+        <f t="shared" si="7"/>
         <v>10.5</v>
       </c>
       <c r="W103" s="8">
@@ -16055,7 +16055,7 @@
         <v>0</v>
       </c>
       <c r="H104" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="I104" s="4">
@@ -16098,7 +16098,7 @@
         <v>0</v>
       </c>
       <c r="V104" s="10">
-        <f>J104+K104+L104-100+M104+ SUM(O104:U104)*5+IF(ISNUMBER(Z104),Z104,0)+Y104</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="W104" s="8">
@@ -16157,7 +16157,7 @@
         <v>0</v>
       </c>
       <c r="H105" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="I105" s="4">
@@ -16200,7 +16200,7 @@
         <v>0</v>
       </c>
       <c r="V105" s="10">
-        <f>J105+K105+L105-100+M105+ SUM(O105:U105)*5+IF(ISNUMBER(Z105),Z105,0)+Y105</f>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="W105" s="8">
@@ -16257,7 +16257,7 @@
         <v>0</v>
       </c>
       <c r="H106" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="I106" s="4">
@@ -16300,7 +16300,7 @@
         <v>3</v>
       </c>
       <c r="V106" s="10">
-        <f>J106+K106+L106-100+M106+ SUM(O106:U106)*5+IF(ISNUMBER(Z106),Z106,0)+Y106</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="W106" s="8">
@@ -16357,7 +16357,7 @@
         <v>0</v>
       </c>
       <c r="H107" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="I107" s="4">
@@ -16400,7 +16400,7 @@
         <v>0</v>
       </c>
       <c r="V107" s="10">
-        <f>J107+K107+L107-100+M107+ SUM(O107:U107)*5+IF(ISNUMBER(Z107),Z107,0)+Y107</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="W107" s="8">
@@ -16459,7 +16459,7 @@
         <v>0</v>
       </c>
       <c r="H108" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I108" s="4">
@@ -16502,7 +16502,7 @@
         <v>0</v>
       </c>
       <c r="V108" s="10">
-        <f>J108+K108+L108-100+M108+ SUM(O108:U108)*5+IF(ISNUMBER(Z108),Z108,0)+Y108</f>
+        <f t="shared" si="7"/>
         <v>-2</v>
       </c>
       <c r="W108" s="8">
@@ -16561,7 +16561,7 @@
         <v>0</v>
       </c>
       <c r="H109" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="I109" s="4">
@@ -16604,7 +16604,7 @@
         <v>0</v>
       </c>
       <c r="V109" s="10">
-        <f>J109+K109+L109-100+M109+ SUM(O109:U109)*5+IF(ISNUMBER(Z109),Z109,0)+Y109</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="W109" s="8">
@@ -16659,7 +16659,7 @@
         <v>0</v>
       </c>
       <c r="H110" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="I110" s="4">
@@ -16702,7 +16702,7 @@
         <v>0</v>
       </c>
       <c r="V110" s="10">
-        <f>J110+K110+L110-100+M110+ SUM(O110:U110)*5+IF(ISNUMBER(Z110),Z110,0)+Y110</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="W110" s="8">
@@ -16759,7 +16759,7 @@
         <v>0</v>
       </c>
       <c r="H111" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I111" s="4">
@@ -16802,7 +16802,7 @@
         <v>0</v>
       </c>
       <c r="V111" s="10">
-        <f>J111+K111+L111-100+M111+ SUM(O111:U111)*5+IF(ISNUMBER(Z111),Z111,0)+Y111</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W111" s="8">
@@ -16857,7 +16857,7 @@
         <v>0</v>
       </c>
       <c r="H112" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="I112" s="4">
@@ -16900,7 +16900,7 @@
         <v>0</v>
       </c>
       <c r="V112" s="10">
-        <f>J112+K112+L112-100+M112+ SUM(O112:U112)*5+IF(ISNUMBER(Z112),Z112,0)+Y112</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="W112" s="8">
@@ -16957,7 +16957,7 @@
         <v>0</v>
       </c>
       <c r="H113" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="I113" s="4">
@@ -17000,7 +17000,7 @@
         <v>0</v>
       </c>
       <c r="V113" s="10">
-        <f>J113+K113+L113-100+M113+ SUM(O113:U113)*5+IF(ISNUMBER(Z113),Z113,0)+Y113</f>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="W113" s="8">
@@ -17059,7 +17059,7 @@
         <v>0</v>
       </c>
       <c r="H114" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="I114" s="4">
@@ -17102,7 +17102,7 @@
         <v>0</v>
       </c>
       <c r="V114" s="18">
-        <f>J114+K114+L114-100+M114+ SUM(O114:U114)*5+IF(ISNUMBER(Z114),Z114,0)+Y114</f>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="W114" s="8">
@@ -17157,7 +17157,7 @@
         <v>0</v>
       </c>
       <c r="H115" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="I115" s="4">
@@ -17200,7 +17200,7 @@
         <v>0</v>
       </c>
       <c r="V115" s="18">
-        <f>J115+K115+L115-100+M115+ SUM(O115:U115)*5+IF(ISNUMBER(Z115),Z115,0)+Y115</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="W115" s="8">
@@ -17257,7 +17257,7 @@
         <v>0</v>
       </c>
       <c r="H116" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="I116" s="4">
@@ -17300,7 +17300,7 @@
         <v>0</v>
       </c>
       <c r="V116" s="36">
-        <f>J116+K116+L116-100+M116+ SUM(O116:U116)*5+IF(ISNUMBER(Z116),Z116,0)+Y116</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="W116" s="8">
@@ -17357,7 +17357,7 @@
         <v>0</v>
       </c>
       <c r="H117" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="I117" s="4">
@@ -17400,7 +17400,7 @@
         <v>0</v>
       </c>
       <c r="V117" s="36">
-        <f>J117+K117+L117-100+M117+ SUM(O117:U117)*5+IF(ISNUMBER(Z117),Z117,0)+Y117</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W117" s="8">
@@ -17457,7 +17457,7 @@
         <v>0</v>
       </c>
       <c r="H118" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="I118" s="4">
@@ -17500,7 +17500,7 @@
         <v>0</v>
       </c>
       <c r="V118" s="18">
-        <f>J118+K118+L118-100+M118+ SUM(O118:U118)*5+IF(ISNUMBER(Z118),Z118,0)+Y118</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="W118" s="8">
@@ -17559,7 +17559,7 @@
         <v>0</v>
       </c>
       <c r="H119" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="I119" s="4">
@@ -17602,7 +17602,7 @@
         <v>0</v>
       </c>
       <c r="V119" s="18">
-        <f>J119+K119+L119-100+M119+ SUM(O119:U119)*5+IF(ISNUMBER(Z119),Z119,0)+Y119</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="W119" s="8">
@@ -17661,7 +17661,7 @@
         <v>0</v>
       </c>
       <c r="H120" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="I120" s="4">
@@ -17704,7 +17704,7 @@
         <v>0</v>
       </c>
       <c r="V120" s="18">
-        <f>J120+K120+L120-100+M120+ SUM(O120:U120)*5+IF(ISNUMBER(Z120),Z120,0)+Y120</f>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="W120" s="8">
@@ -17761,7 +17761,7 @@
         <v>0</v>
       </c>
       <c r="H121" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="I121" s="15">
@@ -17804,7 +17804,7 @@
         <v>0</v>
       </c>
       <c r="V121" s="18">
-        <f>J121+K121+L121-100+M121+ SUM(O121:U121)*5+IF(ISNUMBER(Z121),Z121,0)+Y121</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="W121" s="8">
@@ -17859,7 +17859,7 @@
         <v>0</v>
       </c>
       <c r="H122" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="I122" s="15">
@@ -17902,7 +17902,7 @@
         <v>0</v>
       </c>
       <c r="V122" s="35">
-        <f>J122+K122+L122-100+M122+ SUM(O122:U122)*5+IF(ISNUMBER(Z122),Z122,0)+Y122</f>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="W122" s="8">
@@ -17957,7 +17957,7 @@
         <v>0</v>
       </c>
       <c r="H123" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="I123" s="15">
@@ -18000,7 +18000,7 @@
         <v>0</v>
       </c>
       <c r="V123" s="35">
-        <f>J123+K123+L123-100+M123+ SUM(O123:U123)*5+IF(ISNUMBER(Z123),Z123,0)+Y123</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="W123" s="8">
@@ -18055,7 +18055,7 @@
         <v>0</v>
       </c>
       <c r="H124" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="I124" s="15">
@@ -18098,7 +18098,7 @@
         <v>0</v>
       </c>
       <c r="V124" s="18">
-        <f>J124+K124+L124-100+M124+ SUM(O124:U124)*5+IF(ISNUMBER(Z124),Z124,0)+Y124</f>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="W124" s="8">
@@ -18153,7 +18153,7 @@
         <v>0</v>
       </c>
       <c r="H125" s="41">
-        <f t="shared" ref="H125" si="4">IF(AND(V125&gt;=13,V125&lt;=16),5,IF(AND(V125&gt;=9,V125&lt;=12),4,IF(AND(V125&gt;=5,V125&lt;=8),3,IF(AND(V125&gt;=1,V125&lt;=4),2,IF(AND(V125&gt;=-3,V125&lt;=0),1,IF(AND(V125&gt;=-5,V125&lt;=-4),0,6))))))</f>
+        <f t="shared" ref="H125" si="8">IF(AND(V125&gt;=13,V125&lt;=16),5,IF(AND(V125&gt;=9,V125&lt;=12),4,IF(AND(V125&gt;=5,V125&lt;=8),3,IF(AND(V125&gt;=1,V125&lt;=4),2,IF(AND(V125&gt;=-3,V125&lt;=0),1,IF(AND(V125&gt;=-5,V125&lt;=-4),0,6))))))</f>
         <v>3</v>
       </c>
       <c r="I125" s="15">
@@ -18196,7 +18196,7 @@
         <v>0</v>
       </c>
       <c r="V125" s="10">
-        <f>J125+K125+L125-100+M125+ SUM(O125:U125)*5+IF(ISNUMBER(Z125),Z125,0)+Y125</f>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="W125" s="8">
@@ -18251,7 +18251,7 @@
         <v>0</v>
       </c>
       <c r="H126" s="41">
-        <f t="shared" ref="H126:H127" si="5">IF(AND(V126&gt;=13,V126&lt;=16),5,IF(AND(V126&gt;=9,V126&lt;=12),4,IF(AND(V126&gt;=5,V126&lt;=8),3,IF(AND(V126&gt;=1,V126&lt;=4),2,IF(AND(V126&gt;=-3,V126&lt;=0),1,IF(AND(V126&gt;=-5,V126&lt;=-4),0,6))))))</f>
+        <f t="shared" ref="H126:H127" si="9">IF(AND(V126&gt;=13,V126&lt;=16),5,IF(AND(V126&gt;=9,V126&lt;=12),4,IF(AND(V126&gt;=5,V126&lt;=8),3,IF(AND(V126&gt;=1,V126&lt;=4),2,IF(AND(V126&gt;=-3,V126&lt;=0),1,IF(AND(V126&gt;=-5,V126&lt;=-4),0,6))))))</f>
         <v>2</v>
       </c>
       <c r="I126" s="15">
@@ -18294,7 +18294,7 @@
         <v>0</v>
       </c>
       <c r="V126" s="10">
-        <f>J126+K126+L126-100+M126+ SUM(O126:U126)*5+IF(ISNUMBER(Z126),Z126,0)+Y126</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="W126" s="8">
@@ -18349,7 +18349,7 @@
         <v>0</v>
       </c>
       <c r="H127" s="41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="I127" s="15">
@@ -18392,7 +18392,7 @@
         <v>0</v>
       </c>
       <c r="V127" s="10">
-        <f>J127+K127+L127-100+M127+ SUM(O127:U127)*5+IF(ISNUMBER(Z127),Z127,0)+Y127</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="W127" s="8">
@@ -18447,7 +18447,7 @@
         <v>0</v>
       </c>
       <c r="H128" s="41">
-        <f t="shared" ref="H128" si="6">IF(AND(V128&gt;=13,V128&lt;=16),5,IF(AND(V128&gt;=9,V128&lt;=12),4,IF(AND(V128&gt;=5,V128&lt;=8),3,IF(AND(V128&gt;=1,V128&lt;=4),2,IF(AND(V128&gt;=-3,V128&lt;=0),1,IF(AND(V128&gt;=-5,V128&lt;=-4),0,6))))))</f>
+        <f t="shared" ref="H128" si="10">IF(AND(V128&gt;=13,V128&lt;=16),5,IF(AND(V128&gt;=9,V128&lt;=12),4,IF(AND(V128&gt;=5,V128&lt;=8),3,IF(AND(V128&gt;=1,V128&lt;=4),2,IF(AND(V128&gt;=-3,V128&lt;=0),1,IF(AND(V128&gt;=-5,V128&lt;=-4),0,6))))))</f>
         <v>1</v>
       </c>
       <c r="I128" s="15">
@@ -18490,7 +18490,7 @@
         <v>0</v>
       </c>
       <c r="V128" s="10">
-        <f>J128+K128+L128-100+M128+ SUM(O128:U128)*5+IF(ISNUMBER(Z128),Z128,0)+Y128</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W128" s="8">
@@ -18545,7 +18545,7 @@
         <v>0</v>
       </c>
       <c r="H129" s="41">
-        <f t="shared" ref="H129:H130" si="7">IF(AND(V129&gt;=13,V129&lt;=16),5,IF(AND(V129&gt;=9,V129&lt;=12),4,IF(AND(V129&gt;=5,V129&lt;=8),3,IF(AND(V129&gt;=1,V129&lt;=4),2,IF(AND(V129&gt;=-3,V129&lt;=0),1,IF(AND(V129&gt;=-5,V129&lt;=-4),0,6))))))</f>
+        <f t="shared" ref="H129:H130" si="11">IF(AND(V129&gt;=13,V129&lt;=16),5,IF(AND(V129&gt;=9,V129&lt;=12),4,IF(AND(V129&gt;=5,V129&lt;=8),3,IF(AND(V129&gt;=1,V129&lt;=4),2,IF(AND(V129&gt;=-3,V129&lt;=0),1,IF(AND(V129&gt;=-5,V129&lt;=-4),0,6))))))</f>
         <v>2</v>
       </c>
       <c r="I129" s="15">
@@ -18588,7 +18588,7 @@
         <v>0</v>
       </c>
       <c r="V129" s="10">
-        <f>J129+K129+L129-100+M129+ SUM(O129:U129)*5+IF(ISNUMBER(Z129),Z129,0)+Y129</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="W129" s="8">
@@ -18645,7 +18645,7 @@
         <v>0</v>
       </c>
       <c r="H130" s="41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="I130" s="15">
@@ -18661,10 +18661,10 @@
         <v>0</v>
       </c>
       <c r="M130" s="14">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N130" s="8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O130" s="8">
         <v>0</v>
@@ -18688,7 +18688,7 @@
         <v>0</v>
       </c>
       <c r="V130" s="10">
-        <f>J130+K130+L130-100+M130+ SUM(O130:U130)*5+IF(ISNUMBER(Z130),Z130,0)+Y130</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="W130" s="8">
@@ -18702,13 +18702,13 @@
       </c>
       <c r="Z130" s="10">
         <f>IF(ISBLANK(AA130),0, LOOKUP(AA130,[1]Skill!$A:$A,[1]Skill!$X:$X)*AB130/100)</f>
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="AA130" s="15">
         <v>55990106</v>
       </c>
       <c r="AB130" s="15">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="AC130" s="4" t="s">
         <v>383</v>
@@ -18921,33 +18921,33 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H124">
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="12" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="13" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="83" priority="14" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="6" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="8" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="9" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="10" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18964,16 +18964,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H125:H130">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="74" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19427,19 +19427,19 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="2" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix the weapon qulity error
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Weapon.xlsx
+++ b/ConfigData/Xlsx/Weapon.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -1359,7 +1359,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1596,6 +1596,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1603,6 +1604,7 @@
       <sz val="10.5"/>
       <color theme="1"/>
       <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="42">
@@ -2333,15 +2335,6 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="82">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3185,6 +3178,15 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -3725,72 +3727,6 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
     <mruColors>
       <color rgb="FFCC66FF"/>
     </mruColors>
@@ -5107,7 +5043,6 @@
           <cell r="A162">
             <v>55900028</v>
           </cell>
-          <cell r="Z162"/>
         </row>
         <row r="163">
           <cell r="A163">
@@ -5509,102 +5444,102 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AG133" totalsRowShown="0" dataDxfId="73" tableBorderDxfId="72">
-  <autoFilter ref="A3:AG133"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AG133" totalsRowShown="0" dataDxfId="73" tableBorderDxfId="72">
+  <autoFilter ref="A3:AG133" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A4:AF124">
     <sortCondition ref="A3:A124"/>
   </sortState>
   <tableColumns count="33">
-    <tableColumn id="1" name="Id" dataDxfId="71"/>
-    <tableColumn id="2" name="Name" dataDxfId="70"/>
-    <tableColumn id="3" name="Ename" dataDxfId="69"/>
-    <tableColumn id="4" name="Remark" dataDxfId="68"/>
-    <tableColumn id="5" name="Star" dataDxfId="67"/>
-    <tableColumn id="6" name="Type" dataDxfId="66"/>
-    <tableColumn id="7" name="Attr" dataDxfId="65"/>
-    <tableColumn id="34" name="Quality" dataDxfId="64">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="71"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Ename" dataDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Remark" dataDxfId="68"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Star" dataDxfId="67"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Type" dataDxfId="66"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Attr" dataDxfId="65"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Quality" dataDxfId="64">
       <calculatedColumnFormula>IF(AND(V4&gt;=13,V4&lt;=16),5,IF(AND(V4&gt;=9,V4&lt;=12),4,IF(AND(V4&gt;=5,V4&lt;=8),3,IF(AND(V4&gt;=1,V4&lt;=4),2,IF(AND(V4&gt;=-3,V4&lt;=0),1,IF(AND(V4&gt;=-5,V4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Cost" dataDxfId="63"/>
-    <tableColumn id="8" name="AtkP" dataDxfId="62"/>
-    <tableColumn id="9" name="PArmor" dataDxfId="61"/>
-    <tableColumn id="17" name="MArmor" dataDxfId="60"/>
-    <tableColumn id="25" name="Modify" dataDxfId="59"/>
-    <tableColumn id="27" name="Dura" dataDxfId="58"/>
-    <tableColumn id="20" name="Def" dataDxfId="57"/>
-    <tableColumn id="21" name="Mag" dataDxfId="56"/>
-    <tableColumn id="29" name="Spd" dataDxfId="55"/>
-    <tableColumn id="30" name="Hit" dataDxfId="54"/>
-    <tableColumn id="19" name="Dhit" dataDxfId="53"/>
-    <tableColumn id="12" name="Crt" dataDxfId="52"/>
-    <tableColumn id="11" name="Luk" dataDxfId="51"/>
-    <tableColumn id="32" name="Sum" dataDxfId="50">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Cost" dataDxfId="63"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="AtkP" dataDxfId="62"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="PArmor" dataDxfId="61"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="MArmor" dataDxfId="60"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Modify" dataDxfId="59"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Dura" dataDxfId="58"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Def" dataDxfId="57"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Mag" dataDxfId="56"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Spd" dataDxfId="55"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Hit" dataDxfId="54"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Dhit" dataDxfId="53"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Crt" dataDxfId="52"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Luk" dataDxfId="51"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Sum" dataDxfId="50">
       <calculatedColumnFormula>J4+K4+L4-100+M4+ SUM(O4:U4)*5+IF(ISNUMBER(Z4),Z4,0)+Y4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Range" dataDxfId="49"/>
-    <tableColumn id="31" name="Mov" dataDxfId="48"/>
-    <tableColumn id="24" name="~SkillMark" dataDxfId="47"/>
-    <tableColumn id="33" name="~SkillMark2" dataDxfId="0">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Range" dataDxfId="49"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Mov" dataDxfId="48"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="~SkillMark" dataDxfId="47"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="~SkillMark2" dataDxfId="46">
       <calculatedColumnFormula>IF(ISBLANK(AA4),0, LOOKUP(AA4,[1]Skill!$A:$A,[1]Skill!$Z:$Z)*AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="SkillId" dataDxfId="46"/>
-    <tableColumn id="14" name="Percent" dataDxfId="45"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="44"/>
-    <tableColumn id="26" name="JobId" dataDxfId="43"/>
-    <tableColumn id="18" name="Icon" dataDxfId="42"/>
-    <tableColumn id="22" name="IsSpecial" dataDxfId="41"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="40"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="SkillId" dataDxfId="45"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Percent" dataDxfId="44"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Arrow" dataDxfId="43"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="JobId" dataDxfId="42"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Icon" dataDxfId="41"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="IsSpecial" dataDxfId="40"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="IsNew" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AG4" totalsRowShown="0" dataDxfId="34" tableBorderDxfId="33">
-  <autoFilter ref="A3:AG4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表1_3" displayName="表1_3" ref="A3:AG4" totalsRowShown="0" dataDxfId="33" tableBorderDxfId="32">
+  <autoFilter ref="A3:AG4" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState ref="A4:W130">
     <sortCondition ref="A3:A130"/>
   </sortState>
   <tableColumns count="33">
-    <tableColumn id="1" name="Id" dataDxfId="32"/>
-    <tableColumn id="2" name="Name" dataDxfId="31"/>
-    <tableColumn id="3" name="Ename" dataDxfId="30"/>
-    <tableColumn id="4" name="Remark" dataDxfId="29"/>
-    <tableColumn id="5" name="Star" dataDxfId="28"/>
-    <tableColumn id="6" name="Type" dataDxfId="27"/>
-    <tableColumn id="7" name="Attr" dataDxfId="26"/>
-    <tableColumn id="34" name="Quality" dataDxfId="25">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Ename" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Remark" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Star" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Type" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Attr" dataDxfId="25"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0100-000022000000}" name="Quality" dataDxfId="24">
       <calculatedColumnFormula>IF(AND(V4&gt;=13,V4&lt;=16),5,IF(AND(V4&gt;=9,V4&lt;=12),4,IF(AND(V4&gt;=5,V4&lt;=8),3,IF(AND(V4&gt;=1,V4&lt;=4),2,IF(AND(V4&gt;=-3,V4&lt;=0),1,IF(AND(V4&gt;=-5,V4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Cost" dataDxfId="24"/>
-    <tableColumn id="8" name="AtkP" dataDxfId="23"/>
-    <tableColumn id="9" name="PArmor" dataDxfId="22"/>
-    <tableColumn id="17" name="MArmor" dataDxfId="21"/>
-    <tableColumn id="25" name="Modify" dataDxfId="20"/>
-    <tableColumn id="31" name="Dura" dataDxfId="19"/>
-    <tableColumn id="11" name="Def" dataDxfId="18"/>
-    <tableColumn id="21" name="Mag" dataDxfId="17"/>
-    <tableColumn id="29" name="Spd" dataDxfId="16"/>
-    <tableColumn id="30" name="Hit" dataDxfId="15"/>
-    <tableColumn id="20" name="Dhit" dataDxfId="14"/>
-    <tableColumn id="19" name="Crt" dataDxfId="13"/>
-    <tableColumn id="12" name="Luk" dataDxfId="12"/>
-    <tableColumn id="32" name="Sum" dataDxfId="11">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Cost" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="AtkP" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="PArmor" dataDxfId="21"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="MArmor" dataDxfId="20"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Modify" dataDxfId="19"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0100-00001F000000}" name="Dura" dataDxfId="18"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Def" dataDxfId="17"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="Mag" dataDxfId="16"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0100-00001D000000}" name="Spd" dataDxfId="15"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0100-00001E000000}" name="Hit" dataDxfId="14"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Dhit" dataDxfId="13"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Crt" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Luk" dataDxfId="11"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0100-000020000000}" name="Sum" dataDxfId="10">
       <calculatedColumnFormula>J4+K4+L4-100+M4+ SUM(O4:U4)*5+IF(ISNUMBER(Z4),Z4,0)+Y4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Range" dataDxfId="10"/>
-    <tableColumn id="27" name="Mov" dataDxfId="9"/>
-    <tableColumn id="24" name="~SkillMark" dataDxfId="8"/>
-    <tableColumn id="33" name="~SkillMark2" dataDxfId="7">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Range" dataDxfId="9"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Mov" dataDxfId="8"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="~SkillMark" dataDxfId="7"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0100-000021000000}" name="~SkillMark2" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(AA4),0, LOOKUP(AA4,[1]Skill!$A:$A,[1]Skill!$Z:$Z)*AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="SkillId" dataDxfId="6"/>
-    <tableColumn id="14" name="Percent" dataDxfId="5"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="4"/>
-    <tableColumn id="26" name="JobId"/>
-    <tableColumn id="18" name="Icon" dataDxfId="3"/>
-    <tableColumn id="22" name="IsSpecial" dataDxfId="2"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="SkillId" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Percent" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Arrow" dataDxfId="3"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0100-00001A000000}" name="JobId"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Icon" dataDxfId="2"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="IsSpecial" dataDxfId="1"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="IsNew" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5618,7 +5553,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C7EDCC"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -5930,14 +5865,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B109" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Z111" sqref="Z111"/>
+      <selection pane="bottomRight" activeCell="M29" sqref="M29:M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6327,7 +6262,7 @@
         <v>0</v>
       </c>
       <c r="V4" s="10">
-        <f t="shared" ref="V4:V35" si="1">J4+K4+L4-100+M4+ SUM(O4:U4)*5+IF(ISNUMBER(Z4),Z4,0)+Y4</f>
+        <f>J4+K4+L4-100+M4+ SUM(O4:U4)*5+IF(ISNUMBER(Z4),Z4,0)+Y4</f>
         <v>-5</v>
       </c>
       <c r="W4" s="8">
@@ -6425,7 +6360,7 @@
         <v>0</v>
       </c>
       <c r="V5" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="V4:V35" si="1">J5+K5+L5-100+M5+ SUM(O5:U5)*5+IF(ISNUMBER(Z5),Z5,0)+Y5</f>
         <v>-5</v>
       </c>
       <c r="W5" s="8">
@@ -7165,7 +7100,7 @@
       </c>
       <c r="H13" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I13" s="4">
         <v>2</v>
@@ -7180,7 +7115,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="8">
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="N13" s="8">
         <v>3</v>
@@ -7208,7 +7143,7 @@
       </c>
       <c r="V13" s="10">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>-2</v>
       </c>
       <c r="W13" s="8">
         <v>10</v>
@@ -7267,7 +7202,7 @@
       </c>
       <c r="H14" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I14" s="4">
         <v>2</v>
@@ -7282,7 +7217,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="8">
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="N14" s="8">
         <v>3</v>
@@ -7310,7 +7245,7 @@
       </c>
       <c r="V14" s="18">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>-2</v>
       </c>
       <c r="W14" s="8">
         <v>10</v>
@@ -7369,7 +7304,7 @@
       </c>
       <c r="H15" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I15" s="4">
         <v>2</v>
@@ -7384,7 +7319,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="8">
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="N15" s="8">
         <v>3</v>
@@ -7412,7 +7347,7 @@
       </c>
       <c r="V15" s="10">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>-2</v>
       </c>
       <c r="W15" s="8">
         <v>10</v>
@@ -7471,7 +7406,7 @@
       </c>
       <c r="H16" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I16" s="4">
         <v>2</v>
@@ -7486,7 +7421,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="8">
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="N16" s="8">
         <v>3</v>
@@ -7514,7 +7449,7 @@
       </c>
       <c r="V16" s="10">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>-2</v>
       </c>
       <c r="W16" s="8">
         <v>10</v>
@@ -7573,7 +7508,7 @@
       </c>
       <c r="H17" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I17" s="4">
         <v>2</v>
@@ -7588,7 +7523,7 @@
         <v>0</v>
       </c>
       <c r="M17" s="8">
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="N17" s="8">
         <v>3</v>
@@ -7616,7 +7551,7 @@
       </c>
       <c r="V17" s="18">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>-2</v>
       </c>
       <c r="W17" s="8">
         <v>10</v>
@@ -7675,7 +7610,7 @@
       </c>
       <c r="H18" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I18" s="4">
         <v>2</v>
@@ -7690,7 +7625,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="8">
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="N18" s="8">
         <v>3</v>
@@ -7718,7 +7653,7 @@
       </c>
       <c r="V18" s="10">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>-2</v>
       </c>
       <c r="W18" s="8">
         <v>10</v>
@@ -8779,7 +8714,7 @@
       </c>
       <c r="H29" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I29" s="4">
         <v>1</v>
@@ -8794,7 +8729,7 @@
         <v>0</v>
       </c>
       <c r="M29" s="8">
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="N29" s="8">
         <v>3</v>
@@ -8822,7 +8757,7 @@
       </c>
       <c r="V29" s="10">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>-2</v>
       </c>
       <c r="W29" s="8">
         <v>0</v>
@@ -8881,7 +8816,7 @@
       </c>
       <c r="H30" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I30" s="4">
         <v>1</v>
@@ -8896,7 +8831,7 @@
         <v>0</v>
       </c>
       <c r="M30" s="8">
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="N30" s="8">
         <v>3</v>
@@ -8924,7 +8859,7 @@
       </c>
       <c r="V30" s="18">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>-2</v>
       </c>
       <c r="W30" s="8">
         <v>0</v>
@@ -8983,7 +8918,7 @@
       </c>
       <c r="H31" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I31" s="4">
         <v>1</v>
@@ -8998,7 +8933,7 @@
         <v>0</v>
       </c>
       <c r="M31" s="8">
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="N31" s="8">
         <v>3</v>
@@ -9026,7 +8961,7 @@
       </c>
       <c r="V31" s="10">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>-2</v>
       </c>
       <c r="W31" s="8">
         <v>0</v>
@@ -9085,7 +9020,7 @@
       </c>
       <c r="H32" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I32" s="4">
         <v>1</v>
@@ -9100,7 +9035,7 @@
         <v>0</v>
       </c>
       <c r="M32" s="8">
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="N32" s="8">
         <v>3</v>
@@ -9128,7 +9063,7 @@
       </c>
       <c r="V32" s="10">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>-2</v>
       </c>
       <c r="W32" s="8">
         <v>0</v>
@@ -9187,7 +9122,7 @@
       </c>
       <c r="H33" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I33" s="4">
         <v>1</v>
@@ -9202,7 +9137,7 @@
         <v>0</v>
       </c>
       <c r="M33" s="8">
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="N33" s="8">
         <v>3</v>
@@ -9230,7 +9165,7 @@
       </c>
       <c r="V33" s="10">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>-2</v>
       </c>
       <c r="W33" s="8">
         <v>0</v>
@@ -9289,7 +9224,7 @@
       </c>
       <c r="H34" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I34" s="4">
         <v>1</v>
@@ -9304,7 +9239,7 @@
         <v>0</v>
       </c>
       <c r="M34" s="8">
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="N34" s="8">
         <v>3</v>
@@ -9332,7 +9267,7 @@
       </c>
       <c r="V34" s="10">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>-2</v>
       </c>
       <c r="W34" s="8">
         <v>0</v>
@@ -19288,7 +19223,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AG4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -19717,19 +19652,19 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="2" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19754,7 +19689,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
add the hero card stat
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Weapon.xlsx
+++ b/ConfigData/Xlsx/Weapon.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView minimized="1" xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="396">
   <si>
     <t>铁杖</t>
   </si>
@@ -1353,6 +1353,14 @@
   </si>
   <si>
     <t>Wand of Light</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>英雄卡片</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>IsHeroCard</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2132,7 +2140,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2212,12 +2220,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="38" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2334,15 +2336,200 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="82">
+  <dxfs count="84">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC66FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC66FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -2950,64 +3137,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -3185,6 +3314,15 @@
         </top>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3628,105 +3766,75 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
     <mruColors>
       <color rgb="FFCC66FF"/>
     </mruColors>
@@ -5123,6 +5231,7 @@
           <cell r="A172">
             <v>55900028</v>
           </cell>
+          <cell r="AB172"/>
         </row>
         <row r="173">
           <cell r="A173">
@@ -5572,108 +5681,104 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AG133" totalsRowShown="0" dataDxfId="73" tableBorderDxfId="72">
-  <autoFilter ref="A3:AG133">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="0"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A3:AH133" totalsRowShown="0" dataDxfId="83" tableBorderDxfId="82">
+  <autoFilter ref="A3:AH133"/>
   <sortState ref="A4:AF124">
     <sortCondition ref="A3:A124"/>
   </sortState>
-  <tableColumns count="33">
-    <tableColumn id="1" name="Id" dataDxfId="71"/>
-    <tableColumn id="2" name="Name" dataDxfId="70"/>
-    <tableColumn id="3" name="Ename" dataDxfId="69"/>
-    <tableColumn id="4" name="Remark" dataDxfId="68"/>
-    <tableColumn id="5" name="Star" dataDxfId="67"/>
-    <tableColumn id="6" name="Type" dataDxfId="66"/>
-    <tableColumn id="7" name="Attr" dataDxfId="65"/>
-    <tableColumn id="34" name="Quality" dataDxfId="64">
+  <tableColumns count="34">
+    <tableColumn id="1" name="Id" dataDxfId="81"/>
+    <tableColumn id="2" name="Name" dataDxfId="80"/>
+    <tableColumn id="3" name="Ename" dataDxfId="79"/>
+    <tableColumn id="4" name="Remark" dataDxfId="78"/>
+    <tableColumn id="5" name="Star" dataDxfId="77"/>
+    <tableColumn id="6" name="Type" dataDxfId="76"/>
+    <tableColumn id="7" name="Attr" dataDxfId="75"/>
+    <tableColumn id="34" name="Quality" dataDxfId="74">
       <calculatedColumnFormula>IF(AND(V4&gt;=13,V4&lt;=16),5,IF(AND(V4&gt;=9,V4&lt;=12),4,IF(AND(V4&gt;=5,V4&lt;=8),3,IF(AND(V4&gt;=1,V4&lt;=4),2,IF(AND(V4&gt;=-3,V4&lt;=0),1,IF(AND(V4&gt;=-5,V4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Cost" dataDxfId="63"/>
-    <tableColumn id="8" name="AtkP" dataDxfId="62"/>
-    <tableColumn id="9" name="PArmor" dataDxfId="61"/>
-    <tableColumn id="17" name="MArmor" dataDxfId="60"/>
-    <tableColumn id="25" name="Modify" dataDxfId="59"/>
-    <tableColumn id="27" name="Dura" dataDxfId="58"/>
-    <tableColumn id="20" name="Def" dataDxfId="57"/>
-    <tableColumn id="21" name="Mag" dataDxfId="56"/>
-    <tableColumn id="29" name="Spd" dataDxfId="55"/>
-    <tableColumn id="30" name="Hit" dataDxfId="54"/>
-    <tableColumn id="19" name="Dhit" dataDxfId="53"/>
-    <tableColumn id="12" name="Crt" dataDxfId="52"/>
-    <tableColumn id="11" name="Luk" dataDxfId="51"/>
-    <tableColumn id="32" name="Sum" dataDxfId="50">
+    <tableColumn id="15" name="Cost" dataDxfId="73"/>
+    <tableColumn id="8" name="AtkP" dataDxfId="72"/>
+    <tableColumn id="9" name="PArmor" dataDxfId="71"/>
+    <tableColumn id="17" name="MArmor" dataDxfId="70"/>
+    <tableColumn id="25" name="Modify" dataDxfId="69"/>
+    <tableColumn id="27" name="Dura" dataDxfId="68"/>
+    <tableColumn id="20" name="Def" dataDxfId="67"/>
+    <tableColumn id="21" name="Mag" dataDxfId="66"/>
+    <tableColumn id="29" name="Spd" dataDxfId="65"/>
+    <tableColumn id="30" name="Hit" dataDxfId="64"/>
+    <tableColumn id="19" name="Dhit" dataDxfId="63"/>
+    <tableColumn id="12" name="Crt" dataDxfId="62"/>
+    <tableColumn id="11" name="Luk" dataDxfId="61"/>
+    <tableColumn id="32" name="Sum" dataDxfId="60">
       <calculatedColumnFormula>J4+K4+L4-100+M4+ SUM(O4:U4)*5+IF(ISNUMBER(Z4),Z4,0)+Y4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Range" dataDxfId="49"/>
-    <tableColumn id="31" name="Mov" dataDxfId="48"/>
-    <tableColumn id="24" name="~SkillMark" dataDxfId="47"/>
-    <tableColumn id="33" name="~SkillMark2" dataDxfId="0">
+    <tableColumn id="10" name="Range" dataDxfId="59"/>
+    <tableColumn id="31" name="Mov" dataDxfId="58"/>
+    <tableColumn id="24" name="~SkillMark" dataDxfId="57"/>
+    <tableColumn id="33" name="~SkillMark2" dataDxfId="56">
       <calculatedColumnFormula>IF(ISBLANK(AA4),0, LOOKUP(AA4,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="SkillId" dataDxfId="46"/>
-    <tableColumn id="14" name="Percent" dataDxfId="45"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="44"/>
-    <tableColumn id="26" name="JobId" dataDxfId="43"/>
-    <tableColumn id="18" name="Icon" dataDxfId="42"/>
-    <tableColumn id="22" name="IsSpecial" dataDxfId="41"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="40"/>
+    <tableColumn id="13" name="SkillId" dataDxfId="55"/>
+    <tableColumn id="14" name="Percent" dataDxfId="54"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="53"/>
+    <tableColumn id="26" name="JobId" dataDxfId="52"/>
+    <tableColumn id="18" name="Icon" dataDxfId="51"/>
+    <tableColumn id="22" name="IsSpecial" dataDxfId="50"/>
+    <tableColumn id="28" name="IsHeroCard" dataDxfId="0"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AG4" totalsRowShown="0" dataDxfId="34" tableBorderDxfId="33">
-  <autoFilter ref="A3:AG4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表1_3" displayName="表1_3" ref="A3:AH4" totalsRowShown="0" dataDxfId="48" tableBorderDxfId="47">
+  <autoFilter ref="A3:AH4"/>
   <sortState ref="A4:W130">
     <sortCondition ref="A3:A130"/>
   </sortState>
-  <tableColumns count="33">
-    <tableColumn id="1" name="Id" dataDxfId="32"/>
-    <tableColumn id="2" name="Name" dataDxfId="31"/>
-    <tableColumn id="3" name="Ename" dataDxfId="30"/>
-    <tableColumn id="4" name="Remark" dataDxfId="29"/>
-    <tableColumn id="5" name="Star" dataDxfId="28"/>
-    <tableColumn id="6" name="Type" dataDxfId="27"/>
-    <tableColumn id="7" name="Attr" dataDxfId="26"/>
-    <tableColumn id="34" name="Quality" dataDxfId="25">
+  <tableColumns count="34">
+    <tableColumn id="1" name="Id" dataDxfId="46"/>
+    <tableColumn id="2" name="Name" dataDxfId="45"/>
+    <tableColumn id="3" name="Ename" dataDxfId="44"/>
+    <tableColumn id="4" name="Remark" dataDxfId="43"/>
+    <tableColumn id="5" name="Star" dataDxfId="42"/>
+    <tableColumn id="6" name="Type" dataDxfId="41"/>
+    <tableColumn id="7" name="Attr" dataDxfId="40"/>
+    <tableColumn id="34" name="Quality" dataDxfId="39">
       <calculatedColumnFormula>IF(AND(V4&gt;=13,V4&lt;=16),5,IF(AND(V4&gt;=9,V4&lt;=12),4,IF(AND(V4&gt;=5,V4&lt;=8),3,IF(AND(V4&gt;=1,V4&lt;=4),2,IF(AND(V4&gt;=-3,V4&lt;=0),1,IF(AND(V4&gt;=-5,V4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Cost" dataDxfId="24"/>
-    <tableColumn id="8" name="AtkP" dataDxfId="23"/>
-    <tableColumn id="9" name="PArmor" dataDxfId="22"/>
-    <tableColumn id="17" name="MArmor" dataDxfId="21"/>
-    <tableColumn id="25" name="Modify" dataDxfId="20"/>
-    <tableColumn id="31" name="Dura" dataDxfId="19"/>
-    <tableColumn id="11" name="Def" dataDxfId="18"/>
-    <tableColumn id="21" name="Mag" dataDxfId="17"/>
-    <tableColumn id="29" name="Spd" dataDxfId="16"/>
-    <tableColumn id="30" name="Hit" dataDxfId="15"/>
-    <tableColumn id="20" name="Dhit" dataDxfId="14"/>
-    <tableColumn id="19" name="Crt" dataDxfId="13"/>
-    <tableColumn id="12" name="Luk" dataDxfId="12"/>
-    <tableColumn id="32" name="Sum" dataDxfId="11">
+    <tableColumn id="15" name="Cost" dataDxfId="38"/>
+    <tableColumn id="8" name="AtkP" dataDxfId="37"/>
+    <tableColumn id="9" name="PArmor" dataDxfId="36"/>
+    <tableColumn id="17" name="MArmor" dataDxfId="35"/>
+    <tableColumn id="25" name="Modify" dataDxfId="34"/>
+    <tableColumn id="31" name="Dura" dataDxfId="33"/>
+    <tableColumn id="11" name="Def" dataDxfId="32"/>
+    <tableColumn id="21" name="Mag" dataDxfId="31"/>
+    <tableColumn id="29" name="Spd" dataDxfId="30"/>
+    <tableColumn id="30" name="Hit" dataDxfId="29"/>
+    <tableColumn id="20" name="Dhit" dataDxfId="28"/>
+    <tableColumn id="19" name="Crt" dataDxfId="27"/>
+    <tableColumn id="12" name="Luk" dataDxfId="26"/>
+    <tableColumn id="32" name="Sum" dataDxfId="25">
       <calculatedColumnFormula>J4+K4+L4-100+M4+ SUM(O4:U4)*5+IF(ISNUMBER(Z4),Z4,0)+Y4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Range" dataDxfId="10"/>
-    <tableColumn id="27" name="Mov" dataDxfId="9"/>
-    <tableColumn id="24" name="~SkillMark" dataDxfId="8"/>
-    <tableColumn id="33" name="~SkillMark2" dataDxfId="7">
+    <tableColumn id="10" name="Range" dataDxfId="24"/>
+    <tableColumn id="27" name="Mov" dataDxfId="23"/>
+    <tableColumn id="24" name="~SkillMark" dataDxfId="22"/>
+    <tableColumn id="33" name="~SkillMark2" dataDxfId="21">
       <calculatedColumnFormula>IF(ISBLANK(AA4),0, LOOKUP(AA4,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="SkillId" dataDxfId="6"/>
-    <tableColumn id="14" name="Percent" dataDxfId="5"/>
-    <tableColumn id="16" name="Arrow" dataDxfId="4"/>
+    <tableColumn id="13" name="SkillId" dataDxfId="20"/>
+    <tableColumn id="14" name="Percent" dataDxfId="19"/>
+    <tableColumn id="16" name="Arrow" dataDxfId="18"/>
     <tableColumn id="26" name="JobId"/>
-    <tableColumn id="18" name="Icon" dataDxfId="3"/>
-    <tableColumn id="22" name="IsSpecial" dataDxfId="2"/>
-    <tableColumn id="23" name="IsNew" dataDxfId="1"/>
+    <tableColumn id="18" name="Icon" dataDxfId="17"/>
+    <tableColumn id="22" name="IsSpecial" dataDxfId="16"/>
+    <tableColumn id="28" name="IsHeroCard" dataDxfId="14"/>
+    <tableColumn id="23" name="IsNew" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5687,7 +5792,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -6000,13 +6105,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG133"/>
+  <dimension ref="A1:AH133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="C109" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M25" sqref="M25"/>
+      <selection pane="bottomRight" activeCell="AG1" sqref="AG1:AG3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6023,11 +6128,11 @@
     <col min="28" max="28" width="7.125" customWidth="1"/>
     <col min="29" max="30" width="9" customWidth="1"/>
     <col min="31" max="31" width="7.375" customWidth="1"/>
-    <col min="32" max="33" width="4.375" customWidth="1"/>
-    <col min="36" max="36" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="34" width="4.375" customWidth="1"/>
+    <col min="37" max="37" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="69" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:34" ht="69" x14ac:dyDescent="0.15">
       <c r="A1" s="19" t="s">
         <v>241</v>
       </c>
@@ -6037,7 +6142,7 @@
       <c r="C1" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="27" t="s">
         <v>295</v>
       </c>
       <c r="E1" s="20" t="s">
@@ -6049,7 +6154,7 @@
       <c r="G1" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="31" t="s">
         <v>332</v>
       </c>
       <c r="I1" s="20" t="s">
@@ -6070,25 +6175,25 @@
       <c r="N1" s="20" t="s">
         <v>292</v>
       </c>
-      <c r="O1" s="33" t="s">
+      <c r="O1" s="31" t="s">
         <v>310</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="P1" s="31" t="s">
         <v>311</v>
       </c>
-      <c r="Q1" s="33" t="s">
+      <c r="Q1" s="31" t="s">
         <v>312</v>
       </c>
-      <c r="R1" s="33" t="s">
+      <c r="R1" s="31" t="s">
         <v>313</v>
       </c>
-      <c r="S1" s="33" t="s">
+      <c r="S1" s="31" t="s">
         <v>314</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="T1" s="31" t="s">
         <v>315</v>
       </c>
-      <c r="U1" s="33" t="s">
+      <c r="U1" s="31" t="s">
         <v>316</v>
       </c>
       <c r="V1" s="21" t="s">
@@ -6115,7 +6220,7 @@
       <c r="AC1" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="AD1" s="38" t="s">
+      <c r="AD1" s="36" t="s">
         <v>343</v>
       </c>
       <c r="AE1" s="22" t="s">
@@ -6124,11 +6229,14 @@
       <c r="AF1" s="23" t="s">
         <v>286</v>
       </c>
-      <c r="AG1" s="27" t="s">
+      <c r="AG1" s="23" t="s">
+        <v>394</v>
+      </c>
+      <c r="AH1" s="23" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>110</v>
       </c>
@@ -6138,7 +6246,7 @@
       <c r="C2" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="28" t="s">
         <v>111</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -6216,20 +6324,23 @@
       <c r="AC2" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="AD2" s="39" t="s">
+      <c r="AD2" s="37" t="s">
         <v>344</v>
       </c>
       <c r="AE2" s="3" t="s">
         <v>111</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="AG2" s="28" t="s">
-        <v>252</v>
+        <v>110</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -6251,7 +6362,7 @@
       <c r="G3" t="s">
         <v>116</v>
       </c>
-      <c r="H3" s="34" t="s">
+      <c r="H3" s="32" t="s">
         <v>333</v>
       </c>
       <c r="I3" t="s">
@@ -6272,25 +6383,25 @@
       <c r="N3" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="O3" s="34" t="s">
+      <c r="O3" s="32" t="s">
         <v>326</v>
       </c>
-      <c r="P3" s="34" t="s">
+      <c r="P3" s="32" t="s">
         <v>319</v>
       </c>
-      <c r="Q3" s="34" t="s">
+      <c r="Q3" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="R3" s="34" t="s">
+      <c r="R3" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="S3" s="34" t="s">
+      <c r="S3" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="T3" s="34" t="s">
+      <c r="T3" s="32" t="s">
         <v>323</v>
       </c>
-      <c r="U3" s="34" t="s">
+      <c r="U3" s="32" t="s">
         <v>324</v>
       </c>
       <c r="V3" s="12" t="s">
@@ -6317,7 +6428,7 @@
       <c r="AC3" t="s">
         <v>119</v>
       </c>
-      <c r="AD3" s="40" t="s">
+      <c r="AD3" s="38" t="s">
         <v>345</v>
       </c>
       <c r="AE3" t="s">
@@ -6327,10 +6438,13 @@
         <v>287</v>
       </c>
       <c r="AG3" s="24" t="s">
+        <v>395</v>
+      </c>
+      <c r="AH3" s="24" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>52000001</v>
       </c>
@@ -6424,11 +6538,14 @@
       <c r="AF4" s="26">
         <v>0</v>
       </c>
-      <c r="AG4" s="25">
+      <c r="AG4" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>52000002</v>
       </c>
@@ -6522,11 +6639,14 @@
       <c r="AF5" s="26">
         <v>0</v>
       </c>
-      <c r="AG5" s="25">
+      <c r="AG5" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>52000003</v>
       </c>
@@ -6620,11 +6740,14 @@
       <c r="AF6" s="26">
         <v>0</v>
       </c>
-      <c r="AG6" s="25">
+      <c r="AG6" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>52000004</v>
       </c>
@@ -6718,11 +6841,14 @@
       <c r="AF7" s="26">
         <v>0</v>
       </c>
-      <c r="AG7" s="25">
+      <c r="AG7" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>52000005</v>
       </c>
@@ -6816,11 +6942,14 @@
       <c r="AF8" s="26">
         <v>0</v>
       </c>
-      <c r="AG8" s="25">
+      <c r="AG8" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>52000006</v>
       </c>
@@ -6914,11 +7043,14 @@
       <c r="AF9" s="26">
         <v>0</v>
       </c>
-      <c r="AG9" s="25">
+      <c r="AG9" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>52000007</v>
       </c>
@@ -7012,11 +7144,14 @@
       <c r="AF10" s="26">
         <v>0</v>
       </c>
-      <c r="AG10" s="25">
+      <c r="AG10" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>52000008</v>
       </c>
@@ -7110,11 +7245,14 @@
       <c r="AF11" s="26">
         <v>0</v>
       </c>
-      <c r="AG11" s="25">
+      <c r="AG11" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>52000009</v>
       </c>
@@ -7206,11 +7344,14 @@
       <c r="AF12" s="26">
         <v>0</v>
       </c>
-      <c r="AG12" s="25">
+      <c r="AG12" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>52000010</v>
       </c>
@@ -7308,11 +7449,14 @@
       <c r="AF13" s="26">
         <v>0</v>
       </c>
-      <c r="AG13" s="25">
+      <c r="AG13" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>52000011</v>
       </c>
@@ -7410,11 +7554,14 @@
       <c r="AF14" s="26">
         <v>0</v>
       </c>
-      <c r="AG14" s="25">
+      <c r="AG14" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>52000012</v>
       </c>
@@ -7512,11 +7659,14 @@
       <c r="AF15" s="26">
         <v>0</v>
       </c>
-      <c r="AG15" s="25">
+      <c r="AG15" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>52000013</v>
       </c>
@@ -7614,11 +7764,14 @@
       <c r="AF16" s="26">
         <v>0</v>
       </c>
-      <c r="AG16" s="25">
+      <c r="AG16" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>52000014</v>
       </c>
@@ -7716,11 +7869,14 @@
       <c r="AF17" s="26">
         <v>0</v>
       </c>
-      <c r="AG17" s="25">
+      <c r="AG17" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>52000015</v>
       </c>
@@ -7818,11 +7974,14 @@
       <c r="AF18" s="26">
         <v>0</v>
       </c>
-      <c r="AG18" s="25">
+      <c r="AG18" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>52000016</v>
       </c>
@@ -7920,11 +8079,14 @@
       <c r="AF19" s="26">
         <v>0</v>
       </c>
-      <c r="AG19" s="25">
+      <c r="AG19" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>52000017</v>
       </c>
@@ -8024,11 +8186,14 @@
       <c r="AF20" s="26">
         <v>0</v>
       </c>
-      <c r="AG20" s="25">
+      <c r="AG20" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>52000018</v>
       </c>
@@ -8122,11 +8287,14 @@
       <c r="AF21" s="26">
         <v>0</v>
       </c>
-      <c r="AG21" s="25">
+      <c r="AG21" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH21" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>52000019</v>
       </c>
@@ -8220,11 +8388,14 @@
       <c r="AF22" s="26">
         <v>0</v>
       </c>
-      <c r="AG22" s="25">
+      <c r="AG22" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH22" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>52000020</v>
       </c>
@@ -8318,11 +8489,14 @@
       <c r="AF23" s="26">
         <v>0</v>
       </c>
-      <c r="AG23" s="25">
+      <c r="AG23" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH23" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>52000021</v>
       </c>
@@ -8416,11 +8590,14 @@
       <c r="AF24" s="26">
         <v>0</v>
       </c>
-      <c r="AG24" s="25">
+      <c r="AG24" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH24" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>52000022</v>
       </c>
@@ -8514,11 +8691,14 @@
       <c r="AF25" s="26">
         <v>0</v>
       </c>
-      <c r="AG25" s="25">
+      <c r="AG25" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH25" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>52000023</v>
       </c>
@@ -8614,11 +8794,14 @@
       <c r="AF26" s="26">
         <v>0</v>
       </c>
-      <c r="AG26" s="25">
+      <c r="AG26" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>52000024</v>
       </c>
@@ -8718,11 +8901,14 @@
       <c r="AF27" s="26">
         <v>0</v>
       </c>
-      <c r="AG27" s="25">
+      <c r="AG27" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH27" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>52000025</v>
       </c>
@@ -8820,11 +9006,14 @@
       <c r="AF28" s="26">
         <v>0</v>
       </c>
-      <c r="AG28" s="25">
+      <c r="AG28" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH28" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>52000026</v>
       </c>
@@ -8922,11 +9111,14 @@
       <c r="AF29" s="26">
         <v>0</v>
       </c>
-      <c r="AG29" s="25">
+      <c r="AG29" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH29" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>52000027</v>
       </c>
@@ -9024,11 +9216,14 @@
       <c r="AF30" s="26">
         <v>0</v>
       </c>
-      <c r="AG30" s="25">
+      <c r="AG30" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH30" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>52000028</v>
       </c>
@@ -9126,11 +9321,14 @@
       <c r="AF31" s="26">
         <v>0</v>
       </c>
-      <c r="AG31" s="25">
+      <c r="AG31" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH31" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>52000029</v>
       </c>
@@ -9228,11 +9426,14 @@
       <c r="AF32" s="26">
         <v>0</v>
       </c>
-      <c r="AG32" s="25">
+      <c r="AG32" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH32" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>52000030</v>
       </c>
@@ -9330,11 +9531,14 @@
       <c r="AF33" s="26">
         <v>0</v>
       </c>
-      <c r="AG33" s="25">
+      <c r="AG33" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH33" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>52000031</v>
       </c>
@@ -9432,11 +9636,14 @@
       <c r="AF34" s="26">
         <v>0</v>
       </c>
-      <c r="AG34" s="25">
+      <c r="AG34" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH34" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>52000032</v>
       </c>
@@ -9536,11 +9743,14 @@
       <c r="AF35" s="26">
         <v>0</v>
       </c>
-      <c r="AG35" s="25">
+      <c r="AG35" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH35" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>52000033</v>
       </c>
@@ -9632,11 +9842,14 @@
       <c r="AF36" s="26">
         <v>0</v>
       </c>
-      <c r="AG36" s="25">
+      <c r="AG36" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH36" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>52000034</v>
       </c>
@@ -9730,11 +9943,14 @@
       <c r="AF37" s="26">
         <v>0</v>
       </c>
-      <c r="AG37" s="25">
+      <c r="AG37" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH37" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>52000035</v>
       </c>
@@ -9828,11 +10044,14 @@
       <c r="AF38" s="26">
         <v>0</v>
       </c>
-      <c r="AG38" s="25">
+      <c r="AG38" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH38" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>52000036</v>
       </c>
@@ -9924,11 +10143,14 @@
       <c r="AF39" s="26">
         <v>0</v>
       </c>
-      <c r="AG39" s="25">
+      <c r="AG39" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH39" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>52000037</v>
       </c>
@@ -10028,11 +10250,14 @@
       <c r="AF40" s="26">
         <v>0</v>
       </c>
-      <c r="AG40" s="25">
+      <c r="AG40" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH40" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>52000038</v>
       </c>
@@ -10132,11 +10357,14 @@
       <c r="AF41" s="26">
         <v>0</v>
       </c>
-      <c r="AG41" s="25">
+      <c r="AG41" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH41" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>52000039</v>
       </c>
@@ -10230,11 +10458,14 @@
       <c r="AF42" s="26">
         <v>0</v>
       </c>
-      <c r="AG42" s="25">
+      <c r="AG42" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH42" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>52000040</v>
       </c>
@@ -10328,11 +10559,14 @@
       <c r="AF43" s="26">
         <v>0</v>
       </c>
-      <c r="AG43" s="25">
+      <c r="AG43" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH43" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>52000041</v>
       </c>
@@ -10424,11 +10658,14 @@
       <c r="AF44" s="26">
         <v>0</v>
       </c>
-      <c r="AG44" s="25">
+      <c r="AG44" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH44" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>52000042</v>
       </c>
@@ -10524,11 +10761,14 @@
       <c r="AF45" s="26">
         <v>0</v>
       </c>
-      <c r="AG45" s="25">
+      <c r="AG45" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH45" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>52000043</v>
       </c>
@@ -10626,11 +10866,14 @@
       <c r="AF46" s="26">
         <v>0</v>
       </c>
-      <c r="AG46" s="25">
+      <c r="AG46" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH46" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>52000044</v>
       </c>
@@ -10724,11 +10967,14 @@
       <c r="AF47" s="26">
         <v>0</v>
       </c>
-      <c r="AG47" s="25">
+      <c r="AG47" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH47" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>52000045</v>
       </c>
@@ -10824,11 +11070,14 @@
       <c r="AF48" s="26">
         <v>0</v>
       </c>
-      <c r="AG48" s="25">
+      <c r="AG48" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH48" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>52000046</v>
       </c>
@@ -10920,11 +11169,14 @@
       <c r="AF49" s="26">
         <v>0</v>
       </c>
-      <c r="AG49" s="25">
+      <c r="AG49" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH49" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>52000047</v>
       </c>
@@ -11016,11 +11268,14 @@
       <c r="AF50" s="26">
         <v>0</v>
       </c>
-      <c r="AG50" s="25">
+      <c r="AG50" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH50" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>52000048</v>
       </c>
@@ -11118,11 +11373,14 @@
       <c r="AF51" s="26">
         <v>0</v>
       </c>
-      <c r="AG51" s="25">
+      <c r="AG51" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH51" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>52000049</v>
       </c>
@@ -11214,11 +11472,14 @@
       <c r="AF52" s="26">
         <v>0</v>
       </c>
-      <c r="AG52" s="25">
+      <c r="AG52" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH52" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>52000050</v>
       </c>
@@ -11310,11 +11571,14 @@
       <c r="AF53" s="26">
         <v>0</v>
       </c>
-      <c r="AG53" s="25">
+      <c r="AG53" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH53" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>52000051</v>
       </c>
@@ -11408,11 +11672,14 @@
       <c r="AF54" s="26">
         <v>0</v>
       </c>
-      <c r="AG54" s="25">
+      <c r="AG54" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH54" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>52000052</v>
       </c>
@@ -11506,11 +11773,14 @@
       <c r="AF55" s="26">
         <v>0</v>
       </c>
-      <c r="AG55" s="25">
+      <c r="AG55" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH55" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>52000053</v>
       </c>
@@ -11604,11 +11874,14 @@
       <c r="AF56" s="26">
         <v>0</v>
       </c>
-      <c r="AG56" s="25">
+      <c r="AG56" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH56" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>52000054</v>
       </c>
@@ -11700,11 +11973,14 @@
       <c r="AF57" s="26">
         <v>0</v>
       </c>
-      <c r="AG57" s="25">
+      <c r="AG57" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH57" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A58">
         <v>52000055</v>
       </c>
@@ -11798,11 +12074,14 @@
       <c r="AF58" s="26">
         <v>0</v>
       </c>
-      <c r="AG58" s="25">
+      <c r="AG58" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH58" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>52000056</v>
       </c>
@@ -11882,7 +12161,7 @@
         <f>IF(ISBLANK(AA59),0, LOOKUP(AA59,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB59/100)</f>
         <v>0</v>
       </c>
-      <c r="AA59" s="32"/>
+      <c r="AA59" s="30"/>
       <c r="AB59" s="4"/>
       <c r="AC59" s="4" t="s">
         <v>5</v>
@@ -11896,11 +12175,14 @@
       <c r="AF59" s="26">
         <v>0</v>
       </c>
-      <c r="AG59" s="25">
+      <c r="AG59" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH59" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>52000057</v>
       </c>
@@ -11980,7 +12262,7 @@
         <f>IF(ISBLANK(AA60),0, LOOKUP(AA60,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB60/100)</f>
         <v>0</v>
       </c>
-      <c r="AA60" s="32"/>
+      <c r="AA60" s="30"/>
       <c r="AB60" s="4"/>
       <c r="AC60" s="4" t="s">
         <v>5</v>
@@ -11992,11 +12274,14 @@
       <c r="AF60" s="26">
         <v>0</v>
       </c>
-      <c r="AG60" s="25">
+      <c r="AG60" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH60" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>52000058</v>
       </c>
@@ -12078,7 +12363,7 @@
         <f>IF(ISBLANK(AA61),0, LOOKUP(AA61,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB61/100)</f>
         <v>12</v>
       </c>
-      <c r="AA61" s="37">
+      <c r="AA61" s="35">
         <v>55900018</v>
       </c>
       <c r="AB61" s="4">
@@ -12094,11 +12379,14 @@
       <c r="AF61" s="26">
         <v>0</v>
       </c>
-      <c r="AG61" s="25">
+      <c r="AG61" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH61" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>52000059</v>
       </c>
@@ -12180,7 +12468,7 @@
         <f>IF(ISBLANK(AA62),0, LOOKUP(AA62,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB62/100)</f>
         <v>25</v>
       </c>
-      <c r="AA62" s="37">
+      <c r="AA62" s="35">
         <v>55110003</v>
       </c>
       <c r="AB62" s="4">
@@ -12198,11 +12486,14 @@
       <c r="AF62" s="26">
         <v>0</v>
       </c>
-      <c r="AG62" s="25">
+      <c r="AG62" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH62" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>52000060</v>
       </c>
@@ -12282,7 +12573,7 @@
         <f>IF(ISBLANK(AA63),0, LOOKUP(AA63,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB63/100)</f>
         <v>10</v>
       </c>
-      <c r="AA63" s="37">
+      <c r="AA63" s="35">
         <v>55100001</v>
       </c>
       <c r="AB63" s="4">
@@ -12298,11 +12589,14 @@
       <c r="AF63" s="26">
         <v>0</v>
       </c>
-      <c r="AG63" s="25">
+      <c r="AG63" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH63" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>52000061</v>
       </c>
@@ -12398,11 +12692,14 @@
       <c r="AF64" s="26">
         <v>0</v>
       </c>
-      <c r="AG64" s="25">
+      <c r="AG64" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH64" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>52000062</v>
       </c>
@@ -12500,11 +12797,14 @@
       <c r="AF65" s="26">
         <v>0</v>
       </c>
-      <c r="AG65" s="25">
+      <c r="AG65" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH65" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A66">
         <v>52000063</v>
       </c>
@@ -12586,7 +12886,7 @@
         <f>IF(ISBLANK(AA66),0, LOOKUP(AA66,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB66/100)</f>
         <v>0</v>
       </c>
-      <c r="AA66" s="37"/>
+      <c r="AA66" s="35"/>
       <c r="AB66" s="4"/>
       <c r="AC66" s="4" t="s">
         <v>5</v>
@@ -12598,11 +12898,14 @@
       <c r="AF66" s="26">
         <v>0</v>
       </c>
-      <c r="AG66" s="25">
+      <c r="AG66" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH66" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>52000064</v>
       </c>
@@ -12693,11 +12996,14 @@
       <c r="AF67" s="26">
         <v>0</v>
       </c>
-      <c r="AG67" s="25">
+      <c r="AG67" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH67" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>52000065</v>
       </c>
@@ -12777,7 +13083,7 @@
         <f>IF(ISBLANK(AA68),0, LOOKUP(AA68,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB68/100)</f>
         <v>0</v>
       </c>
-      <c r="AA68" s="37"/>
+      <c r="AA68" s="35"/>
       <c r="AB68" s="4"/>
       <c r="AC68" s="4" t="s">
         <v>37</v>
@@ -12791,11 +13097,14 @@
       <c r="AF68" s="26">
         <v>0</v>
       </c>
-      <c r="AG68" s="25">
+      <c r="AG68" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH68" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>52000066</v>
       </c>
@@ -12875,7 +13184,7 @@
         <f>IF(ISBLANK(AA69),0, LOOKUP(AA69,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB69/100)</f>
         <v>0</v>
       </c>
-      <c r="AA69" s="32"/>
+      <c r="AA69" s="30"/>
       <c r="AB69" s="4"/>
       <c r="AC69" s="4" t="s">
         <v>1</v>
@@ -12887,11 +13196,14 @@
       <c r="AF69" s="26">
         <v>0</v>
       </c>
-      <c r="AG69" s="25">
+      <c r="AG69" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH69" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A70">
         <v>52000067</v>
       </c>
@@ -12971,7 +13283,7 @@
         <f>IF(ISBLANK(AA70),0, LOOKUP(AA70,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB70/100)</f>
         <v>0</v>
       </c>
-      <c r="AA70" s="32"/>
+      <c r="AA70" s="30"/>
       <c r="AB70" s="4"/>
       <c r="AC70" s="4" t="s">
         <v>3</v>
@@ -12983,11 +13295,14 @@
       <c r="AF70" s="26">
         <v>0</v>
       </c>
-      <c r="AG70" s="25">
+      <c r="AG70" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH70" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>52000068</v>
       </c>
@@ -13067,7 +13382,7 @@
         <f>IF(ISBLANK(AA71),0, LOOKUP(AA71,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB71/100)</f>
         <v>0</v>
       </c>
-      <c r="AA71" s="32"/>
+      <c r="AA71" s="30"/>
       <c r="AB71" s="4"/>
       <c r="AC71" s="4" t="s">
         <v>5</v>
@@ -13079,11 +13394,14 @@
       <c r="AF71" s="26">
         <v>0</v>
       </c>
-      <c r="AG71" s="25">
+      <c r="AG71" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH71" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>52000069</v>
       </c>
@@ -13174,11 +13492,14 @@
       <c r="AF72" s="26">
         <v>0</v>
       </c>
-      <c r="AG72" s="25">
+      <c r="AG72" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH72" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>52000070</v>
       </c>
@@ -13258,7 +13579,7 @@
         <f>IF(ISBLANK(AA73),0, LOOKUP(AA73,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB73/100)</f>
         <v>60</v>
       </c>
-      <c r="AA73" s="37">
+      <c r="AA73" s="35">
         <v>55110013</v>
       </c>
       <c r="AB73" s="4">
@@ -13274,11 +13595,14 @@
       <c r="AF73" s="26">
         <v>0</v>
       </c>
-      <c r="AG73" s="25">
+      <c r="AG73" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH73" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A74">
         <v>52000071</v>
       </c>
@@ -13360,7 +13684,7 @@
         <f>IF(ISBLANK(AA74),0, LOOKUP(AA74,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB74/100)</f>
         <v>5</v>
       </c>
-      <c r="AA74" s="37">
+      <c r="AA74" s="35">
         <v>55500001</v>
       </c>
       <c r="AB74" s="4">
@@ -13376,11 +13700,14 @@
       <c r="AF74" s="26">
         <v>0</v>
       </c>
-      <c r="AG74" s="25">
+      <c r="AG74" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH74" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A75">
         <v>52000072</v>
       </c>
@@ -13462,7 +13789,7 @@
         <f>IF(ISBLANK(AA75),0, LOOKUP(AA75,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB75/100)</f>
         <v>5</v>
       </c>
-      <c r="AA75" s="37">
+      <c r="AA75" s="35">
         <v>55500003</v>
       </c>
       <c r="AB75" s="4">
@@ -13478,11 +13805,14 @@
       <c r="AF75" s="26">
         <v>0</v>
       </c>
-      <c r="AG75" s="25">
+      <c r="AG75" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH75" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A76">
         <v>52000073</v>
       </c>
@@ -13578,11 +13908,14 @@
       <c r="AF76" s="26">
         <v>0</v>
       </c>
-      <c r="AG76" s="25">
+      <c r="AG76" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH76" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A77">
         <v>52000074</v>
       </c>
@@ -13664,7 +13997,7 @@
         <f>IF(ISBLANK(AA77),0, LOOKUP(AA77,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB77/100)</f>
         <v>5</v>
       </c>
-      <c r="AA77" s="37">
+      <c r="AA77" s="35">
         <v>55500014</v>
       </c>
       <c r="AB77" s="4">
@@ -13680,11 +14013,14 @@
       <c r="AF77" s="26">
         <v>0</v>
       </c>
-      <c r="AG77" s="25">
+      <c r="AG77" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH77" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A78">
         <v>52000075</v>
       </c>
@@ -13766,7 +14102,7 @@
         <f>IF(ISBLANK(AA78),0, LOOKUP(AA78,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB78/100)</f>
         <v>5</v>
       </c>
-      <c r="AA78" s="37">
+      <c r="AA78" s="35">
         <v>55500008</v>
       </c>
       <c r="AB78" s="4">
@@ -13782,11 +14118,14 @@
       <c r="AF78" s="26">
         <v>0</v>
       </c>
-      <c r="AG78" s="25">
+      <c r="AG78" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH78" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A79">
         <v>52000076</v>
       </c>
@@ -13868,7 +14207,7 @@
         <f>IF(ISBLANK(AA79),0, LOOKUP(AA79,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB79/100)</f>
         <v>5</v>
       </c>
-      <c r="AA79" s="37">
+      <c r="AA79" s="35">
         <v>55500005</v>
       </c>
       <c r="AB79" s="4">
@@ -13884,11 +14223,14 @@
       <c r="AF79" s="26">
         <v>0</v>
       </c>
-      <c r="AG79" s="25">
+      <c r="AG79" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH79" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A80">
         <v>52000077</v>
       </c>
@@ -13970,7 +14312,7 @@
         <f>IF(ISBLANK(AA80),0, LOOKUP(AA80,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB80/100)</f>
         <v>5</v>
       </c>
-      <c r="AA80" s="37">
+      <c r="AA80" s="35">
         <v>55500010</v>
       </c>
       <c r="AB80" s="4">
@@ -13986,11 +14328,14 @@
       <c r="AF80" s="26">
         <v>0</v>
       </c>
-      <c r="AG80" s="25">
+      <c r="AG80" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH80" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A81">
         <v>52000078</v>
       </c>
@@ -14072,7 +14417,7 @@
         <f>IF(ISBLANK(AA81),0, LOOKUP(AA81,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB81/100)</f>
         <v>5</v>
       </c>
-      <c r="AA81" s="37">
+      <c r="AA81" s="35">
         <v>55500009</v>
       </c>
       <c r="AB81" s="4">
@@ -14088,11 +14433,14 @@
       <c r="AF81" s="26">
         <v>0</v>
       </c>
-      <c r="AG81" s="25">
+      <c r="AG81" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH81" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A82">
         <v>52000079</v>
       </c>
@@ -14174,7 +14522,7 @@
         <f>IF(ISBLANK(AA82),0, LOOKUP(AA82,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB82/100)</f>
         <v>5</v>
       </c>
-      <c r="AA82" s="37">
+      <c r="AA82" s="35">
         <v>55500011</v>
       </c>
       <c r="AB82" s="4">
@@ -14190,11 +14538,14 @@
       <c r="AF82" s="26">
         <v>0</v>
       </c>
-      <c r="AG82" s="25">
+      <c r="AG82" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH82" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A83">
         <v>52000080</v>
       </c>
@@ -14276,7 +14627,7 @@
         <f>IF(ISBLANK(AA83),0, LOOKUP(AA83,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB83/100)</f>
         <v>5</v>
       </c>
-      <c r="AA83" s="37">
+      <c r="AA83" s="35">
         <v>55500001</v>
       </c>
       <c r="AB83" s="4">
@@ -14292,11 +14643,14 @@
       <c r="AF83" s="26">
         <v>0</v>
       </c>
-      <c r="AG83" s="25">
+      <c r="AG83" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH83" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A84">
         <v>52000081</v>
       </c>
@@ -14378,7 +14732,7 @@
         <f>IF(ISBLANK(AA84),0, LOOKUP(AA84,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB84/100)</f>
         <v>5</v>
       </c>
-      <c r="AA84" s="37">
+      <c r="AA84" s="35">
         <v>55500012</v>
       </c>
       <c r="AB84" s="4">
@@ -14394,11 +14748,14 @@
       <c r="AF84" s="26">
         <v>0</v>
       </c>
-      <c r="AG84" s="25">
+      <c r="AG84" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH84" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A85">
         <v>52000082</v>
       </c>
@@ -14478,7 +14835,7 @@
         <f>IF(ISBLANK(AA85),0, LOOKUP(AA85,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB85/100)</f>
         <v>0</v>
       </c>
-      <c r="AA85" s="32"/>
+      <c r="AA85" s="30"/>
       <c r="AB85" s="4"/>
       <c r="AC85" s="4" t="s">
         <v>305</v>
@@ -14490,11 +14847,14 @@
       <c r="AF85" s="26">
         <v>0</v>
       </c>
-      <c r="AG85" s="25">
+      <c r="AG85" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH85" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A86">
         <v>52000083</v>
       </c>
@@ -14574,7 +14934,7 @@
         <f>IF(ISBLANK(AA86),0, LOOKUP(AA86,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB86/100)</f>
         <v>0</v>
       </c>
-      <c r="AA86" s="32"/>
+      <c r="AA86" s="30"/>
       <c r="AB86" s="4"/>
       <c r="AC86" s="4" t="s">
         <v>28</v>
@@ -14588,11 +14948,14 @@
       <c r="AF86" s="26">
         <v>0</v>
       </c>
-      <c r="AG86" s="25">
+      <c r="AG86" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH86" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A87">
         <v>52000084</v>
       </c>
@@ -14672,7 +15035,7 @@
         <f>IF(ISBLANK(AA87),0, LOOKUP(AA87,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB87/100)</f>
         <v>0</v>
       </c>
-      <c r="AA87" s="32"/>
+      <c r="AA87" s="30"/>
       <c r="AB87" s="4"/>
       <c r="AC87" s="4" t="s">
         <v>30</v>
@@ -14686,11 +15049,14 @@
       <c r="AF87" s="26">
         <v>0</v>
       </c>
-      <c r="AG87" s="25">
+      <c r="AG87" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH87" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A88">
         <v>52000085</v>
       </c>
@@ -14770,7 +15136,7 @@
         <f>IF(ISBLANK(AA88),0, LOOKUP(AA88,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB88/100)</f>
         <v>0</v>
       </c>
-      <c r="AA88" s="32"/>
+      <c r="AA88" s="30"/>
       <c r="AB88" s="4"/>
       <c r="AC88" s="4" t="s">
         <v>307</v>
@@ -14782,11 +15148,14 @@
       <c r="AF88" s="26">
         <v>0</v>
       </c>
-      <c r="AG88" s="25">
+      <c r="AG88" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH88" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A89">
         <v>52000086</v>
       </c>
@@ -14868,7 +15237,7 @@
         <f>IF(ISBLANK(AA89),0, LOOKUP(AA89,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB89/100)</f>
         <v>20</v>
       </c>
-      <c r="AA89" s="32">
+      <c r="AA89" s="30">
         <v>55510009</v>
       </c>
       <c r="AB89" s="4">
@@ -14886,11 +15255,14 @@
       <c r="AF89" s="26">
         <v>0</v>
       </c>
-      <c r="AG89" s="25">
+      <c r="AG89" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH89" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A90">
         <v>52000087</v>
       </c>
@@ -14972,7 +15344,7 @@
         <f>IF(ISBLANK(AA90),0, LOOKUP(AA90,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB90/100)</f>
         <v>15</v>
       </c>
-      <c r="AA90" s="32">
+      <c r="AA90" s="30">
         <v>55510002</v>
       </c>
       <c r="AB90" s="4">
@@ -14990,11 +15362,14 @@
       <c r="AF90" s="26">
         <v>0</v>
       </c>
-      <c r="AG90" s="25">
+      <c r="AG90" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH90" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A91">
         <v>52000088</v>
       </c>
@@ -15074,7 +15449,7 @@
         <f>IF(ISBLANK(AA91),0, LOOKUP(AA91,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB91/100)</f>
         <v>0</v>
       </c>
-      <c r="AA91" s="32"/>
+      <c r="AA91" s="30"/>
       <c r="AB91" s="4"/>
       <c r="AC91" s="4" t="s">
         <v>303</v>
@@ -15088,11 +15463,14 @@
       <c r="AF91" s="26">
         <v>0</v>
       </c>
-      <c r="AG91" s="25">
+      <c r="AG91" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH91" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A92">
         <v>52000089</v>
       </c>
@@ -15172,7 +15550,7 @@
         <f>IF(ISBLANK(AA92),0, LOOKUP(AA92,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB92/100)</f>
         <v>0</v>
       </c>
-      <c r="AA92" s="32"/>
+      <c r="AA92" s="30"/>
       <c r="AB92" s="4"/>
       <c r="AC92" s="4" t="s">
         <v>306</v>
@@ -15186,11 +15564,14 @@
       <c r="AF92" s="26">
         <v>0</v>
       </c>
-      <c r="AG92" s="25">
+      <c r="AG92" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH92" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A93">
         <v>52000090</v>
       </c>
@@ -15270,7 +15651,7 @@
         <f>IF(ISBLANK(AA93),0, LOOKUP(AA93,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB93/100)</f>
         <v>0</v>
       </c>
-      <c r="AA93" s="32"/>
+      <c r="AA93" s="30"/>
       <c r="AB93" s="4"/>
       <c r="AC93" s="4" t="s">
         <v>85</v>
@@ -15284,11 +15665,14 @@
       <c r="AF93" s="26">
         <v>0</v>
       </c>
-      <c r="AG93" s="25">
+      <c r="AG93" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH93" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A94">
         <v>52000091</v>
       </c>
@@ -15368,7 +15752,7 @@
         <f>IF(ISBLANK(AA94),0, LOOKUP(AA94,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB94/100)</f>
         <v>35</v>
       </c>
-      <c r="AA94" s="37">
+      <c r="AA94" s="35">
         <v>55110014</v>
       </c>
       <c r="AB94" s="4">
@@ -15386,11 +15770,14 @@
       <c r="AF94" s="26">
         <v>0</v>
       </c>
-      <c r="AG94" s="25">
+      <c r="AG94" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH94" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A95">
         <v>52000092</v>
       </c>
@@ -15472,7 +15859,7 @@
         <f>IF(ISBLANK(AA95),0, LOOKUP(AA95,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB95/100)</f>
         <v>8.4</v>
       </c>
-      <c r="AA95" s="37">
+      <c r="AA95" s="35">
         <v>55510004</v>
       </c>
       <c r="AB95" s="4">
@@ -15490,11 +15877,14 @@
       <c r="AF95" s="26">
         <v>0</v>
       </c>
-      <c r="AG95" s="25">
+      <c r="AG95" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH95" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A96">
         <v>52000093</v>
       </c>
@@ -15574,7 +15964,7 @@
         <f>IF(ISBLANK(AA96),0, LOOKUP(AA96,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB96/100)</f>
         <v>0</v>
       </c>
-      <c r="AA96" s="32"/>
+      <c r="AA96" s="30"/>
       <c r="AB96" s="4"/>
       <c r="AC96" s="4" t="s">
         <v>3</v>
@@ -15588,11 +15978,14 @@
       <c r="AF96" s="26">
         <v>0</v>
       </c>
-      <c r="AG96" s="25">
+      <c r="AG96" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH96" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A97">
         <v>52000094</v>
       </c>
@@ -15672,7 +16065,7 @@
         <f>IF(ISBLANK(AA97),0, LOOKUP(AA97,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB97/100)</f>
         <v>0</v>
       </c>
-      <c r="AA97" s="32"/>
+      <c r="AA97" s="30"/>
       <c r="AB97" s="4"/>
       <c r="AC97" s="4" t="s">
         <v>3</v>
@@ -15686,11 +16079,14 @@
       <c r="AF97" s="26">
         <v>0</v>
       </c>
-      <c r="AG97" s="25">
+      <c r="AG97" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH97" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A98">
         <v>52000095</v>
       </c>
@@ -15770,7 +16166,7 @@
         <f>IF(ISBLANK(AA98),0, LOOKUP(AA98,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB98/100)</f>
         <v>12</v>
       </c>
-      <c r="AA98" s="37">
+      <c r="AA98" s="35">
         <v>55110009</v>
       </c>
       <c r="AB98" s="4">
@@ -15788,11 +16184,14 @@
       <c r="AF98" s="26">
         <v>0</v>
       </c>
-      <c r="AG98" s="25">
+      <c r="AG98" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH98" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A99">
         <v>52000096</v>
       </c>
@@ -15874,7 +16273,7 @@
         <f>IF(ISBLANK(AA99),0, LOOKUP(AA99,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB99/100)</f>
         <v>40</v>
       </c>
-      <c r="AA99" s="37">
+      <c r="AA99" s="35">
         <v>55200004</v>
       </c>
       <c r="AB99" s="4">
@@ -15892,11 +16291,14 @@
       <c r="AF99" s="26">
         <v>0</v>
       </c>
-      <c r="AG99" s="25">
+      <c r="AG99" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH99" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A100">
         <v>52000097</v>
       </c>
@@ -15976,7 +16378,7 @@
         <f>IF(ISBLANK(AA100),0, LOOKUP(AA100,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB100/100)</f>
         <v>20</v>
       </c>
-      <c r="AA100" s="37">
+      <c r="AA100" s="35">
         <v>55110010</v>
       </c>
       <c r="AB100" s="4">
@@ -15994,11 +16396,14 @@
       <c r="AF100" s="26">
         <v>0</v>
       </c>
-      <c r="AG100" s="25">
+      <c r="AG100" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH100" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A101">
         <v>52000098</v>
       </c>
@@ -16080,7 +16485,7 @@
         <f>IF(ISBLANK(AA101),0, LOOKUP(AA101,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB101/100)</f>
         <v>14.8</v>
       </c>
-      <c r="AA101" s="37">
+      <c r="AA101" s="35">
         <v>55510019</v>
       </c>
       <c r="AB101" s="4">
@@ -16096,11 +16501,14 @@
       <c r="AF101" s="26">
         <v>0</v>
       </c>
-      <c r="AG101" s="25">
+      <c r="AG101" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH101" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A102">
         <v>52000099</v>
       </c>
@@ -16180,7 +16588,7 @@
         <f>IF(ISBLANK(AA102),0, LOOKUP(AA102,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB102/100)</f>
         <v>0</v>
       </c>
-      <c r="AA102" s="37"/>
+      <c r="AA102" s="35"/>
       <c r="AB102" s="4"/>
       <c r="AC102" s="4" t="s">
         <v>5</v>
@@ -16192,11 +16600,14 @@
       <c r="AF102" s="26">
         <v>0</v>
       </c>
-      <c r="AG102" s="25">
+      <c r="AG102" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH102" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A103">
         <v>52000100</v>
       </c>
@@ -16278,7 +16689,7 @@
         <f>IF(ISBLANK(AA103),0, LOOKUP(AA103,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB103/100)</f>
         <v>49.5</v>
       </c>
-      <c r="AA103" s="37">
+      <c r="AA103" s="35">
         <v>55990105</v>
       </c>
       <c r="AB103" s="4">
@@ -16296,11 +16707,14 @@
       <c r="AF103" s="26">
         <v>0</v>
       </c>
-      <c r="AG103" s="25">
+      <c r="AG103" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH103" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A104">
         <v>52000101</v>
       </c>
@@ -16382,7 +16796,7 @@
         <f>IF(ISBLANK(AA104),0, LOOKUP(AA104,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB104/100)</f>
         <v>35</v>
       </c>
-      <c r="AA104" s="37">
+      <c r="AA104" s="35">
         <v>55990103</v>
       </c>
       <c r="AB104" s="4">
@@ -16398,11 +16812,14 @@
       <c r="AF104" s="26">
         <v>0</v>
       </c>
-      <c r="AG104" s="25">
+      <c r="AG104" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH104" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A105">
         <v>52000102</v>
       </c>
@@ -16484,7 +16901,7 @@
         <f>IF(ISBLANK(AA105),0, LOOKUP(AA105,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB105/100)</f>
         <v>20</v>
       </c>
-      <c r="AA105" s="37">
+      <c r="AA105" s="35">
         <v>55700004</v>
       </c>
       <c r="AB105" s="4">
@@ -16500,11 +16917,14 @@
       <c r="AF105" s="26">
         <v>0</v>
       </c>
-      <c r="AG105" s="25">
+      <c r="AG105" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH105" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A106">
         <v>52000103</v>
       </c>
@@ -16584,7 +17004,7 @@
         <f>IF(ISBLANK(AA106),0, LOOKUP(AA106,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB106/100)</f>
         <v>0</v>
       </c>
-      <c r="AA106" s="32"/>
+      <c r="AA106" s="30"/>
       <c r="AB106" s="4"/>
       <c r="AC106" s="4" t="s">
         <v>5</v>
@@ -16598,11 +17018,14 @@
       <c r="AF106" s="26">
         <v>0</v>
       </c>
-      <c r="AG106" s="25">
+      <c r="AG106" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH106" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A107">
         <v>52000104</v>
       </c>
@@ -16684,7 +17107,7 @@
         <f>IF(ISBLANK(AA107),0, LOOKUP(AA107,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB107/100)</f>
         <v>12</v>
       </c>
-      <c r="AA107" s="37">
+      <c r="AA107" s="35">
         <v>55510013</v>
       </c>
       <c r="AB107" s="4">
@@ -16702,11 +17125,14 @@
       <c r="AF107" s="26">
         <v>0</v>
       </c>
-      <c r="AG107" s="25">
+      <c r="AG107" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH107" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A108">
         <v>52000105</v>
       </c>
@@ -16786,7 +17212,7 @@
         <f>IF(ISBLANK(AA108),0, LOOKUP(AA108,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB108/100)</f>
         <v>15</v>
       </c>
-      <c r="AA108" s="37">
+      <c r="AA108" s="35">
         <v>55990101</v>
       </c>
       <c r="AB108" s="4">
@@ -16804,11 +17230,14 @@
       <c r="AF108" s="26">
         <v>0</v>
       </c>
-      <c r="AG108" s="25">
+      <c r="AG108" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH108" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A109">
         <v>52000106</v>
       </c>
@@ -16888,7 +17317,7 @@
         <f>IF(ISBLANK(AA109),0, LOOKUP(AA109,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB109/100)</f>
         <v>0</v>
       </c>
-      <c r="AA109" s="37"/>
+      <c r="AA109" s="35"/>
       <c r="AB109" s="4"/>
       <c r="AC109" s="4" t="s">
         <v>5</v>
@@ -16902,11 +17331,14 @@
       <c r="AF109" s="26">
         <v>0</v>
       </c>
-      <c r="AG109" s="25">
+      <c r="AG109" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH109" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A110">
         <v>52000107</v>
       </c>
@@ -17002,11 +17434,14 @@
       <c r="AF110" s="26">
         <v>0</v>
       </c>
-      <c r="AG110" s="25">
+      <c r="AG110" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH110" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A111">
         <v>52000108</v>
       </c>
@@ -17086,7 +17521,7 @@
         <f>IF(ISBLANK(AA111),0, LOOKUP(AA111,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB111/100)</f>
         <v>0</v>
       </c>
-      <c r="AA111" s="37"/>
+      <c r="AA111" s="35"/>
       <c r="AB111" s="4"/>
       <c r="AC111" s="4" t="s">
         <v>3</v>
@@ -17098,11 +17533,14 @@
       <c r="AF111" s="26">
         <v>0</v>
       </c>
-      <c r="AG111" s="25">
+      <c r="AG111" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH111" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A112">
         <v>52000109</v>
       </c>
@@ -17184,7 +17622,7 @@
         <f>IF(ISBLANK(AA112),0, LOOKUP(AA112,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB112/100)</f>
         <v>25</v>
       </c>
-      <c r="AA112" s="37">
+      <c r="AA112" s="35">
         <v>55510006</v>
       </c>
       <c r="AB112" s="4">
@@ -17200,11 +17638,14 @@
       <c r="AF112" s="26">
         <v>0</v>
       </c>
-      <c r="AG112" s="25">
+      <c r="AG112" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH112" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A113">
         <v>52000110</v>
       </c>
@@ -17284,7 +17725,7 @@
         <f>IF(ISBLANK(AA113),0, LOOKUP(AA113,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB113/100)</f>
         <v>15</v>
       </c>
-      <c r="AA113" s="37">
+      <c r="AA113" s="35">
         <v>55990101</v>
       </c>
       <c r="AB113" s="4">
@@ -17302,11 +17743,14 @@
       <c r="AF113" s="26">
         <v>0</v>
       </c>
-      <c r="AG113" s="25">
+      <c r="AG113" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH113" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A114">
         <v>52000111</v>
       </c>
@@ -17386,7 +17830,7 @@
         <f>IF(ISBLANK(AA114),0, LOOKUP(AA114,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB114/100)</f>
         <v>0</v>
       </c>
-      <c r="AA114" s="37"/>
+      <c r="AA114" s="35"/>
       <c r="AB114" s="4"/>
       <c r="AC114" s="4" t="s">
         <v>3</v>
@@ -17400,11 +17844,14 @@
       <c r="AF114" s="26">
         <v>0</v>
       </c>
-      <c r="AG114" s="25">
+      <c r="AG114" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH114" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A115">
         <v>52000112</v>
       </c>
@@ -17484,7 +17931,7 @@
         <f>IF(ISBLANK(AA115),0, LOOKUP(AA115,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB115/100)</f>
         <v>0</v>
       </c>
-      <c r="AA115" s="37"/>
+      <c r="AA115" s="35"/>
       <c r="AB115" s="4"/>
       <c r="AC115" s="4" t="s">
         <v>5</v>
@@ -17498,11 +17945,14 @@
       <c r="AF115" s="26">
         <v>0</v>
       </c>
-      <c r="AG115" s="25">
+      <c r="AG115" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH115" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A116">
         <v>52000113</v>
       </c>
@@ -17567,7 +18017,7 @@
       <c r="U116" s="8">
         <v>0</v>
       </c>
-      <c r="V116" s="36">
+      <c r="V116" s="34">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
@@ -17598,11 +18048,14 @@
       <c r="AF116" s="26">
         <v>0</v>
       </c>
-      <c r="AG116" s="25">
+      <c r="AG116" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH116" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A117">
         <v>52000114</v>
       </c>
@@ -17667,7 +18120,7 @@
       <c r="U117" s="8">
         <v>0</v>
       </c>
-      <c r="V117" s="36">
+      <c r="V117" s="34">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
@@ -17684,7 +18137,7 @@
         <f>IF(ISBLANK(AA117),0, LOOKUP(AA117,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB117/100)</f>
         <v>10</v>
       </c>
-      <c r="AA117" s="37">
+      <c r="AA117" s="35">
         <v>55510007</v>
       </c>
       <c r="AB117" s="4">
@@ -17700,11 +18153,14 @@
       <c r="AF117" s="26">
         <v>0</v>
       </c>
-      <c r="AG117" s="25">
+      <c r="AG117" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH117" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A118">
         <v>52000115</v>
       </c>
@@ -17784,7 +18240,7 @@
         <f>IF(ISBLANK(AA118),0, LOOKUP(AA118,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB118/100)</f>
         <v>30</v>
       </c>
-      <c r="AA118" s="37">
+      <c r="AA118" s="35">
         <v>55110012</v>
       </c>
       <c r="AB118" s="4">
@@ -17802,11 +18258,14 @@
       <c r="AF118" s="26">
         <v>0</v>
       </c>
-      <c r="AG118" s="25">
+      <c r="AG118" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH118" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A119">
         <v>52000116</v>
       </c>
@@ -17886,7 +18345,7 @@
         <f>IF(ISBLANK(AA119),0, LOOKUP(AA119,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB119/100)</f>
         <v>30</v>
       </c>
-      <c r="AA119" s="37">
+      <c r="AA119" s="35">
         <v>55610001</v>
       </c>
       <c r="AB119" s="4">
@@ -17902,11 +18361,14 @@
       <c r="AF119" s="26">
         <v>0</v>
       </c>
-      <c r="AG119" s="25">
+      <c r="AG119" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH119" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A120">
         <v>52000117</v>
       </c>
@@ -17988,7 +18450,7 @@
         <f>IF(ISBLANK(AA120),0, LOOKUP(AA120,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB120/100)</f>
         <v>50</v>
       </c>
-      <c r="AA120" s="37">
+      <c r="AA120" s="35">
         <v>55990104</v>
       </c>
       <c r="AB120" s="4">
@@ -18004,11 +18466,14 @@
       <c r="AF120" s="26">
         <v>0</v>
       </c>
-      <c r="AG120" s="25">
+      <c r="AG120" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH120" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A121">
         <v>52000118</v>
       </c>
@@ -18102,11 +18567,14 @@
       <c r="AF121" s="26">
         <v>0</v>
       </c>
-      <c r="AG121" s="25">
+      <c r="AG121" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH121" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A122">
         <v>52000119</v>
       </c>
@@ -18169,7 +18637,7 @@
       <c r="U122" s="8">
         <v>0</v>
       </c>
-      <c r="V122" s="35">
+      <c r="V122" s="33">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
@@ -18200,11 +18668,14 @@
       <c r="AF122" s="26">
         <v>0</v>
       </c>
-      <c r="AG122" s="25">
+      <c r="AG122" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH122" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A123">
         <v>52000120</v>
       </c>
@@ -18267,7 +18738,7 @@
       <c r="U123" s="8">
         <v>0</v>
       </c>
-      <c r="V123" s="35">
+      <c r="V123" s="33">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
@@ -18298,11 +18769,14 @@
       <c r="AF123" s="26">
         <v>0</v>
       </c>
-      <c r="AG123" s="25">
+      <c r="AG123" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH123" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A124">
         <v>52000121</v>
       </c>
@@ -18396,11 +18870,14 @@
       <c r="AF124" s="26">
         <v>0</v>
       </c>
-      <c r="AG124" s="25">
+      <c r="AG124" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH124" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:33" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:34" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A125">
         <v>52000122</v>
       </c>
@@ -18410,7 +18887,7 @@
       <c r="C125" s="15" t="s">
         <v>366</v>
       </c>
-      <c r="D125" s="42"/>
+      <c r="D125" s="40"/>
       <c r="E125" s="15">
         <v>4</v>
       </c>
@@ -18420,7 +18897,7 @@
       <c r="G125" s="15">
         <v>0</v>
       </c>
-      <c r="H125" s="41">
+      <c r="H125" s="39">
         <f t="shared" ref="H125" si="8">IF(AND(V125&gt;=13,V125&lt;=16),5,IF(AND(V125&gt;=9,V125&lt;=12),4,IF(AND(V125&gt;=5,V125&lt;=8),3,IF(AND(V125&gt;=1,V125&lt;=4),2,IF(AND(V125&gt;=-3,V125&lt;=0),1,IF(AND(V125&gt;=-5,V125&lt;=-4),0,6))))))</f>
         <v>3</v>
       </c>
@@ -18494,11 +18971,14 @@
       <c r="AF125" s="26">
         <v>0</v>
       </c>
-      <c r="AG125" s="15">
+      <c r="AG125" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH125" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:33" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:34" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A126">
         <v>52000123</v>
       </c>
@@ -18508,7 +18988,7 @@
       <c r="C126" s="15" t="s">
         <v>373</v>
       </c>
-      <c r="D126" s="42"/>
+      <c r="D126" s="40"/>
       <c r="E126" s="15">
         <v>3</v>
       </c>
@@ -18518,7 +18998,7 @@
       <c r="G126" s="15">
         <v>0</v>
       </c>
-      <c r="H126" s="41">
+      <c r="H126" s="39">
         <f t="shared" ref="H126:H127" si="9">IF(AND(V126&gt;=13,V126&lt;=16),5,IF(AND(V126&gt;=9,V126&lt;=12),4,IF(AND(V126&gt;=5,V126&lt;=8),3,IF(AND(V126&gt;=1,V126&lt;=4),2,IF(AND(V126&gt;=-3,V126&lt;=0),1,IF(AND(V126&gt;=-5,V126&lt;=-4),0,6))))))</f>
         <v>2</v>
       </c>
@@ -18592,11 +19072,14 @@
       <c r="AF126" s="26">
         <v>0</v>
       </c>
-      <c r="AG126" s="15">
+      <c r="AG126" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH126" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:33" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:34" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A127">
         <v>52000124</v>
       </c>
@@ -18606,7 +19089,7 @@
       <c r="C127" s="15" t="s">
         <v>374</v>
       </c>
-      <c r="D127" s="42"/>
+      <c r="D127" s="40"/>
       <c r="E127" s="15">
         <v>6</v>
       </c>
@@ -18616,7 +19099,7 @@
       <c r="G127" s="15">
         <v>0</v>
       </c>
-      <c r="H127" s="41">
+      <c r="H127" s="39">
         <f t="shared" si="9"/>
         <v>3</v>
       </c>
@@ -18690,11 +19173,14 @@
       <c r="AF127" s="26">
         <v>0</v>
       </c>
-      <c r="AG127" s="15">
+      <c r="AG127" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH127" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:33" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:34" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A128">
         <v>52000125</v>
       </c>
@@ -18704,7 +19190,7 @@
       <c r="C128" s="15" t="s">
         <v>376</v>
       </c>
-      <c r="D128" s="42"/>
+      <c r="D128" s="40"/>
       <c r="E128" s="15">
         <v>2</v>
       </c>
@@ -18714,7 +19200,7 @@
       <c r="G128" s="15">
         <v>0</v>
       </c>
-      <c r="H128" s="41">
+      <c r="H128" s="39">
         <f t="shared" ref="H128" si="10">IF(AND(V128&gt;=13,V128&lt;=16),5,IF(AND(V128&gt;=9,V128&lt;=12),4,IF(AND(V128&gt;=5,V128&lt;=8),3,IF(AND(V128&gt;=1,V128&lt;=4),2,IF(AND(V128&gt;=-3,V128&lt;=0),1,IF(AND(V128&gt;=-5,V128&lt;=-4),0,6))))))</f>
         <v>1</v>
       </c>
@@ -18788,11 +19274,14 @@
       <c r="AF128" s="26">
         <v>0</v>
       </c>
-      <c r="AG128" s="15">
+      <c r="AG128" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH128" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:33" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:34" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A129">
         <v>52000126</v>
       </c>
@@ -18802,7 +19291,7 @@
       <c r="C129" s="15" t="s">
         <v>379</v>
       </c>
-      <c r="D129" s="42"/>
+      <c r="D129" s="40"/>
       <c r="E129" s="15">
         <v>3</v>
       </c>
@@ -18812,7 +19301,7 @@
       <c r="G129" s="15">
         <v>0</v>
       </c>
-      <c r="H129" s="41">
+      <c r="H129" s="39">
         <f t="shared" ref="H129:H130" si="11">IF(AND(V129&gt;=13,V129&lt;=16),5,IF(AND(V129&gt;=9,V129&lt;=12),4,IF(AND(V129&gt;=5,V129&lt;=8),3,IF(AND(V129&gt;=1,V129&lt;=4),2,IF(AND(V129&gt;=-3,V129&lt;=0),1,IF(AND(V129&gt;=-5,V129&lt;=-4),0,6))))))</f>
         <v>2</v>
       </c>
@@ -18825,7 +19314,7 @@
       <c r="K129" s="16">
         <v>0</v>
       </c>
-      <c r="L129" s="43">
+      <c r="L129" s="41">
         <v>0</v>
       </c>
       <c r="M129" s="14">
@@ -18886,11 +19375,14 @@
       <c r="AF129" s="26">
         <v>0</v>
       </c>
-      <c r="AG129" s="15">
+      <c r="AG129" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH129" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:33" hidden="1" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A130">
         <v>52000127</v>
       </c>
@@ -18900,7 +19392,7 @@
       <c r="C130" s="15" t="s">
         <v>380</v>
       </c>
-      <c r="D130" s="44" t="s">
+      <c r="D130" s="42" t="s">
         <v>382</v>
       </c>
       <c r="E130" s="15">
@@ -18912,7 +19404,7 @@
       <c r="G130" s="15">
         <v>0</v>
       </c>
-      <c r="H130" s="41">
+      <c r="H130" s="39">
         <f t="shared" si="11"/>
         <v>3</v>
       </c>
@@ -18990,11 +19482,14 @@
       <c r="AF130" s="26">
         <v>0</v>
       </c>
-      <c r="AG130" s="15">
+      <c r="AG130" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH130" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:33" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:34" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A131">
         <v>52000128</v>
       </c>
@@ -19004,7 +19499,7 @@
       <c r="C131" s="15" t="s">
         <v>387</v>
       </c>
-      <c r="D131" s="42"/>
+      <c r="D131" s="40"/>
       <c r="E131" s="15">
         <v>2</v>
       </c>
@@ -19014,7 +19509,7 @@
       <c r="G131" s="15">
         <v>0</v>
       </c>
-      <c r="H131" s="41">
+      <c r="H131" s="39">
         <f t="shared" ref="H131" si="12">IF(AND(V131&gt;=13,V131&lt;=16),5,IF(AND(V131&gt;=9,V131&lt;=12),4,IF(AND(V131&gt;=5,V131&lt;=8),3,IF(AND(V131&gt;=1,V131&lt;=4),2,IF(AND(V131&gt;=-3,V131&lt;=0),1,IF(AND(V131&gt;=-5,V131&lt;=-4),0,6))))))</f>
         <v>1</v>
       </c>
@@ -19027,7 +19522,7 @@
       <c r="K131" s="16">
         <v>0</v>
       </c>
-      <c r="L131" s="43">
+      <c r="L131" s="41">
         <v>0</v>
       </c>
       <c r="M131" s="14">
@@ -19092,11 +19587,14 @@
       <c r="AF131" s="26">
         <v>0</v>
       </c>
-      <c r="AG131" s="15">
+      <c r="AG131" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH131" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:33" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:34" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A132">
         <v>52000129</v>
       </c>
@@ -19106,7 +19604,7 @@
       <c r="C132" s="15" t="s">
         <v>389</v>
       </c>
-      <c r="D132" s="42"/>
+      <c r="D132" s="40"/>
       <c r="E132" s="15">
         <v>5</v>
       </c>
@@ -19116,7 +19614,7 @@
       <c r="G132" s="15">
         <v>0</v>
       </c>
-      <c r="H132" s="41">
+      <c r="H132" s="39">
         <f t="shared" ref="H132:H133" si="14">IF(AND(V132&gt;=13,V132&lt;=16),5,IF(AND(V132&gt;=9,V132&lt;=12),4,IF(AND(V132&gt;=5,V132&lt;=8),3,IF(AND(V132&gt;=1,V132&lt;=4),2,IF(AND(V132&gt;=-3,V132&lt;=0),1,IF(AND(V132&gt;=-5,V132&lt;=-4),0,6))))))</f>
         <v>4</v>
       </c>
@@ -19129,7 +19627,7 @@
       <c r="K132" s="16">
         <v>0</v>
       </c>
-      <c r="L132" s="43">
+      <c r="L132" s="41">
         <v>0</v>
       </c>
       <c r="M132" s="14">
@@ -19194,44 +19692,47 @@
       <c r="AF132" s="26">
         <v>0</v>
       </c>
-      <c r="AG132" s="15">
+      <c r="AG132" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH132" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:33" ht="14.25" hidden="1" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:34" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A133">
         <v>52000130</v>
       </c>
-      <c r="B133" s="51" t="s">
+      <c r="B133" s="49" t="s">
         <v>392</v>
       </c>
       <c r="C133" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="D133" s="46"/>
-      <c r="E133" s="45">
+      <c r="D133" s="44"/>
+      <c r="E133" s="43">
         <v>1</v>
       </c>
-      <c r="F133" s="45">
+      <c r="F133" s="43">
         <v>100</v>
       </c>
-      <c r="G133" s="45">
-        <v>0</v>
-      </c>
-      <c r="H133" s="47">
+      <c r="G133" s="43">
+        <v>0</v>
+      </c>
+      <c r="H133" s="45">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="I133" s="45">
+      <c r="I133" s="43">
         <v>1</v>
       </c>
-      <c r="J133" s="48">
+      <c r="J133" s="46">
         <v>100</v>
       </c>
-      <c r="K133" s="48">
-        <v>0</v>
-      </c>
-      <c r="L133" s="49">
+      <c r="K133" s="46">
+        <v>0</v>
+      </c>
+      <c r="L133" s="47">
         <v>0</v>
       </c>
       <c r="M133" s="14">
@@ -19278,19 +19779,22 @@
         <f>IF(ISBLANK(AA133),0, LOOKUP(AA133,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB133/100)</f>
         <v>0</v>
       </c>
-      <c r="AA133" s="45"/>
-      <c r="AB133" s="45"/>
-      <c r="AC133" s="45" t="s">
+      <c r="AA133" s="43"/>
+      <c r="AB133" s="43"/>
+      <c r="AC133" s="43" t="s">
         <v>388</v>
       </c>
-      <c r="AD133" s="45"/>
-      <c r="AE133" s="50">
+      <c r="AD133" s="43"/>
+      <c r="AE133" s="48">
         <v>130</v>
       </c>
       <c r="AF133" s="26">
         <v>0</v>
       </c>
-      <c r="AG133" s="45">
+      <c r="AG133" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH133" s="43">
         <v>1</v>
       </c>
     </row>
@@ -19309,16 +19813,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H133">
-    <cfRule type="cellIs" dxfId="81" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="18" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="19" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="19" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19335,16 +19839,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H133">
-    <cfRule type="cellIs" dxfId="77" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19358,13 +19862,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG4"/>
+  <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P7" sqref="P7"/>
+      <selection pane="bottomRight" activeCell="AF1" sqref="AF1:AH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -19381,10 +19885,10 @@
     <col min="27" max="28" width="7.125" customWidth="1"/>
     <col min="29" max="30" width="9" customWidth="1"/>
     <col min="31" max="31" width="7.375" customWidth="1"/>
-    <col min="32" max="33" width="4.375" customWidth="1"/>
+    <col min="32" max="34" width="4.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="69" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:34" ht="69" x14ac:dyDescent="0.15">
       <c r="A1" s="19" t="s">
         <v>241</v>
       </c>
@@ -19394,7 +19898,7 @@
       <c r="C1" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="27" t="s">
         <v>295</v>
       </c>
       <c r="E1" s="20" t="s">
@@ -19406,7 +19910,7 @@
       <c r="G1" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="31" t="s">
         <v>332</v>
       </c>
       <c r="I1" s="20" t="s">
@@ -19427,25 +19931,25 @@
       <c r="N1" s="20" t="s">
         <v>292</v>
       </c>
-      <c r="O1" s="33" t="s">
+      <c r="O1" s="31" t="s">
         <v>310</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="P1" s="31" t="s">
         <v>311</v>
       </c>
-      <c r="Q1" s="33" t="s">
+      <c r="Q1" s="31" t="s">
         <v>312</v>
       </c>
-      <c r="R1" s="33" t="s">
+      <c r="R1" s="31" t="s">
         <v>313</v>
       </c>
-      <c r="S1" s="33" t="s">
+      <c r="S1" s="31" t="s">
         <v>314</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="T1" s="31" t="s">
         <v>315</v>
       </c>
-      <c r="U1" s="33" t="s">
+      <c r="U1" s="31" t="s">
         <v>316</v>
       </c>
       <c r="V1" s="21" t="s">
@@ -19472,7 +19976,7 @@
       <c r="AC1" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="AD1" s="38" t="s">
+      <c r="AD1" s="36" t="s">
         <v>343</v>
       </c>
       <c r="AE1" s="22" t="s">
@@ -19481,11 +19985,14 @@
       <c r="AF1" s="23" t="s">
         <v>286</v>
       </c>
-      <c r="AG1" s="27" t="s">
+      <c r="AG1" s="23" t="s">
+        <v>394</v>
+      </c>
+      <c r="AH1" s="23" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>110</v>
       </c>
@@ -19495,7 +20002,7 @@
       <c r="C2" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="28" t="s">
         <v>111</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -19573,7 +20080,7 @@
       <c r="AC2" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="AD2" s="39" t="s">
+      <c r="AD2" s="37" t="s">
         <v>344</v>
       </c>
       <c r="AE2" s="3" t="s">
@@ -19582,11 +20089,14 @@
       <c r="AF2" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="AG2" s="28" t="s">
+      <c r="AG2" s="3" t="s">
         <v>110</v>
       </c>
+      <c r="AH2" s="3" t="s">
+        <v>110</v>
+      </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -19608,7 +20118,7 @@
       <c r="G3" t="s">
         <v>116</v>
       </c>
-      <c r="H3" s="34" t="s">
+      <c r="H3" s="32" t="s">
         <v>333</v>
       </c>
       <c r="I3" t="s">
@@ -19629,25 +20139,25 @@
       <c r="N3" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="O3" s="34" t="s">
+      <c r="O3" s="32" t="s">
         <v>325</v>
       </c>
-      <c r="P3" s="34" t="s">
+      <c r="P3" s="32" t="s">
         <v>319</v>
       </c>
-      <c r="Q3" s="34" t="s">
+      <c r="Q3" s="32" t="s">
         <v>320</v>
       </c>
-      <c r="R3" s="34" t="s">
+      <c r="R3" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="S3" s="34" t="s">
+      <c r="S3" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="T3" s="34" t="s">
+      <c r="T3" s="32" t="s">
         <v>323</v>
       </c>
-      <c r="U3" s="34" t="s">
+      <c r="U3" s="32" t="s">
         <v>324</v>
       </c>
       <c r="V3" s="12" t="s">
@@ -19674,7 +20184,7 @@
       <c r="AC3" t="s">
         <v>119</v>
       </c>
-      <c r="AD3" s="40" t="s">
+      <c r="AD3" s="38" t="s">
         <v>345</v>
       </c>
       <c r="AE3" t="s">
@@ -19684,10 +20194,13 @@
         <v>287</v>
       </c>
       <c r="AG3" s="24" t="s">
+        <v>395</v>
+      </c>
+      <c r="AH3" s="24" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>52100000</v>
       </c>
@@ -19697,7 +20210,7 @@
       <c r="C4" s="15" t="s">
         <v>291</v>
       </c>
-      <c r="D4" s="31"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="15">
         <v>1</v>
       </c>
@@ -19720,7 +20233,7 @@
       <c r="K4" s="16">
         <v>0</v>
       </c>
-      <c r="L4" s="43">
+      <c r="L4" s="41">
         <v>0</v>
       </c>
       <c r="M4" s="14">
@@ -19779,26 +20292,29 @@
       <c r="AF4" s="26">
         <v>1</v>
       </c>
-      <c r="AG4" s="25">
+      <c r="AG4" s="26">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="25">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
finish a relic weapon
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Weapon.xlsx
+++ b/ConfigData/Xlsx/Weapon.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F632F1DC-B59F-4502-BF97-3BC42A12DE1D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{965FC768-97FC-4D30-8DEF-020227E17AA6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="标准" sheetId="1" r:id="rId1"/>
@@ -30,17 +30,29 @@
     <author>Real</author>
   </authors>
   <commentList>
-    <comment ref="AE2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="AE2" authorId="0" shapeId="0" xr:uid="{851EFE79-1D31-4189-9BC9-4859FA22DABA}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
           </rPr>
-          <t>delegate(IPlayer p, IPlayer r, ITrap t, int cid, int id, int type)</t>
+          <t>Real:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+IPlayer p, IRelic r, int cid, int type, IMonster m,ref bool result</t>
         </r>
       </text>
     </comment>
@@ -54,17 +66,29 @@
     <author>Real</author>
   </authors>
   <commentList>
-    <comment ref="AE2" authorId="0" shapeId="0" xr:uid="{EDE12423-3F02-4449-B80C-92BD7F531A90}">
+    <comment ref="AE2" authorId="0" shapeId="0" xr:uid="{49614F33-8AA3-4B37-AFBA-B9AA122414D4}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
           </rPr>
-          <t>delegate(IPlayer p, IPlayer r, ITrap t, int cid, int id, int type)</t>
+          <t>Real:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+IPlayer p, IRelic r, int cid, int type, IMonster m,ref bool result</t>
         </r>
       </text>
     </comment>
@@ -73,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="411">
   <si>
     <t>铁杖</t>
   </si>
@@ -1461,6 +1485,14 @@
   </si>
   <si>
     <t>RelicUseEffect</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(p==r.Owner){m.AddActionRate(0.3);result=true;}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>yellowsplash</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1468,7 +1500,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1709,14 +1741,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
-      <name val="Tahoma"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="44">
+  <fills count="46">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1959,6 +2005,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2253,7 +2311,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2407,6 +2465,12 @@
     <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="44" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2453,208 +2517,6 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="94">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3365,6 +3227,64 @@
         <name val="宋体"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -4104,6 +4024,150 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC66FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC66FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC66FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -6017,110 +6081,110 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AK134" totalsRowShown="0" dataDxfId="93" tableBorderDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AK134" totalsRowShown="0" dataDxfId="81" tableBorderDxfId="80">
   <autoFilter ref="A3:AK134" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A4:AI124">
     <sortCondition ref="A3:A124"/>
   </sortState>
   <tableColumns count="37">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="91"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="90"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Ename" dataDxfId="89"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Remark" dataDxfId="88"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Star" dataDxfId="87"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Type" dataDxfId="86"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Attr" dataDxfId="85"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Quality" dataDxfId="84">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="79"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="78"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Ename" dataDxfId="77"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Remark" dataDxfId="76"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Star" dataDxfId="75"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Type" dataDxfId="74"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Attr" dataDxfId="73"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Quality" dataDxfId="72">
       <calculatedColumnFormula>IF(AND(V4&gt;=13,V4&lt;=16),5,IF(AND(V4&gt;=9,V4&lt;=12),4,IF(AND(V4&gt;=5,V4&lt;=8),3,IF(AND(V4&gt;=1,V4&lt;=4),2,IF(AND(V4&gt;=-3,V4&lt;=0),1,IF(AND(V4&gt;=-5,V4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Cost" dataDxfId="83"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="AtkP" dataDxfId="82"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="PArmor" dataDxfId="81"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="MArmor" dataDxfId="80"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Modify" dataDxfId="79"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Dura" dataDxfId="78"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Def" dataDxfId="77"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Mag" dataDxfId="76"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Spd" dataDxfId="75"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Hit" dataDxfId="74"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Dhit" dataDxfId="73"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Crt" dataDxfId="72"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Luk" dataDxfId="71"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Sum" dataDxfId="70">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Cost" dataDxfId="71"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="AtkP" dataDxfId="70"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="PArmor" dataDxfId="69"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="MArmor" dataDxfId="68"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Modify" dataDxfId="67"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Dura" dataDxfId="66"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Def" dataDxfId="65"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Mag" dataDxfId="64"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Spd" dataDxfId="63"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Hit" dataDxfId="62"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Dhit" dataDxfId="61"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Crt" dataDxfId="60"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Luk" dataDxfId="59"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Sum" dataDxfId="58">
       <calculatedColumnFormula>J4+K4+L4-100+M4+ SUM(O4:U4)*5+IF(ISNUMBER(Z4),Z4,0)+Y4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Range" dataDxfId="69"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Mov" dataDxfId="68"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="~SkillMark" dataDxfId="67"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="~SkillMark2" dataDxfId="66">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Range" dataDxfId="57"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Mov" dataDxfId="56"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="~SkillMark" dataDxfId="55"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="~SkillMark2" dataDxfId="54">
       <calculatedColumnFormula>IF(ISBLANK(AA4),0, LOOKUP(AA4,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="SkillId" dataDxfId="65"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Percent" dataDxfId="64"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Arrow" dataDxfId="63"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="RelicType" dataDxfId="62"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="RelicUseEffect" dataDxfId="61"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="RelicEffect" dataDxfId="60"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="JobId" dataDxfId="59"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Icon" dataDxfId="58"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="IsSpecial" dataDxfId="57"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="IsHeroCard" dataDxfId="56"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="IsNew" dataDxfId="55"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="SkillId" dataDxfId="53"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Percent" dataDxfId="52"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Arrow" dataDxfId="51"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="RelicType" dataDxfId="50"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="RelicUseEffect" dataDxfId="49"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="RelicEffect" dataDxfId="48"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="JobId" dataDxfId="47"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Icon" dataDxfId="46"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="IsSpecial" dataDxfId="45"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="IsHeroCard" dataDxfId="44"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="IsNew" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表1_3" displayName="表1_3" ref="A3:AK4" totalsRowShown="0" dataDxfId="54" tableBorderDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表1_3" displayName="表1_3" ref="A3:AK4" totalsRowShown="0" dataDxfId="37" tableBorderDxfId="36">
   <autoFilter ref="A3:AK4" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState ref="A4:W130">
     <sortCondition ref="A3:A130"/>
   </sortState>
   <tableColumns count="37">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Ename" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Remark" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Star" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Type" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Attr" dataDxfId="46"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0100-000022000000}" name="Quality" dataDxfId="45">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Ename" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Remark" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Star" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Type" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Attr" dataDxfId="29"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0100-000022000000}" name="Quality" dataDxfId="28">
       <calculatedColumnFormula>IF(AND(V4&gt;=13,V4&lt;=16),5,IF(AND(V4&gt;=9,V4&lt;=12),4,IF(AND(V4&gt;=5,V4&lt;=8),3,IF(AND(V4&gt;=1,V4&lt;=4),2,IF(AND(V4&gt;=-3,V4&lt;=0),1,IF(AND(V4&gt;=-5,V4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Cost" dataDxfId="44"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="AtkP" dataDxfId="43"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="PArmor" dataDxfId="42"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="MArmor" dataDxfId="41"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Modify" dataDxfId="40"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0100-00001F000000}" name="Dura" dataDxfId="39"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Def" dataDxfId="38"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="Mag" dataDxfId="37"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0100-00001D000000}" name="Spd" dataDxfId="36"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0100-00001E000000}" name="Hit" dataDxfId="35"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Dhit" dataDxfId="34"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Crt" dataDxfId="33"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Luk" dataDxfId="32"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0100-000020000000}" name="Sum" dataDxfId="31">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Cost" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="AtkP" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="PArmor" dataDxfId="25"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="MArmor" dataDxfId="24"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Modify" dataDxfId="23"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0100-00001F000000}" name="Dura" dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Def" dataDxfId="21"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="Mag" dataDxfId="20"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0100-00001D000000}" name="Spd" dataDxfId="19"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0100-00001E000000}" name="Hit" dataDxfId="18"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Dhit" dataDxfId="17"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Crt" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Luk" dataDxfId="15"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0100-000020000000}" name="Sum" dataDxfId="14">
       <calculatedColumnFormula>J4+K4+L4-100+M4+ SUM(O4:U4)*5+IF(ISNUMBER(Z4),Z4,0)+Y4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Range" dataDxfId="30"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Mov" dataDxfId="29"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="~SkillMark" dataDxfId="28"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0100-000021000000}" name="~SkillMark2" dataDxfId="27">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Range" dataDxfId="13"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Mov" dataDxfId="12"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="~SkillMark" dataDxfId="11"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0100-000021000000}" name="~SkillMark2" dataDxfId="10">
       <calculatedColumnFormula>IF(ISBLANK(AA4),0, LOOKUP(AA4,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="SkillId" dataDxfId="26"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Percent" dataDxfId="25"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Arrow" dataDxfId="24"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0100-000023000000}" name="RelicType" dataDxfId="23"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0100-000024000000}" name="RelicUseEffect" dataDxfId="22"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0100-000026000000}" name="RelicEffect" dataDxfId="21"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="SkillId" dataDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Percent" dataDxfId="8"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Arrow" dataDxfId="7"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0100-000023000000}" name="RelicType" dataDxfId="6"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0100-000024000000}" name="RelicUseEffect" dataDxfId="5"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0100-000026000000}" name="RelicEffect" dataDxfId="4"/>
     <tableColumn id="26" xr3:uid="{00000000-0010-0000-0100-00001A000000}" name="JobId"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Icon" dataDxfId="20"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="IsSpecial" dataDxfId="19"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="IsHeroCard" dataDxfId="18"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="IsNew" dataDxfId="17"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Icon" dataDxfId="3"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="IsSpecial" dataDxfId="2"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="IsHeroCard" dataDxfId="1"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="IsNew" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6449,11 +6513,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK134"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="J88" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AD1" sqref="AD1:AF3"/>
+      <selection pane="bottomRight" activeCell="T97" sqref="T97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6468,7 +6532,9 @@
     <col min="25" max="26" width="4.75" customWidth="1"/>
     <col min="27" max="27" width="9.5" customWidth="1"/>
     <col min="28" max="28" width="7.125" customWidth="1"/>
-    <col min="29" max="33" width="9" customWidth="1"/>
+    <col min="29" max="30" width="9" customWidth="1"/>
+    <col min="31" max="31" width="18.5" customWidth="1"/>
+    <col min="32" max="33" width="9" customWidth="1"/>
     <col min="34" max="34" width="7.375" customWidth="1"/>
     <col min="35" max="37" width="4.375" customWidth="1"/>
     <col min="40" max="40" width="9.5" bestFit="1" customWidth="1"/>
@@ -17201,8 +17267,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:37" x14ac:dyDescent="0.15">
-      <c r="A102">
+    <row r="102" spans="1:37" ht="45" x14ac:dyDescent="0.15">
+      <c r="A102" s="52">
         <v>52000099</v>
       </c>
       <c r="B102" s="4" t="s">
@@ -17286,9 +17352,15 @@
       <c r="AC102" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AD102" s="4"/>
-      <c r="AE102" s="4"/>
-      <c r="AF102" s="4"/>
+      <c r="AD102" s="4">
+        <v>2</v>
+      </c>
+      <c r="AE102" s="51" t="s">
+        <v>409</v>
+      </c>
+      <c r="AF102" s="4" t="s">
+        <v>410</v>
+      </c>
       <c r="AG102" s="4"/>
       <c r="AH102" s="5">
         <v>99</v>
@@ -20720,16 +20792,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H134">
-    <cfRule type="cellIs" dxfId="16" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="21" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="22" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="23" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="24" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="90" priority="24" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20746,16 +20818,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H133">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="86" priority="9" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20772,16 +20844,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H134">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="82" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20798,11 +20870,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AD1" sqref="AD1:AF3"/>
+      <selection pane="bottomRight" activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -21266,19 +21338,19 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="6" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
change a parms name for relic event
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Weapon.xlsx
+++ b/ConfigData/Xlsx/Weapon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8F293F50-01BD-4CCB-A288-F3021EA30697}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{303419C5-5A32-4F53-A2A3-F6B44B602094}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
             <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
-IPlayer p, IRelic r, int cid, int type, IMonster m,ref bool result</t>
+IPlayer p, IRelic r, int cid, int type, IMonster t,ref bool result</t>
         </r>
       </text>
     </comment>
@@ -1484,14 +1484,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>if(p==r.Owner){m.AddActionRate(0.3);result=true;}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>yellowsplash</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>触发描述</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -1504,11 +1496,19 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>自己召唤单位时，提升其25%初始机动力</t>
+    <t>Summon</t>
+  </si>
+  <si>
+    <t>if(p==r.Owner){t.Action.AddMArmor(100);result=true;}</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Summon</t>
+    <t>protect</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>自己召唤单位时，召唤单位获得100点魔甲</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2546,266 +2546,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC66FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -2878,6 +2618,35 @@
         <right style="thin">
           <color theme="4"/>
         </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
         <top style="thin">
           <color theme="4"/>
         </top>
@@ -3505,6 +3274,64 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -3611,6 +3438,35 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </font>
       <border diagonalUp="0" diagonalDown="0">
@@ -4241,6 +4097,150 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC66FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC66FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC66FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -6154,112 +6154,112 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AL134" totalsRowShown="0" dataDxfId="95" tableBorderDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AL134" totalsRowShown="0" dataDxfId="83" tableBorderDxfId="82">
   <autoFilter ref="A3:AL134" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A4:AJ124">
     <sortCondition ref="A3:A124"/>
   </sortState>
   <tableColumns count="38">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="92"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Ename" dataDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Remark" dataDxfId="90"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Star" dataDxfId="89"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Type" dataDxfId="88"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Attr" dataDxfId="87"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Quality" dataDxfId="86">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Ename" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Remark" dataDxfId="78"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Star" dataDxfId="77"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Type" dataDxfId="76"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Attr" dataDxfId="75"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Quality" dataDxfId="74">
       <calculatedColumnFormula>IF(AND(V4&gt;=13,V4&lt;=16),5,IF(AND(V4&gt;=9,V4&lt;=12),4,IF(AND(V4&gt;=5,V4&lt;=8),3,IF(AND(V4&gt;=1,V4&lt;=4),2,IF(AND(V4&gt;=-3,V4&lt;=0),1,IF(AND(V4&gt;=-5,V4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Cost" dataDxfId="85"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="AtkP" dataDxfId="84"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="PArmor" dataDxfId="83"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="MArmor" dataDxfId="82"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Modify" dataDxfId="81"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Dura" dataDxfId="80"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Def" dataDxfId="79"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Mag" dataDxfId="78"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Spd" dataDxfId="77"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Hit" dataDxfId="76"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Dhit" dataDxfId="75"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Crt" dataDxfId="74"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Luk" dataDxfId="73"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Sum" dataDxfId="72">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Cost" dataDxfId="73"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="AtkP" dataDxfId="72"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="PArmor" dataDxfId="71"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="MArmor" dataDxfId="70"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Modify" dataDxfId="69"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Dura" dataDxfId="68"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Def" dataDxfId="67"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Mag" dataDxfId="66"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Spd" dataDxfId="65"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Hit" dataDxfId="64"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Dhit" dataDxfId="63"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Crt" dataDxfId="62"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Luk" dataDxfId="61"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Sum" dataDxfId="60">
       <calculatedColumnFormula>J4+K4+L4-100+M4+ SUM(O4:U4)*5+IF(ISNUMBER(Z4),Z4,0)+Y4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Range" dataDxfId="71"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Mov" dataDxfId="70"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="~SkillMark" dataDxfId="69"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="~SkillMark2" dataDxfId="68">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Range" dataDxfId="59"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Mov" dataDxfId="58"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="~SkillMark" dataDxfId="57"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="~SkillMark2" dataDxfId="56">
       <calculatedColumnFormula>IF(ISBLANK(AA4),0, LOOKUP(AA4,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="SkillId" dataDxfId="67"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Percent" dataDxfId="66"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Arrow" dataDxfId="65"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="RelicType" dataDxfId="64"/>
-    <tableColumn id="36" xr3:uid="{EE6227AF-06FE-4A25-A447-E5690B97E348}" name="Descript" dataDxfId="18"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="RelicUseEffect" dataDxfId="63"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="RelicEffect" dataDxfId="62"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="JobId" dataDxfId="61"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Icon" dataDxfId="60"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="IsSpecial" dataDxfId="59"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="IsHeroCard" dataDxfId="58"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="IsNew" dataDxfId="57"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="SkillId" dataDxfId="55"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Percent" dataDxfId="54"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Arrow" dataDxfId="53"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="RelicType" dataDxfId="52"/>
+    <tableColumn id="36" xr3:uid="{EE6227AF-06FE-4A25-A447-E5690B97E348}" name="Descript" dataDxfId="51"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="RelicUseEffect" dataDxfId="50"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="RelicEffect" dataDxfId="49"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="JobId" dataDxfId="48"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Icon" dataDxfId="47"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="IsSpecial" dataDxfId="46"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="IsHeroCard" dataDxfId="45"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="IsNew" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表1_3" displayName="表1_3" ref="A3:AL4" totalsRowShown="0" dataDxfId="56" tableBorderDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表1_3" displayName="表1_3" ref="A3:AL4" totalsRowShown="0" dataDxfId="38" tableBorderDxfId="37">
   <autoFilter ref="A3:AL4" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState ref="A4:W130">
     <sortCondition ref="A3:A130"/>
   </sortState>
   <tableColumns count="38">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Ename" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Remark" dataDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Star" dataDxfId="50"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Type" dataDxfId="49"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Attr" dataDxfId="48"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0100-000022000000}" name="Quality" dataDxfId="47">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Ename" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Remark" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Star" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Type" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Attr" dataDxfId="30"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0100-000022000000}" name="Quality" dataDxfId="29">
       <calculatedColumnFormula>IF(AND(V4&gt;=13,V4&lt;=16),5,IF(AND(V4&gt;=9,V4&lt;=12),4,IF(AND(V4&gt;=5,V4&lt;=8),3,IF(AND(V4&gt;=1,V4&lt;=4),2,IF(AND(V4&gt;=-3,V4&lt;=0),1,IF(AND(V4&gt;=-5,V4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Cost" dataDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="AtkP" dataDxfId="45"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="PArmor" dataDxfId="44"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="MArmor" dataDxfId="43"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Modify" dataDxfId="42"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0100-00001F000000}" name="Dura" dataDxfId="41"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Def" dataDxfId="40"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="Mag" dataDxfId="39"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0100-00001D000000}" name="Spd" dataDxfId="38"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0100-00001E000000}" name="Hit" dataDxfId="37"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Dhit" dataDxfId="36"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Crt" dataDxfId="35"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Luk" dataDxfId="34"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0100-000020000000}" name="Sum" dataDxfId="33">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Cost" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="AtkP" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="PArmor" dataDxfId="26"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="MArmor" dataDxfId="25"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Modify" dataDxfId="24"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0100-00001F000000}" name="Dura" dataDxfId="23"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Def" dataDxfId="22"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="Mag" dataDxfId="21"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0100-00001D000000}" name="Spd" dataDxfId="20"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0100-00001E000000}" name="Hit" dataDxfId="19"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Dhit" dataDxfId="18"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Crt" dataDxfId="17"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Luk" dataDxfId="16"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0100-000020000000}" name="Sum" dataDxfId="15">
       <calculatedColumnFormula>J4+K4+L4-100+M4+ SUM(O4:U4)*5+IF(ISNUMBER(Z4),Z4,0)+Y4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Range" dataDxfId="32"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Mov" dataDxfId="31"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="~SkillMark" dataDxfId="30"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0100-000021000000}" name="~SkillMark2" dataDxfId="29">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Range" dataDxfId="14"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Mov" dataDxfId="13"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="~SkillMark" dataDxfId="12"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0100-000021000000}" name="~SkillMark2" dataDxfId="11">
       <calculatedColumnFormula>IF(ISBLANK(AA4),0, LOOKUP(AA4,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="SkillId" dataDxfId="28"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Percent" dataDxfId="27"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Arrow" dataDxfId="26"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0100-000023000000}" name="RelicType" dataDxfId="25"/>
-    <tableColumn id="37" xr3:uid="{92C1838C-6C54-42C7-90D5-F24CAD0817D2}" name="Descript" dataDxfId="0"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0100-000024000000}" name="RelicUseEffect" dataDxfId="24"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0100-000026000000}" name="RelicEffect" dataDxfId="23"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="SkillId" dataDxfId="10"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Percent" dataDxfId="9"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Arrow" dataDxfId="8"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0100-000023000000}" name="RelicType" dataDxfId="7"/>
+    <tableColumn id="37" xr3:uid="{92C1838C-6C54-42C7-90D5-F24CAD0817D2}" name="Descript" dataDxfId="6"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0100-000024000000}" name="RelicUseEffect" dataDxfId="5"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0100-000026000000}" name="RelicEffect" dataDxfId="4"/>
     <tableColumn id="26" xr3:uid="{00000000-0010-0000-0100-00001A000000}" name="JobId"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Icon" dataDxfId="22"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="IsSpecial" dataDxfId="21"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="IsHeroCard" dataDxfId="20"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="IsNew" dataDxfId="19"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Icon" dataDxfId="3"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="IsSpecial" dataDxfId="2"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="IsHeroCard" dataDxfId="1"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="IsNew" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6589,10 +6589,10 @@
   <dimension ref="A1:AL134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B91" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="M91" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F100" sqref="F100"/>
+      <selection pane="bottomRight" activeCell="AE102" sqref="AE102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6708,7 +6708,7 @@
         <v>405</v>
       </c>
       <c r="AE1" s="48" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="AF1" s="48" t="s">
         <v>400</v>
@@ -6824,7 +6824,7 @@
         <v>111</v>
       </c>
       <c r="AE2" s="49" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="AF2" s="49" t="s">
         <v>404</v>
@@ -6940,7 +6940,7 @@
         <v>406</v>
       </c>
       <c r="AE3" s="50" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="AF3" s="50" t="s">
         <v>407</v>
@@ -17533,16 +17533,16 @@
       <c r="AB102" s="4"/>
       <c r="AC102" s="4"/>
       <c r="AD102" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="AE102" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="AE102" s="4" t="s">
+      <c r="AF102" s="51" t="s">
+        <v>412</v>
+      </c>
+      <c r="AG102" s="4" t="s">
         <v>413</v>
-      </c>
-      <c r="AF102" s="51" t="s">
-        <v>408</v>
-      </c>
-      <c r="AG102" s="4" t="s">
-        <v>409</v>
       </c>
       <c r="AH102" s="4"/>
       <c r="AI102" s="5">
@@ -21007,16 +21007,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H134">
-    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="21" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="22" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="23" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="24" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="92" priority="24" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21033,16 +21033,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H133">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="7" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="8" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="88" priority="9" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21059,16 +21059,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H134">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="84" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21201,7 +21201,7 @@
         <v>405</v>
       </c>
       <c r="AE1" s="48" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="AF1" s="48" t="s">
         <v>400</v>
@@ -21317,7 +21317,7 @@
         <v>111</v>
       </c>
       <c r="AE2" s="49" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="AF2" s="49" t="s">
         <v>404</v>
@@ -21433,7 +21433,7 @@
         <v>406</v>
       </c>
       <c r="AE3" s="50" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="AF3" s="50" t="s">
         <v>407</v>
@@ -21563,19 +21563,19 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="2" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add a new relic card
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Weapon.xlsx
+++ b/ConfigData/Xlsx/Weapon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{303419C5-5A32-4F53-A2A3-F6B44B602094}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8015EB1F-C6C2-4710-B7BB-CC42525D2A75}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="420">
   <si>
     <t>铁杖</t>
   </si>
@@ -1508,6 +1508,25 @@
   </si>
   <si>
     <t>自己召唤单位时，召唤单位获得100点魔甲</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑莲花</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Black Lotus</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EpRecover</t>
+  </si>
+  <si>
+    <t>每回合30%的机会恢复三种能量各一点</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>if(p==r.Owner){if(MathTool.GetRandom(100)&lt;30)p.Action.SetLastEp(4);result=true;}</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2531,7 +2550,55 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="96">
+  <dxfs count="100">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC66FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -6154,112 +6221,112 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AL134" totalsRowShown="0" dataDxfId="83" tableBorderDxfId="82">
-  <autoFilter ref="A3:AL134" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A3:AL135" totalsRowShown="0" dataDxfId="87" tableBorderDxfId="86">
+  <autoFilter ref="A3:AL135" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="A4:AJ124">
     <sortCondition ref="A3:A124"/>
   </sortState>
   <tableColumns count="38">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Ename" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Remark" dataDxfId="78"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Star" dataDxfId="77"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Type" dataDxfId="76"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Attr" dataDxfId="75"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Quality" dataDxfId="74">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Id" dataDxfId="85"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="84"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Ename" dataDxfId="83"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Remark" dataDxfId="82"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Star" dataDxfId="81"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Type" dataDxfId="80"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Attr" dataDxfId="79"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Quality" dataDxfId="78">
       <calculatedColumnFormula>IF(AND(V4&gt;=13,V4&lt;=16),5,IF(AND(V4&gt;=9,V4&lt;=12),4,IF(AND(V4&gt;=5,V4&lt;=8),3,IF(AND(V4&gt;=1,V4&lt;=4),2,IF(AND(V4&gt;=-3,V4&lt;=0),1,IF(AND(V4&gt;=-5,V4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Cost" dataDxfId="73"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="AtkP" dataDxfId="72"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="PArmor" dataDxfId="71"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="MArmor" dataDxfId="70"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Modify" dataDxfId="69"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Dura" dataDxfId="68"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Def" dataDxfId="67"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Mag" dataDxfId="66"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Spd" dataDxfId="65"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Hit" dataDxfId="64"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Dhit" dataDxfId="63"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Crt" dataDxfId="62"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Luk" dataDxfId="61"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Sum" dataDxfId="60">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Cost" dataDxfId="77"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="AtkP" dataDxfId="76"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="PArmor" dataDxfId="75"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="MArmor" dataDxfId="74"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Modify" dataDxfId="73"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Dura" dataDxfId="72"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Def" dataDxfId="71"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Mag" dataDxfId="70"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Spd" dataDxfId="69"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Hit" dataDxfId="68"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Dhit" dataDxfId="67"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Crt" dataDxfId="66"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Luk" dataDxfId="65"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Sum" dataDxfId="64">
       <calculatedColumnFormula>J4+K4+L4-100+M4+ SUM(O4:U4)*5+IF(ISNUMBER(Z4),Z4,0)+Y4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Range" dataDxfId="59"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Mov" dataDxfId="58"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="~SkillMark" dataDxfId="57"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="~SkillMark2" dataDxfId="56">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Range" dataDxfId="63"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Mov" dataDxfId="62"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="~SkillMark" dataDxfId="61"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="~SkillMark2" dataDxfId="60">
       <calculatedColumnFormula>IF(ISBLANK(AA4),0, LOOKUP(AA4,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="SkillId" dataDxfId="55"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Percent" dataDxfId="54"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Arrow" dataDxfId="53"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="RelicType" dataDxfId="52"/>
-    <tableColumn id="36" xr3:uid="{EE6227AF-06FE-4A25-A447-E5690B97E348}" name="Descript" dataDxfId="51"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="RelicUseEffect" dataDxfId="50"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="RelicEffect" dataDxfId="49"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="JobId" dataDxfId="48"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Icon" dataDxfId="47"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="IsSpecial" dataDxfId="46"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="IsHeroCard" dataDxfId="45"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="IsNew" dataDxfId="44"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="SkillId" dataDxfId="59"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Percent" dataDxfId="58"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Arrow" dataDxfId="57"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="RelicType" dataDxfId="56"/>
+    <tableColumn id="36" xr3:uid="{EE6227AF-06FE-4A25-A447-E5690B97E348}" name="Descript" dataDxfId="55"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="RelicUseEffect" dataDxfId="54"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="RelicEffect" dataDxfId="53"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="JobId" dataDxfId="52"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Icon" dataDxfId="51"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="IsSpecial" dataDxfId="50"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="IsHeroCard" dataDxfId="49"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="IsNew" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表1_3" displayName="表1_3" ref="A3:AL4" totalsRowShown="0" dataDxfId="38" tableBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="表1_3" displayName="表1_3" ref="A3:AL4" totalsRowShown="0" dataDxfId="42" tableBorderDxfId="41">
   <autoFilter ref="A3:AL4" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState ref="A4:W130">
     <sortCondition ref="A3:A130"/>
   </sortState>
   <tableColumns count="38">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Ename" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Remark" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Star" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Type" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Attr" dataDxfId="30"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0100-000022000000}" name="Quality" dataDxfId="29">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Id" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Ename" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Remark" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Star" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Type" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Attr" dataDxfId="34"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0100-000022000000}" name="Quality" dataDxfId="33">
       <calculatedColumnFormula>IF(AND(V4&gt;=13,V4&lt;=16),5,IF(AND(V4&gt;=9,V4&lt;=12),4,IF(AND(V4&gt;=5,V4&lt;=8),3,IF(AND(V4&gt;=1,V4&lt;=4),2,IF(AND(V4&gt;=-3,V4&lt;=0),1,IF(AND(V4&gt;=-5,V4&lt;=-4),0,6))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Cost" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="AtkP" dataDxfId="27"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="PArmor" dataDxfId="26"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="MArmor" dataDxfId="25"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Modify" dataDxfId="24"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0100-00001F000000}" name="Dura" dataDxfId="23"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Def" dataDxfId="22"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="Mag" dataDxfId="21"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0100-00001D000000}" name="Spd" dataDxfId="20"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0100-00001E000000}" name="Hit" dataDxfId="19"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Dhit" dataDxfId="18"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Crt" dataDxfId="17"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Luk" dataDxfId="16"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0100-000020000000}" name="Sum" dataDxfId="15">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Cost" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="AtkP" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="PArmor" dataDxfId="30"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="MArmor" dataDxfId="29"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="Modify" dataDxfId="28"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0100-00001F000000}" name="Dura" dataDxfId="27"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Def" dataDxfId="26"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="Mag" dataDxfId="25"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0100-00001D000000}" name="Spd" dataDxfId="24"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0100-00001E000000}" name="Hit" dataDxfId="23"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Dhit" dataDxfId="22"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Crt" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Luk" dataDxfId="20"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0100-000020000000}" name="Sum" dataDxfId="19">
       <calculatedColumnFormula>J4+K4+L4-100+M4+ SUM(O4:U4)*5+IF(ISNUMBER(Z4),Z4,0)+Y4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Range" dataDxfId="14"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Mov" dataDxfId="13"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="~SkillMark" dataDxfId="12"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0100-000021000000}" name="~SkillMark2" dataDxfId="11">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Range" dataDxfId="18"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0100-00001B000000}" name="Mov" dataDxfId="17"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0100-000018000000}" name="~SkillMark" dataDxfId="16"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0100-000021000000}" name="~SkillMark2" dataDxfId="15">
       <calculatedColumnFormula>IF(ISBLANK(AA4),0, LOOKUP(AA4,[1]Skill!$A:$A,[1]Skill!$AB:$AB)*AB4/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="SkillId" dataDxfId="10"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Percent" dataDxfId="9"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Arrow" dataDxfId="8"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0100-000023000000}" name="RelicType" dataDxfId="7"/>
-    <tableColumn id="37" xr3:uid="{92C1838C-6C54-42C7-90D5-F24CAD0817D2}" name="Descript" dataDxfId="6"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0100-000024000000}" name="RelicUseEffect" dataDxfId="5"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0100-000026000000}" name="RelicEffect" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="SkillId" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Percent" dataDxfId="13"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Arrow" dataDxfId="12"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0100-000023000000}" name="RelicType" dataDxfId="11"/>
+    <tableColumn id="37" xr3:uid="{92C1838C-6C54-42C7-90D5-F24CAD0817D2}" name="Descript" dataDxfId="10"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0100-000024000000}" name="RelicUseEffect" dataDxfId="9"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0100-000026000000}" name="RelicEffect" dataDxfId="8"/>
     <tableColumn id="26" xr3:uid="{00000000-0010-0000-0100-00001A000000}" name="JobId"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Icon" dataDxfId="3"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="IsSpecial" dataDxfId="2"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="IsHeroCard" dataDxfId="1"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="IsNew" dataDxfId="0"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Icon" dataDxfId="7"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="IsSpecial" dataDxfId="6"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0100-00001C000000}" name="IsHeroCard" dataDxfId="5"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="IsNew" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6586,13 +6653,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL134"/>
+  <dimension ref="A1:AL135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="M91" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B94" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AE102" sqref="AE102"/>
+      <selection pane="bottomRight" activeCell="I102" sqref="I102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -17462,7 +17529,7 @@
       </c>
       <c r="D102" s="25"/>
       <c r="E102" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F102">
         <v>104</v>
@@ -17472,10 +17539,10 @@
       </c>
       <c r="H102" s="4">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I102" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J102" s="6">
         <v>0</v>
@@ -17515,7 +17582,7 @@
       </c>
       <c r="V102" s="10">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W102" s="8">
         <v>0</v>
@@ -17527,7 +17594,7 @@
         <v>0</v>
       </c>
       <c r="Z102" s="8">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="AA102" s="35"/>
       <c r="AB102" s="4"/>
@@ -20333,7 +20400,7 @@
         <v>0</v>
       </c>
       <c r="AL128" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:38" ht="14.25" x14ac:dyDescent="0.15">
@@ -20438,7 +20505,7 @@
         <v>0</v>
       </c>
       <c r="AL129" s="15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:38" x14ac:dyDescent="0.15">
@@ -20684,7 +20751,7 @@
         <v>0</v>
       </c>
       <c r="H132" s="39">
-        <f t="shared" ref="H132:H134" si="14">IF(AND(V132&gt;=13,V132&lt;=16),5,IF(AND(V132&gt;=9,V132&lt;=12),4,IF(AND(V132&gt;=5,V132&lt;=8),3,IF(AND(V132&gt;=1,V132&lt;=4),2,IF(AND(V132&gt;=-3,V132&lt;=0),1,IF(AND(V132&gt;=-5,V132&lt;=-4),0,6))))))</f>
+        <f t="shared" ref="H132:H135" si="14">IF(AND(V132&gt;=13,V132&lt;=16),5,IF(AND(V132&gt;=9,V132&lt;=12),4,IF(AND(V132&gt;=5,V132&lt;=8),3,IF(AND(V132&gt;=1,V132&lt;=4),2,IF(AND(V132&gt;=-3,V132&lt;=0),1,IF(AND(V132&gt;=-5,V132&lt;=-4),0,6))))))</f>
         <v>4</v>
       </c>
       <c r="I132" s="15">
@@ -20992,10 +21059,116 @@
         <v>1</v>
       </c>
     </row>
+    <row r="135" spans="1:38" ht="60" x14ac:dyDescent="0.15">
+      <c r="A135">
+        <v>52000132</v>
+      </c>
+      <c r="B135" s="15" t="s">
+        <v>415</v>
+      </c>
+      <c r="C135" s="15" t="s">
+        <v>416</v>
+      </c>
+      <c r="D135" s="40"/>
+      <c r="E135" s="15">
+        <v>5</v>
+      </c>
+      <c r="F135" s="15">
+        <v>104</v>
+      </c>
+      <c r="G135" s="15">
+        <v>0</v>
+      </c>
+      <c r="H135" s="39">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="I135" s="15">
+        <v>5</v>
+      </c>
+      <c r="J135" s="16">
+        <v>0</v>
+      </c>
+      <c r="K135" s="16">
+        <v>0</v>
+      </c>
+      <c r="L135" s="41">
+        <v>0</v>
+      </c>
+      <c r="M135" s="14">
+        <v>0</v>
+      </c>
+      <c r="N135" s="8">
+        <v>30</v>
+      </c>
+      <c r="O135" s="8">
+        <v>0</v>
+      </c>
+      <c r="P135" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q135" s="8">
+        <v>0</v>
+      </c>
+      <c r="R135" s="8">
+        <v>0</v>
+      </c>
+      <c r="S135" s="8">
+        <v>0</v>
+      </c>
+      <c r="T135" s="8">
+        <v>0</v>
+      </c>
+      <c r="U135" s="8">
+        <v>0</v>
+      </c>
+      <c r="V135" s="10">
+        <f t="shared" ref="V135" si="17">J135+K135+L135-100+M135+ SUM(O135:U135)*5+IF(ISNUMBER(Z135),Z135,0)+Y135</f>
+        <v>7</v>
+      </c>
+      <c r="W135" s="8">
+        <v>0</v>
+      </c>
+      <c r="X135" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y135" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z135" s="10">
+        <v>107</v>
+      </c>
+      <c r="AA135" s="15"/>
+      <c r="AB135" s="15"/>
+      <c r="AC135" s="15"/>
+      <c r="AD135" s="15" t="s">
+        <v>417</v>
+      </c>
+      <c r="AE135" s="15" t="s">
+        <v>418</v>
+      </c>
+      <c r="AF135" s="51" t="s">
+        <v>419</v>
+      </c>
+      <c r="AG135" s="15"/>
+      <c r="AH135" s="15"/>
+      <c r="AI135" s="17">
+        <v>132</v>
+      </c>
+      <c r="AJ135" s="26">
+        <v>0</v>
+      </c>
+      <c r="AK135" s="26">
+        <v>0</v>
+      </c>
+      <c r="AL135" s="15">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="V4:V134">
-    <cfRule type="colorScale" priority="105">
+  <conditionalFormatting sqref="V4:V135">
+    <cfRule type="colorScale" priority="110">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -21006,21 +21179,47 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H134">
-    <cfRule type="cellIs" dxfId="95" priority="21" operator="equal">
+  <conditionalFormatting sqref="H4:H135">
+    <cfRule type="cellIs" dxfId="99" priority="26" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="27" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="28" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="24" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="96" priority="29" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V133">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H133">
+    <cfRule type="cellIs" dxfId="95" priority="11" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="12" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="13" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="92" priority="14" operator="greaterThanOrEqual">
+      <formula>4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V134">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -21032,7 +21231,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H133">
+  <conditionalFormatting sqref="H134">
     <cfRule type="cellIs" dxfId="91" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -21046,7 +21245,7 @@
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V134">
+  <conditionalFormatting sqref="V135">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -21058,17 +21257,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H134">
-    <cfRule type="cellIs" dxfId="87" priority="1" operator="equal">
+  <conditionalFormatting sqref="H135">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThanOrEqual">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21563,19 +21762,19 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="43" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="2" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="6" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>